<commit_message>
#84 Fixing sheet protection in Excel file.
</commit_message>
<xml_diff>
--- a/database/VideosUkGebärden.xlsx
+++ b/database/VideosUkGebärden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User-Matthias\Dev\Android\UKGM\src\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52DEA75-C0B7-44D5-8E3B-08E17057C694}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52ECEE2-A082-41D6-8E2F-C57934224599}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{978A20FD-486C-4CB5-9933-67C562CBE71F}"/>
   </bookViews>
@@ -2488,7 +2488,7 @@
   <dimension ref="A1:F265"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B265" sqref="B265"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5270,11 +5270,6 @@
       <formula>NOT(ISERROR(SEARCH("Nein",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D211" xr:uid="{6A2F4277-BEEA-43C0-9379-0B2D99A4D641}">
-      <formula1>$O$2:$O$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
#97 Adding missing semicolon to update statements
</commit_message>
<xml_diff>
--- a/database/VideosUkGebärden.xlsx
+++ b/database/VideosUkGebärden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User-Matthias\Dev\Android\UKGM\src\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFB4A21-4C4C-446A-86F3-F104EB05B258}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2B944E-8B07-44CD-A7FB-D1B076536E84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{978A20FD-486C-4CB5-9933-67C562CBE71F}"/>
   </bookViews>
@@ -2640,56 +2640,7 @@
     <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{28FF20A6-2C0A-453F-9445-4F430706AF1A}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="16"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="31"/>
-          <bgColor indexed="47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="17"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="27"/>
-          <bgColor indexed="42"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3018,8 +2969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C22E1E0-4D2F-4ED8-9423-514FCF041C4D}">
   <dimension ref="A1:H264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="A215" sqref="A215"/>
+    <sheetView tabSelected="1" topLeftCell="G197" workbookViewId="0">
+      <selection activeCell="H212" sqref="H212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3076,8 +3027,8 @@
         <v>820</v>
       </c>
       <c r="H2" t="str">
-        <f>"update signs set name_de = """&amp;B2&amp;""", mnemonic = """&amp;C2&amp;""", tag1 ="""&amp;D2&amp;""", tag2 ="""&amp;E2&amp;""", tag3 ="""&amp;F2&amp;""" where name = """&amp;A2&amp;""""</f>
-        <v>update signs set name_de = "Dann/Danach", mnemonic = "Die Zukunft liegt vor mir", tag1 ="Zeit", tag2 ="Teil 2", tag3 ="" where name = "afterwards"</v>
+        <f>"update signs set name_de = """&amp;B2&amp;""", mnemonic = """&amp;C2&amp;""", tag1 ="""&amp;D2&amp;""", tag2 ="""&amp;E2&amp;""", tag3 ="""&amp;F2&amp;""" where name = """&amp;A2&amp;""";"</f>
+        <v>update signs set name_de = "Dann/Danach", mnemonic = "Die Zukunft liegt vor mir", tag1 ="Zeit", tag2 ="Teil 2", tag3 ="" where name = "afterwards";</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -3100,8 +3051,8 @@
         <v>820</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H66" si="0">"update signs set name_de = """&amp;B3&amp;""", mnemonic = """&amp;C3&amp;""", tag1 ="""&amp;D3&amp;""", tag2 ="""&amp;E3&amp;""", tag3 ="""&amp;F3&amp;""" where name = """&amp;A3&amp;""""</f>
-        <v>update signs set name_de = "Noch mal", mnemonic = "Gebärde 'eins' kommt von hinten nach vorn", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="" where name = "again"</v>
+        <f t="shared" ref="H3:H66" si="0">"update signs set name_de = """&amp;B3&amp;""", mnemonic = """&amp;C3&amp;""", tag1 ="""&amp;D3&amp;""", tag2 ="""&amp;E3&amp;""", tag3 ="""&amp;F3&amp;""" where name = """&amp;A3&amp;""";"</f>
+        <v>update signs set name_de = "Noch mal", mnemonic = "Gebärde 'eins' kommt von hinten nach vorn", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="" where name = "again";</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -3125,7 +3076,7 @@
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Flugzeug/Fliegen", mnemonic = "Y-Hand startet vom Boden", tag1 ="Fahrzeug", tag2 ="Teil 3", tag3 ="" where name = "airplane"</v>
+        <v>update signs set name_de = "Flugzeug/Fliegen", mnemonic = "Y-Hand startet vom Boden", tag1 ="Fahrzeug", tag2 ="Teil 3", tag3 ="" where name = "airplane";</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -3149,7 +3100,7 @@
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Allah", mnemonic = "Faust öffnet nach vorn", tag1 ="Religion", tag2 ="Teil 3", tag3 ="" where name = "allah"</v>
+        <v>update signs set name_de = "Allah", mnemonic = "Faust öffnet nach vorn", tag1 ="Religion", tag2 ="Teil 3", tag3 ="" where name = "allah";</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -3173,7 +3124,7 @@
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Alleine", mnemonic = "Erhobenen Zeigefinger von oben nach unten ziehen", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="" where name = "alone"</v>
+        <v>update signs set name_de = "Alleine", mnemonic = "Erhobenen Zeigefinger von oben nach unten ziehen", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="" where name = "alone";</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -3197,7 +3148,7 @@
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Entschuldigung", mnemonic = "Handfläche kreist auf Handrücken", tag1 ="Interaktion", tag2 ="Teil 3", tag3 ="" where name = "apology"</v>
+        <v>update signs set name_de = "Entschuldigung", mnemonic = "Handfläche kreist auf Handrücken", tag1 ="Interaktion", tag2 ="Teil 3", tag3 ="" where name = "apology";</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -3221,7 +3172,7 @@
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Apfel", mnemonic = "Abbeißen", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "apple"</v>
+        <v>update signs set name_de = "Apfel", mnemonic = "Abbeißen", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "apple";</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -3245,7 +3196,7 @@
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Geht es dir gut?", mnemonic = "Mit fragender Mimik 'du' und 'gut' gebärden", tag1 ="Interaktion", tag2 ="Teil 2", tag3 ="" where name = "are_you_ok"</v>
+        <v>update signs set name_de = "Geht es dir gut?", mnemonic = "Mit fragender Mimik 'du' und 'gut' gebärden", tag1 ="Interaktion", tag2 ="Teil 2", tag3 ="" where name = "are_you_ok";</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -3272,7 +3223,7 @@
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Auch", mnemonic = "Komma in die Luft malen", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="Interaktion" where name = "as_well"</v>
+        <v>update signs set name_de = "Auch", mnemonic = "Komma in die Luft malen", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="Interaktion" where name = "as_well";</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -3296,7 +3247,7 @@
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Baby", mnemonic = "Baby auf Arm schaukeln", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "baby"</v>
+        <v>update signs set name_de = "Baby", mnemonic = "Baby auf Arm schaukeln", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "baby";</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -3320,7 +3271,7 @@
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Schlecht/Doof", mnemonic = "Daumen runter", tag1 ="Eigenschaften", tag2 ="Teil 1", tag3 ="" where name = "bad"</v>
+        <v>update signs set name_de = "Schlecht/Doof", mnemonic = "Daumen runter", tag1 ="Eigenschaften", tag2 ="Teil 1", tag3 ="" where name = "bad";</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -3344,7 +3295,7 @@
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Tasche", mnemonic = "Taschengriff ergreifen und hochnehmen", tag1 ="Behälter", tag2 ="Teil 2", tag3 ="" where name = "bag"</v>
+        <v>update signs set name_de = "Tasche", mnemonic = "Taschengriff ergreifen und hochnehmen", tag1 ="Behälter", tag2 ="Teil 2", tag3 ="" where name = "bag";</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -3371,7 +3322,7 @@
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Backen/Kneten", mnemonic = "Mit Händen kneten", tag1 ="Ernährung", tag2 ="Teil 2", tag3 ="Verb" where name = "baking"</v>
+        <v>update signs set name_de = "Backen/Kneten", mnemonic = "Mit Händen kneten", tag1 ="Ernährung", tag2 ="Teil 2", tag3 ="Verb" where name = "baking";</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -3395,7 +3346,7 @@
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Ball", mnemonic = "Mit Handflächen Ball umfahren", tag1 ="Spielen", tag2 ="Teil 2", tag3 ="" where name = "ball"</v>
+        <v>update signs set name_de = "Ball", mnemonic = "Mit Handflächen Ball umfahren", tag1 ="Spielen", tag2 ="Teil 2", tag3 ="" where name = "ball";</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -3419,7 +3370,7 @@
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Banane", mnemonic = "Dominante Hand schält", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "banana"</v>
+        <v>update signs set name_de = "Banane", mnemonic = "Dominante Hand schält", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "banana";</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -3446,7 +3397,7 @@
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Baden", mnemonic = "Rücken mit Handtuch abrubbeln", tag1 ="Körperpflege", tag2 ="Teil 1", tag3 ="Verb" where name = "bathing"</v>
+        <v>update signs set name_de = "Baden", mnemonic = "Rücken mit Handtuch abrubbeln", tag1 ="Körperpflege", tag2 ="Teil 1", tag3 ="Verb" where name = "bathing";</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -3470,7 +3421,7 @@
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Badezimmer", mnemonic = "Erst 'baden' dann 'Zimmer'", tag1 ="Haus", tag2 ="Teil 3", tag3 ="" where name = "bathroom"</v>
+        <v>update signs set name_de = "Badezimmer", mnemonic = "Erst 'baden' dann 'Zimmer'", tag1 ="Haus", tag2 ="Teil 3", tag3 ="" where name = "bathroom";</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -3494,7 +3445,7 @@
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Bett", mnemonic = "Kopf legt sich  schlafen", tag1 ="Haus", tag2 ="Teil 1", tag3 ="" where name = "bed"</v>
+        <v>update signs set name_de = "Bett", mnemonic = "Kopf legt sich  schlafen", tag1 ="Haus", tag2 ="Teil 1", tag3 ="" where name = "bed";</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -3521,7 +3472,7 @@
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Vorher", mnemonic = "Vergangenheit liegt hinter mir", tag1 ="Zeit", tag2 ="Teil 2", tag3 ="Zeit" where name = "before"</v>
+        <v>update signs set name_de = "Vorher", mnemonic = "Vergangenheit liegt hinter mir", tag1 ="Zeit", tag2 ="Teil 2", tag3 ="Zeit" where name = "before";</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -3548,7 +3499,7 @@
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Anfangen", mnemonic = "Eine Arbeit aufnehmen", tag1 ="Arbeit", tag2 ="Teil 2", tag3 ="Verb" where name = "begin"</v>
+        <v>update signs set name_de = "Anfangen", mnemonic = "Eine Arbeit aufnehmen", tag1 ="Arbeit", tag2 ="Teil 2", tag3 ="Verb" where name = "begin";</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -3575,7 +3526,7 @@
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Unter", mnemonic = "Handrücken unter Handfläche legen", tag1 ="Kleine Worte", tag2 ="Teil 2", tag3 ="Präposition" where name = "below"</v>
+        <v>update signs set name_de = "Unter", mnemonic = "Handrücken unter Handfläche legen", tag1 ="Kleine Worte", tag2 ="Teil 2", tag3 ="Präposition" where name = "below";</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -3599,7 +3550,7 @@
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Groß", mnemonic = "Hände maximal breit auseinander", tag1 ="Eigenschaften", tag2 ="Teil 3", tag3 ="" where name = "big"</v>
+        <v>update signs set name_de = "Groß", mnemonic = "Hände maximal breit auseinander", tag1 ="Eigenschaften", tag2 ="Teil 3", tag3 ="" where name = "big";</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -3623,7 +3574,7 @@
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Fahrrad", mnemonic = "Fäuste fahren", tag1 ="Fahrzeug", tag2 ="Teil 3", tag3 ="" where name = "bike"</v>
+        <v>update signs set name_de = "Fahrrad", mnemonic = "Fäuste fahren", tag1 ="Fahrzeug", tag2 ="Teil 3", tag3 ="" where name = "bike";</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -3647,7 +3598,7 @@
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Vogel", mnemonic = "Schnabel auf und zu", tag1 ="Tier", tag2 ="Teil 2", tag3 ="" where name = "bird"</v>
+        <v>update signs set name_de = "Vogel", mnemonic = "Schnabel auf und zu", tag1 ="Tier", tag2 ="Teil 2", tag3 ="" where name = "bird";</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -3671,7 +3622,7 @@
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Pflanze/blühen", mnemonic = "Pflanze wächst aus Boden/neben Körper", tag1 ="Natur", tag2 ="Teil 2", tag3 ="" where name = "bloom"</v>
+        <v>update signs set name_de = "Pflanze/blühen", mnemonic = "Pflanze wächst aus Boden/neben Körper", tag1 ="Natur", tag2 ="Teil 2", tag3 ="" where name = "bloom";</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -3698,7 +3649,7 @@
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Blau", mnemonic = "Fluss von oben nach unten schlängeln", tag1 ="Farbe", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "blue"</v>
+        <v>update signs set name_de = "Blau", mnemonic = "Fluss von oben nach unten schlängeln", tag1 ="Farbe", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "blue";</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -3725,7 +3676,7 @@
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Buch", mnemonic = "Handflächen öffnen sich wie Buch", tag1 ="Spielen", tag2 ="Teil 2", tag3 ="Lernen" where name = "book"</v>
+        <v>update signs set name_de = "Buch", mnemonic = "Handflächen öffnen sich wie Buch", tag1 ="Spielen", tag2 ="Teil 2", tag3 ="Lernen" where name = "book";</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -3749,7 +3700,7 @@
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Junge", mnemonic = "2x mit gestreckter Hand grüßen", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "boy"</v>
+        <v>update signs set name_de = "Junge", mnemonic = "2x mit gestreckter Hand grüßen", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "boy";</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -3773,7 +3724,7 @@
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Brot", mnemonic = "Eine Scheibe abschneiden", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "bread"</v>
+        <v>update signs set name_de = "Brot", mnemonic = "Eine Scheibe abschneiden", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "bread";</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -3797,7 +3748,7 @@
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Kaputt", mnemonic = "Fäuste zerbrechen etwas", tag1 ="Eigenschaften", tag2 ="Teil 3", tag3 ="" where name = "broken"</v>
+        <v>update signs set name_de = "Kaputt", mnemonic = "Fäuste zerbrechen etwas", tag1 ="Eigenschaften", tag2 ="Teil 3", tag3 ="" where name = "broken";</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -3821,7 +3772,7 @@
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Bürsten/Kämmen", mnemonic = "Faust bürstet über Haare", tag1 ="Körperpflege", tag2 ="Teil 3", tag3 ="" where name = "brush_hair"</v>
+        <v>update signs set name_de = "Bürsten/Kämmen", mnemonic = "Faust bürstet über Haare", tag1 ="Körperpflege", tag2 ="Teil 3", tag3 ="" where name = "brush_hair";</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -3845,7 +3796,7 @@
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Zähne putzen", mnemonic = "Zeigefinger putzt Zähne auf und ab", tag1 ="Körperpflege", tag2 ="Teil 3", tag3 ="" where name = "brush_teeth"</v>
+        <v>update signs set name_de = "Zähne putzen", mnemonic = "Zeigefinger putzt Zähne auf und ab", tag1 ="Körperpflege", tag2 ="Teil 3", tag3 ="" where name = "brush_teeth";</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -3869,7 +3820,7 @@
       </c>
       <c r="H34" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Buddha", mnemonic = "O-Hände bewegen sich nach vorn", tag1 ="Religion", tag2 ="Teil 3", tag3 ="" where name = "buddha"</v>
+        <v>update signs set name_de = "Buddha", mnemonic = "O-Hände bewegen sich nach vorn", tag1 ="Religion", tag2 ="Teil 3", tag3 ="" where name = "buddha";</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -3893,7 +3844,7 @@
       </c>
       <c r="H35" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Bauen/Bauklötze", mnemonic = "Hände stapeln", tag1 ="Spielen", tag2 ="Teil 2", tag3 ="" where name = "build"</v>
+        <v>update signs set name_de = "Bauen/Bauklötze", mnemonic = "Hände stapeln", tag1 ="Spielen", tag2 ="Teil 2", tag3 ="" where name = "build";</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -3917,7 +3868,7 @@
       </c>
       <c r="H36" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Bus", mnemonic = "Buslänge zeigen, diagonal", tag1 ="Fahrzeug", tag2 ="Teil 1", tag3 ="" where name = "bus"</v>
+        <v>update signs set name_de = "Bus", mnemonic = "Buslänge zeigen, diagonal", tag1 ="Fahrzeug", tag2 ="Teil 1", tag3 ="" where name = "bus";</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
@@ -3941,7 +3892,7 @@
       </c>
       <c r="H37" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Butter", mnemonic = "Zeigefinger streicht Butter auf Brot", tag1 ="Lebensmittel", tag2 ="Teil 3", tag3 ="" where name = "butter"</v>
+        <v>update signs set name_de = "Butter", mnemonic = "Zeigefinger streicht Butter auf Brot", tag1 ="Lebensmittel", tag2 ="Teil 3", tag3 ="" where name = "butter";</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -3965,7 +3916,7 @@
       </c>
       <c r="H38" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Schmetterling", mnemonic = "Hände verhaken und Flügel flattern", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "butterfly"</v>
+        <v>update signs set name_de = "Schmetterling", mnemonic = "Hände verhaken und Flügel flattern", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "butterfly";</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -3992,7 +3943,7 @@
       </c>
       <c r="H39" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Kakao", mnemonic = "Daumen tippt 2x an Mundwinkel", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="Getränk" where name = "cacao"</v>
+        <v>update signs set name_de = "Kakao", mnemonic = "Daumen tippt 2x an Mundwinkel", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="Getränk" where name = "cacao";</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
@@ -4016,7 +3967,7 @@
       </c>
       <c r="H40" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Bonbon", mnemonic = "Bonbon in Wange", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "candy"</v>
+        <v>update signs set name_de = "Bonbon", mnemonic = "Bonbon in Wange", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "candy";</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -4040,7 +3991,7 @@
       </c>
       <c r="H41" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Auto", mnemonic = "lenken mimen", tag1 ="Fahrzeug", tag2 ="Teil 1", tag3 ="" where name = "car"</v>
+        <v>update signs set name_de = "Auto", mnemonic = "lenken mimen", tag1 ="Fahrzeug", tag2 ="Teil 1", tag3 ="" where name = "car";</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
@@ -4064,7 +4015,7 @@
       </c>
       <c r="H42" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Achtung/Vorsicht", mnemonic = "V-Hände gucken weit zu den Seiten", tag1 ="Interaktion", tag2 ="Teil 3", tag3 ="" where name = "careful"</v>
+        <v>update signs set name_de = "Achtung/Vorsicht", mnemonic = "V-Hände gucken weit zu den Seiten", tag1 ="Interaktion", tag2 ="Teil 3", tag3 ="" where name = "careful";</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
@@ -4088,7 +4039,7 @@
       </c>
       <c r="H43" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Möhre", mnemonic = "Schrappen", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "carrot"</v>
+        <v>update signs set name_de = "Möhre", mnemonic = "Schrappen", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "carrot";</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
@@ -4112,7 +4063,7 @@
       </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Katze", mnemonic = "3 Schnurrhaare andeuten", tag1 ="Tier", tag2 ="Teil 2", tag3 ="" where name = "cat"</v>
+        <v>update signs set name_de = "Katze", mnemonic = "3 Schnurrhaare andeuten", tag1 ="Tier", tag2 ="Teil 2", tag3 ="" where name = "cat";</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
@@ -4136,7 +4087,7 @@
       </c>
       <c r="H45" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Stuhl", mnemonic = "Gebeugte Finger  als Lehne", tag1 ="Haus", tag2 ="Teil 1", tag3 ="" where name = "chair"</v>
+        <v>update signs set name_de = "Stuhl", mnemonic = "Gebeugte Finger  als Lehne", tag1 ="Haus", tag2 ="Teil 1", tag3 ="" where name = "chair";</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
@@ -4160,7 +4111,7 @@
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Huhn", mnemonic = "Mit Zeigefinger und Daumen picken", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "chicken"</v>
+        <v>update signs set name_de = "Huhn", mnemonic = "Mit Zeigefinger und Daumen picken", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "chicken";</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
@@ -4184,7 +4135,7 @@
       </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Kinder", mnemonic = "Köpfe wie Orgelpfeifen zeigen", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "children"</v>
+        <v>update signs set name_de = "Kinder", mnemonic = "Köpfe wie Orgelpfeifen zeigen", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "children";</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
@@ -4208,7 +4159,7 @@
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Schokolade", mnemonic = "Tafel zeigen", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "chocolade"</v>
+        <v>update signs set name_de = "Schokolade", mnemonic = "Tafel zeigen", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "chocolade";</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
@@ -4232,7 +4183,7 @@
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Sauber", mnemonic = "Hand sauber wischen", tag1 ="Eigenschaften", tag2 ="Teil 2", tag3 ="" where name = "clean"</v>
+        <v>update signs set name_de = "Sauber", mnemonic = "Hand sauber wischen", tag1 ="Eigenschaften", tag2 ="Teil 2", tag3 ="" where name = "clean";</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
@@ -4259,7 +4210,7 @@
       </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Klettern", mnemonic = "Mit Krallhänden nach oben klettern", tag1 ="Freizeit", tag2 ="Teil 3", tag3 ="Verb" where name = "climbing"</v>
+        <v>update signs set name_de = "Klettern", mnemonic = "Mit Krallhänden nach oben klettern", tag1 ="Freizeit", tag2 ="Teil 3", tag3 ="Verb" where name = "climbing";</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
@@ -4286,7 +4237,7 @@
       </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Schlüssel/Schließen", mnemonic = "Auf- und zuschließen", tag1 ="Haus", tag2 ="Teil 2", tag3 ="Verb" where name = "close"</v>
+        <v>update signs set name_de = "Schlüssel/Schließen", mnemonic = "Auf- und zuschließen", tag1 ="Haus", tag2 ="Teil 2", tag3 ="Verb" where name = "close";</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
@@ -4310,7 +4261,7 @@
       </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Kaffee", mnemonic = "Kaffee mahlen", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "coffee"</v>
+        <v>update signs set name_de = "Kaffee", mnemonic = "Kaffee mahlen", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "coffee";</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
@@ -4334,7 +4285,7 @@
       </c>
       <c r="H53" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Kalt/Frieren", mnemonic = "Vor Kälte zittern", tag1 ="Eigenschaften", tag2 ="Teil 2", tag3 ="" where name = "cold"</v>
+        <v>update signs set name_de = "Kalt/Frieren", mnemonic = "Vor Kälte zittern", tag1 ="Eigenschaften", tag2 ="Teil 2", tag3 ="" where name = "cold";</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
@@ -4361,7 +4312,7 @@
       </c>
       <c r="H54" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Kommen", mnemonic = "Heranwinken", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Verb" where name = "come_here"</v>
+        <v>update signs set name_de = "Kommen", mnemonic = "Heranwinken", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Verb" where name = "come_here";</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
@@ -4385,7 +4336,7 @@
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Keks", mnemonic = "Abbeißen", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "cookie"</v>
+        <v>update signs set name_de = "Keks", mnemonic = "Abbeißen", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "cookie";</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
@@ -4412,7 +4363,7 @@
       </c>
       <c r="H56" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Kochen", mnemonic = "In Stielkasserolle rühren", tag1 ="Ernährung", tag2 ="Teil 2", tag3 ="Verb" where name = "cooking"</v>
+        <v>update signs set name_de = "Kochen", mnemonic = "In Stielkasserolle rühren", tag1 ="Ernährung", tag2 ="Teil 2", tag3 ="Verb" where name = "cooking";</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
@@ -4436,7 +4387,7 @@
       </c>
       <c r="H57" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Kuh", mnemonic = "Hörner nachahmen", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "cow"</v>
+        <v>update signs set name_de = "Kuh", mnemonic = "Hörner nachahmen", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "cow";</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
@@ -4460,7 +4411,7 @@
       </c>
       <c r="H58" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Gurke", mnemonic = "Gurke nachformen", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "cucumber"</v>
+        <v>update signs set name_de = "Gurke", mnemonic = "Gurke nachformen", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "cucumber";</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
@@ -4484,7 +4435,7 @@
       </c>
       <c r="H59" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Schrank", mnemonic = "Mit Handflächen Schrank umreißen", tag1 ="Haus", tag2 ="Teil 2", tag3 ="" where name = "cupboard"</v>
+        <v>update signs set name_de = "Schrank", mnemonic = "Mit Handflächen Schrank umreißen", tag1 ="Haus", tag2 ="Teil 2", tag3 ="" where name = "cupboard";</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.35">
@@ -4508,7 +4459,7 @@
       </c>
       <c r="H60" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Hörgerät", mnemonic = "Hörgerät hinter Ohr mimen", tag1 ="Behinderung", tag2 ="Teil 3", tag3 ="" where name = "deaf_aid"</v>
+        <v>update signs set name_de = "Hörgerät", mnemonic = "Hörgerät hinter Ohr mimen", tag1 ="Behinderung", tag2 ="Teil 3", tag3 ="" where name = "deaf_aid";</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
@@ -4532,7 +4483,7 @@
       </c>
       <c r="H61" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Windel", mnemonic = "Handflächen kletten Windel zu", tag1 ="Körperpflege", tag2 ="Teil 3", tag3 ="" where name = "diaper"</v>
+        <v>update signs set name_de = "Windel", mnemonic = "Handflächen kletten Windel zu", tag1 ="Körperpflege", tag2 ="Teil 3", tag3 ="" where name = "diaper";</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
@@ -4559,7 +4510,7 @@
       </c>
       <c r="H62" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Schmutzig", mnemonic = "Krümel auf Hand verteilen", tag1 ="Körperpflege", tag2 ="Teil 2", tag3 ="Eigenschaften" where name = "dirty"</v>
+        <v>update signs set name_de = "Schmutzig", mnemonic = "Krümel auf Hand verteilen", tag1 ="Körperpflege", tag2 ="Teil 2", tag3 ="Eigenschaften" where name = "dirty";</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
@@ -4583,7 +4534,7 @@
       </c>
       <c r="H63" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Arzt/Doktor", mnemonic = "Auf Handrücken pieksen", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "doctor"</v>
+        <v>update signs set name_de = "Arzt/Doktor", mnemonic = "Auf Handrücken pieksen", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "doctor";</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
@@ -4607,7 +4558,7 @@
       </c>
       <c r="H64" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Hund", mnemonic = "Hund zu sich 'heranklopfen'", tag1 ="Tier", tag2 ="Teil 2", tag3 ="" where name = "dog"</v>
+        <v>update signs set name_de = "Hund", mnemonic = "Hund zu sich 'heranklopfen'", tag1 ="Tier", tag2 ="Teil 2", tag3 ="" where name = "dog";</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
@@ -4631,7 +4582,7 @@
       </c>
       <c r="H65" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Puppe", mnemonic = "Baby still auf Arm halten", tag1 ="Spielen", tag2 ="Teil 1", tag3 ="" where name = "doll"</v>
+        <v>update signs set name_de = "Puppe", mnemonic = "Baby still auf Arm halten", tag1 ="Spielen", tag2 ="Teil 1", tag3 ="" where name = "doll";</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
@@ -4658,7 +4609,7 @@
       </c>
       <c r="H66" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Fertig", mnemonic = "Handkante auf Handfläche 'schlagen'", tag1 ="Eigenschaften", tag2 ="Teil 1", tag3 ="kleine _Worte" where name = "done"</v>
+        <v>update signs set name_de = "Fertig", mnemonic = "Handkante auf Handfläche 'schlagen'", tag1 ="Eigenschaften", tag2 ="Teil 1", tag3 ="kleine _Worte" where name = "done";</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
@@ -4681,8 +4632,8 @@
         <v>820</v>
       </c>
       <c r="H67" t="str">
-        <f t="shared" ref="H67:H130" si="1">"update signs set name_de = """&amp;B67&amp;""", mnemonic = """&amp;C67&amp;""", tag1 ="""&amp;D67&amp;""", tag2 ="""&amp;E67&amp;""", tag3 ="""&amp;F67&amp;""" where name = """&amp;A67&amp;""""</f>
-        <v>update signs set name_de = "Tür/Tor", mnemonic = "Mit gestreckter Hand 'Türöffnen' zeigen", tag1 ="Haus", tag2 ="Teil 2", tag3 ="" where name = "door"</v>
+        <f t="shared" ref="H67:H130" si="1">"update signs set name_de = """&amp;B67&amp;""", mnemonic = """&amp;C67&amp;""", tag1 ="""&amp;D67&amp;""", tag2 ="""&amp;E67&amp;""", tag3 ="""&amp;F67&amp;""" where name = """&amp;A67&amp;""";"</f>
+        <v>update signs set name_de = "Tür/Tor", mnemonic = "Mit gestreckter Hand 'Türöffnen' zeigen", tag1 ="Haus", tag2 ="Teil 2", tag3 ="" where name = "door";</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
@@ -4709,7 +4660,7 @@
       </c>
       <c r="H68" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Unten/ Tief", mnemonic = "Nach unten zeigen", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "down"</v>
+        <v>update signs set name_de = "Unten/ Tief", mnemonic = "Nach unten zeigen", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "down";</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
@@ -4736,7 +4687,7 @@
       </c>
       <c r="H69" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Getränk", mnemonic = "Getränk/Trinkgefäß", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="Getränk" where name = "drink"</v>
+        <v>update signs set name_de = "Getränk", mnemonic = "Getränk/Trinkgefäß", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="Getränk" where name = "drink";</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.35">
@@ -4763,7 +4714,7 @@
       </c>
       <c r="H70" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Trinken", mnemonic = "Getränk zum Mund führen", tag1 ="Ernährung", tag2 ="Teil 1", tag3 ="Verb" where name = "drinking"</v>
+        <v>update signs set name_de = "Trinken", mnemonic = "Getränk zum Mund führen", tag1 ="Ernährung", tag2 ="Teil 1", tag3 ="Verb" where name = "drinking";</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.35">
@@ -4787,7 +4738,7 @@
       </c>
       <c r="H71" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Tropfen", mnemonic = "Zeigefinger tropft (tippen)", tag1 ="Krankheit", tag2 ="Teil 3", tag3 ="" where name = "drop"</v>
+        <v>update signs set name_de = "Tropfen", mnemonic = "Zeigefinger tropft (tippen)", tag1 ="Krankheit", tag2 ="Teil 3", tag3 ="" where name = "drop";</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.35">
@@ -4814,7 +4765,7 @@
       </c>
       <c r="H72" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Essen", mnemonic = "Essen nachahmen", tag1 ="Ernährung", tag2 ="Teil 1", tag3 ="Verb" where name = "eating"</v>
+        <v>update signs set name_de = "Essen", mnemonic = "Essen nachahmen", tag1 ="Ernährung", tag2 ="Teil 1", tag3 ="Verb" where name = "eating";</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
@@ -4838,7 +4789,7 @@
       </c>
       <c r="H73" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Ei", mnemonic = "Eigröße zeigen", tag1 ="Lebensmittel", tag2 ="Teil 3", tag3 ="" where name = "egg"</v>
+        <v>update signs set name_de = "Ei", mnemonic = "Eigröße zeigen", tag1 ="Lebensmittel", tag2 ="Teil 3", tag3 ="" where name = "egg";</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
@@ -4865,7 +4816,7 @@
       </c>
       <c r="H74" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Leer", mnemonic = "Alles weg", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "empty"</v>
+        <v>update signs set name_de = "Leer", mnemonic = "Alles weg", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "empty";</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
@@ -4892,7 +4843,7 @@
       </c>
       <c r="H75" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Runterfallen", mnemonic = "Zeige-und Mittelfinger fallen von Handfläche", tag1 ="Freizeit", tag2 ="Teil 3", tag3 ="Verb" where name = "fall_down"</v>
+        <v>update signs set name_de = "Runterfallen", mnemonic = "Zeige-und Mittelfinger fallen von Handfläche", tag1 ="Freizeit", tag2 ="Teil 3", tag3 ="Verb" where name = "fall_down";</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.35">
@@ -4919,7 +4870,7 @@
       </c>
       <c r="H76" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Zuerst", mnemonic = "Daumen taucht von unten auf", tag1 ="Kleine Worte", tag2 ="Teil 2", tag3 ="Zeit" where name = "first"</v>
+        <v>update signs set name_de = "Zuerst", mnemonic = "Daumen taucht von unten auf", tag1 ="Kleine Worte", tag2 ="Teil 2", tag3 ="Zeit" where name = "first";</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.35">
@@ -4943,7 +4894,7 @@
       </c>
       <c r="H77" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Fisch", mnemonic = "Hand schlängelt sich durch's Wasser", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "fish"</v>
+        <v>update signs set name_de = "Fisch", mnemonic = "Hand schlängelt sich durch's Wasser", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "fish";</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.35">
@@ -4970,7 +4921,7 @@
       </c>
       <c r="H78" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Blume", mnemonic = "Blüte öffnet sich unter Nase", tag1 ="draußen", tag2 ="Teil 2", tag3 ="Pflanzen" where name = "flower"</v>
+        <v>update signs set name_de = "Blume", mnemonic = "Blüte öffnet sich unter Nase", tag1 ="draußen", tag2 ="Teil 2", tag3 ="Pflanzen" where name = "flower";</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.35">
@@ -4997,7 +4948,7 @@
       </c>
       <c r="H79" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Lieb", mnemonic = "Wange 1x von oben nach unten streicheln", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Eigenschaften" where name = "fond"</v>
+        <v>update signs set name_de = "Lieb", mnemonic = "Wange 1x von oben nach unten streicheln", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Eigenschaften" where name = "fond";</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.35">
@@ -5024,7 +4975,7 @@
       </c>
       <c r="H80" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Fußball spielen", mnemonic = "Faust tritt in Handfläche", tag1 ="Freizeit", tag2 ="Teil 3", tag3 ="Verb" where name = "football"</v>
+        <v>update signs set name_de = "Fußball spielen", mnemonic = "Faust tritt in Handfläche", tag1 ="Freizeit", tag2 ="Teil 3", tag3 ="Verb" where name = "football";</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.35">
@@ -5048,7 +4999,7 @@
       </c>
       <c r="H81" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Gabel", mnemonic = "Gabel piekt in Handfläche", tag1 ="Ernährung", tag2 ="Teil 2", tag3 ="" where name = "fork"</v>
+        <v>update signs set name_de = "Gabel", mnemonic = "Gabel piekt in Handfläche", tag1 ="Ernährung", tag2 ="Teil 2", tag3 ="" where name = "fork";</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.35">
@@ -5072,7 +5023,7 @@
       </c>
       <c r="H82" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Freund/In", mnemonic = "2x Hände schütteln", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "friend"</v>
+        <v>update signs set name_de = "Freund/In", mnemonic = "2x Hände schütteln", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "friend";</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.35">
@@ -5099,7 +5050,7 @@
       </c>
       <c r="H83" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Voll", mnemonic = "Bis oben randvoll", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "full"</v>
+        <v>update signs set name_de = "Voll", mnemonic = "Bis oben randvoll", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "full";</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.35">
@@ -5126,7 +5077,7 @@
       </c>
       <c r="H84" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Spaß", mnemonic = "2x Nasenspitze stupsen", tag1 ="Interaktion", tag2 ="Teil 3", tag3 ="Freizeit" where name = "fun"</v>
+        <v>update signs set name_de = "Spaß", mnemonic = "2x Nasenspitze stupsen", tag1 ="Interaktion", tag2 ="Teil 3", tag3 ="Freizeit" where name = "fun";</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.35">
@@ -5150,7 +5101,7 @@
       </c>
       <c r="H85" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Mädchen", mnemonic = "Mit Daumen 2x Trägerkleid andeuten", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "girl"</v>
+        <v>update signs set name_de = "Mädchen", mnemonic = "Mit Daumen 2x Trägerkleid andeuten", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "girl";</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.35">
@@ -5177,7 +5128,7 @@
       </c>
       <c r="H86" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Geben", mnemonic = "Richtungsgebärde von … zu …", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Verb" where name = "give"</v>
+        <v>update signs set name_de = "Geben", mnemonic = "Richtungsgebärde von … zu …", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Verb" where name = "give";</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.35">
@@ -5201,7 +5152,7 @@
       </c>
       <c r="H87" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Brille", mnemonic = "Zeigefinger und Daumen formen Brille", tag1 ="Behinderung", tag2 ="Teil 3", tag3 ="" where name = "glasses"</v>
+        <v>update signs set name_de = "Brille", mnemonic = "Zeigefinger und Daumen formen Brille", tag1 ="Behinderung", tag2 ="Teil 3", tag3 ="" where name = "glasses";</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.35">
@@ -5228,7 +5179,7 @@
       </c>
       <c r="H88" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "weg!", mnemonic = "Wegwerf-Bewegung", tag1 ="kleine Wörter", tag2 ="Teil 1", tag3 ="Eigenschaften" where name = "go_away"</v>
+        <v>update signs set name_de = "weg!", mnemonic = "Wegwerf-Bewegung", tag1 ="kleine Wörter", tag2 ="Teil 1", tag3 ="Eigenschaften" where name = "go_away";</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.35">
@@ -5252,7 +5203,7 @@
       </c>
       <c r="H89" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Geh da hin", mnemonic = "Richtung zeigen", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="" where name = "go_there"</v>
+        <v>update signs set name_de = "Geh da hin", mnemonic = "Richtung zeigen", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="" where name = "go_there";</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.35">
@@ -5276,7 +5227,7 @@
       </c>
       <c r="H90" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Gott", mnemonic = "Dreieinigkeit fährt in den Himmel", tag1 ="Religion", tag2 ="Teil 3", tag3 ="" where name = "god"</v>
+        <v>update signs set name_de = "Gott", mnemonic = "Dreieinigkeit fährt in den Himmel", tag1 ="Religion", tag2 ="Teil 3", tag3 ="" where name = "god";</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.35">
@@ -5303,7 +5254,7 @@
       </c>
       <c r="H91" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Gut/Prima", mnemonic = "Daumen hoch", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="Eigenschaften" where name = "good"</v>
+        <v>update signs set name_de = "Gut/Prima", mnemonic = "Daumen hoch", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="Eigenschaften" where name = "good";</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.35">
@@ -5327,7 +5278,7 @@
       </c>
       <c r="H92" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Oma", mnemonic = "Dutt andeuten", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "grandma"</v>
+        <v>update signs set name_de = "Oma", mnemonic = "Dutt andeuten", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "grandma";</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.35">
@@ -5351,7 +5302,7 @@
       </c>
       <c r="H93" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Opa", mnemonic = "Zwirbelbart andeuten", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "grandpa"</v>
+        <v>update signs set name_de = "Opa", mnemonic = "Zwirbelbart andeuten", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "grandpa";</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.35">
@@ -5378,7 +5329,7 @@
       </c>
       <c r="H94" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Grün", mnemonic = "Grasbüschel wackelt", tag1 ="Farbe", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "green"</v>
+        <v>update signs set name_de = "Grün", mnemonic = "Grasbüschel wackelt", tag1 ="Farbe", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "green";</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.35">
@@ -5405,7 +5356,7 @@
       </c>
       <c r="H95" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Hallo/Tschüss", mnemonic = "Winken", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Kleine Worte" where name = "hello"</v>
+        <v>update signs set name_de = "Hallo/Tschüss", mnemonic = "Winken", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Kleine Worte" where name = "hello";</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.35">
@@ -5432,7 +5383,7 @@
       </c>
       <c r="H96" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Ich helfe dir", mnemonic = "2. Hand hilft der anderen", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Verb" where name = "helping"</v>
+        <v>update signs set name_de = "Ich helfe dir", mnemonic = "2. Hand hilft der anderen", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Verb" where name = "helping";</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.35">
@@ -5456,7 +5407,7 @@
       </c>
       <c r="H97" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Hier", mnemonic = "Punkt zeigen", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="" where name = "here"</v>
+        <v>update signs set name_de = "Hier", mnemonic = "Punkt zeigen", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="" where name = "here";</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.35">
@@ -5480,7 +5431,7 @@
       </c>
       <c r="H98" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Pferd", mnemonic = "Mit Zügeln reiten", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "horse"</v>
+        <v>update signs set name_de = "Pferd", mnemonic = "Mit Zügeln reiten", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "horse";</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.35">
@@ -5507,7 +5458,7 @@
       </c>
       <c r="H99" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Heiß/Warm", mnemonic = "Schweiß von Stirn wischen", tag1 ="draußen", tag2 ="Teil 2", tag3 ="Eigenschaften" where name = "hot"</v>
+        <v>update signs set name_de = "Heiß/Warm", mnemonic = "Schweiß von Stirn wischen", tag1 ="draußen", tag2 ="Teil 2", tag3 ="Eigenschaften" where name = "hot";</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.35">
@@ -5531,7 +5482,7 @@
       </c>
       <c r="H100" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Haus", mnemonic = "Dach andeuten", tag1 ="Haus", tag2 ="Teil 1", tag3 ="" where name = "house"</v>
+        <v>update signs set name_de = "Haus", mnemonic = "Dach andeuten", tag1 ="Haus", tag2 ="Teil 1", tag3 ="" where name = "house";</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.35">
@@ -5555,7 +5506,7 @@
       </c>
       <c r="H101" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Ich", mnemonic = "Mit Zeigefinger auf sich zeigen", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "i"</v>
+        <v>update signs set name_de = "Ich", mnemonic = "Mit Zeigefinger auf sich zeigen", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "i";</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.35">
@@ -5579,7 +5530,7 @@
       </c>
       <c r="H102" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Eis", mnemonic = "Eis lecken", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "ice"</v>
+        <v>update signs set name_de = "Eis", mnemonic = "Eis lecken", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "ice";</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.35">
@@ -5606,7 +5557,7 @@
       </c>
       <c r="H103" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "In", mnemonic = "In ein 'Regal' oder in ein 'Gefäß' zeigen", tag1 ="Kleine Worte", tag2 ="Teil 2", tag3 ="Präposition" where name = "in"</v>
+        <v>update signs set name_de = "In", mnemonic = "In ein 'Regal' oder in ein 'Gefäß' zeigen", tag1 ="Kleine Worte", tag2 ="Teil 2", tag3 ="Präposition" where name = "in";</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.35">
@@ -5633,7 +5584,7 @@
       </c>
       <c r="H104" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Jesus", mnemonic = "Mittelfinger tippen auf Nagelmale", tag1 ="Religion", tag2 ="Teil 3", tag3 ="Person" where name = "jesus"</v>
+        <v>update signs set name_de = "Jesus", mnemonic = "Mittelfinger tippen auf Nagelmale", tag1 ="Religion", tag2 ="Teil 3", tag3 ="Person" where name = "jesus";</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.35">
@@ -5660,7 +5611,7 @@
       </c>
       <c r="H105" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Saft", mnemonic = "Saft läuft aus gepresster Frucht", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="Getränk" where name = "juice"</v>
+        <v>update signs set name_de = "Saft", mnemonic = "Saft läuft aus gepresster Frucht", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="Getränk" where name = "juice";</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.35">
@@ -5687,7 +5638,7 @@
       </c>
       <c r="H106" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Springen/Hüpfen", mnemonic = "Zeige-und Mittelfinger hüpfen auf Handfläche", tag1 ="Freizeit", tag2 ="Teil 3", tag3 ="Verb" where name = "jump"</v>
+        <v>update signs set name_de = "Springen/Hüpfen", mnemonic = "Zeige-und Mittelfinger hüpfen auf Handfläche", tag1 ="Freizeit", tag2 ="Teil 3", tag3 ="Verb" where name = "jump";</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.35">
@@ -5714,7 +5665,7 @@
       </c>
       <c r="H107" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Kindergarten", mnemonic = "Kinder' und 'Garten' zeigen", tag1 ="Haus", tag2 ="Teil 2", tag3 ="Spielen" where name = "kindergarden"</v>
+        <v>update signs set name_de = "Kindergarten", mnemonic = "Kinder' und 'Garten' zeigen", tag1 ="Haus", tag2 ="Teil 2", tag3 ="Spielen" where name = "kindergarden";</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.35">
@@ -5738,7 +5689,7 @@
       </c>
       <c r="H108" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Küche", mnemonic = "Erst 'kochen' dann 'Zimmer'", tag1 ="Haus", tag2 ="Teil 3", tag3 ="" where name = "kitchen"</v>
+        <v>update signs set name_de = "Küche", mnemonic = "Erst 'kochen' dann 'Zimmer'", tag1 ="Haus", tag2 ="Teil 3", tag3 ="" where name = "kitchen";</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.35">
@@ -5765,7 +5716,7 @@
       </c>
       <c r="H109" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Messer/Schneiden", mnemonic = "Beide Zeigefinger schneiden", tag1 ="Ernährung", tag2 ="Teil 2", tag3 ="Verb" where name = "knife"</v>
+        <v>update signs set name_de = "Messer/Schneiden", mnemonic = "Beide Zeigefinger schneiden", tag1 ="Ernährung", tag2 ="Teil 2", tag3 ="Verb" where name = "knife";</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.35">
@@ -5789,7 +5740,7 @@
       </c>
       <c r="H110" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Licht/Lampe", mnemonic = "Strahlende Lampe seitlich oben neben Kopf", tag1 ="Haus", tag2 ="Teil 2", tag3 ="" where name = "lamp"</v>
+        <v>update signs set name_de = "Licht/Lampe", mnemonic = "Strahlende Lampe seitlich oben neben Kopf", tag1 ="Haus", tag2 ="Teil 2", tag3 ="" where name = "lamp";</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.35">
@@ -5816,7 +5767,7 @@
       </c>
       <c r="H111" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Später", mnemonic = "Wellenförmige Bewegung", tag1 ="Kleine Worte", tag2 ="Teil 2", tag3 ="Zeit" where name = "later"</v>
+        <v>update signs set name_de = "Später", mnemonic = "Wellenförmige Bewegung", tag1 ="Kleine Worte", tag2 ="Teil 2", tag3 ="Zeit" where name = "later";</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.35">
@@ -5843,7 +5794,7 @@
       </c>
       <c r="H112" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Hören", mnemonic = "Schall kommt an das Ohr", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Verb" where name = "listening"</v>
+        <v>update signs set name_de = "Hören", mnemonic = "Schall kommt an das Ohr", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Verb" where name = "listening";</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.35">
@@ -5870,7 +5821,7 @@
       </c>
       <c r="H113" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Sehen/Gucken", mnemonic = "Richtungsgebärde", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Verb" where name = "look"</v>
+        <v>update signs set name_de = "Sehen/Gucken", mnemonic = "Richtungsgebärde", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Verb" where name = "look";</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.35">
@@ -5897,7 +5848,7 @@
       </c>
       <c r="H114" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Machen", mnemonic = "Obere Faust klopft drehend auf untere Faust", tag1 ="Arbeit", tag2 ="Teil 1", tag3 ="Verb" where name = "make"</v>
+        <v>update signs set name_de = "Machen", mnemonic = "Obere Faust klopft drehend auf untere Faust", tag1 ="Arbeit", tag2 ="Teil 1", tag3 ="Verb" where name = "make";</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.35">
@@ -5921,7 +5872,7 @@
       </c>
       <c r="H115" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Mama", mnemonic = "Wange kreisend streicheln", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "mama"</v>
+        <v>update signs set name_de = "Mama", mnemonic = "Wange kreisend streicheln", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "mama";</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.35">
@@ -5945,7 +5896,7 @@
       </c>
       <c r="H116" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Mann", mnemonic = "Hut an Krempe fassen", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "man"</v>
+        <v>update signs set name_de = "Mann", mnemonic = "Hut an Krempe fassen", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "man";</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.35">
@@ -5972,7 +5923,7 @@
       </c>
       <c r="H117" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Viele", mnemonic = "Finger zappeln am Kinn zur dominanten Seite", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="Menge" where name = "many"</v>
+        <v>update signs set name_de = "Viele", mnemonic = "Finger zappeln am Kinn zur dominanten Seite", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="Menge" where name = "many";</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.35">
@@ -5996,7 +5947,7 @@
       </c>
       <c r="H118" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Marmelade", mnemonic = "Hand streicht flächig auf Brotscheibe", tag1 ="Lebensmittel", tag2 ="Teil 3", tag3 ="" where name = "marmelade"</v>
+        <v>update signs set name_de = "Marmelade", mnemonic = "Hand streicht flächig auf Brotscheibe", tag1 ="Lebensmittel", tag2 ="Teil 3", tag3 ="" where name = "marmelade";</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.35">
@@ -6023,7 +5974,7 @@
       </c>
       <c r="H119" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Milch", mnemonic = "Melken", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="Getränk" where name = "milk"</v>
+        <v>update signs set name_de = "Milch", mnemonic = "Melken", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="Getränk" where name = "milk";</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.35">
@@ -6050,7 +6001,7 @@
       </c>
       <c r="H120" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Mehr", mnemonic = "Handfläche bewegt sich nach oben vorn", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="Menge" where name = "more"</v>
+        <v>update signs set name_de = "Mehr", mnemonic = "Handfläche bewegt sich nach oben vorn", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="Menge" where name = "more";</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.35">
@@ -6074,7 +6025,7 @@
       </c>
       <c r="H121" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Motorrad/Mofa", mnemonic = "An Lenker gibt eine Faust Gas", tag1 ="Fahrzeug", tag2 ="Teil 3", tag3 ="" where name = "motorcycle"</v>
+        <v>update signs set name_de = "Motorrad/Mofa", mnemonic = "An Lenker gibt eine Faust Gas", tag1 ="Fahrzeug", tag2 ="Teil 3", tag3 ="" where name = "motorcycle";</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.35">
@@ -6101,7 +6052,7 @@
       </c>
       <c r="H122" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Singen/Musik", mnemonic = "Dirigieren", tag1 ="Spielen", tag2 ="Teil 1", tag3 ="Verb" where name = "music"</v>
+        <v>update signs set name_de = "Singen/Musik", mnemonic = "Dirigieren", tag1 ="Spielen", tag2 ="Teil 1", tag3 ="Verb" where name = "music";</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.35">
@@ -6128,7 +6079,7 @@
       </c>
       <c r="H123" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Nein", mnemonic = "Schnell von einer zur anderen Seite", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="Interaktion" where name = "no"</v>
+        <v>update signs set name_de = "Nein", mnemonic = "Schnell von einer zur anderen Seite", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="Interaktion" where name = "no";</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.35">
@@ -6152,7 +6103,7 @@
       </c>
       <c r="H124" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Nudeln", mnemonic = "Spaghetti aufwickeln", tag1 ="Lebensmittel", tag2 ="Teil 3", tag3 ="" where name = "noodles"</v>
+        <v>update signs set name_de = "Nudeln", mnemonic = "Spaghetti aufwickeln", tag1 ="Lebensmittel", tag2 ="Teil 3", tag3 ="" where name = "noodles";</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.35">
@@ -6179,7 +6130,7 @@
       </c>
       <c r="H125" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Jetzt", mnemonic = "Ich bin die Gegenwart", tag1 ="Kleine Worte", tag2 ="Teil 2", tag3 ="Zeit" where name = "now"</v>
+        <v>update signs set name_de = "Jetzt", mnemonic = "Ich bin die Gegenwart", tag1 ="Kleine Worte", tag2 ="Teil 2", tag3 ="Zeit" where name = "now";</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.35">
@@ -6206,7 +6157,7 @@
       </c>
       <c r="H126" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Auf", mnemonic = "Handfläche auf Handrücken legen", tag1 ="Kleine Worte", tag2 ="Teil 2", tag3 ="Präposition" where name = "on_sth"</v>
+        <v>update signs set name_de = "Auf", mnemonic = "Handfläche auf Handrücken legen", tag1 ="Kleine Worte", tag2 ="Teil 2", tag3 ="Präposition" where name = "on_sth";</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.35">
@@ -6233,7 +6184,7 @@
       </c>
       <c r="H127" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Eins/Ein", mnemonic = "Zeigefinger und Handrücken zum Gegenüber", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="Menge" where name = "one"</v>
+        <v>update signs set name_de = "Eins/Ein", mnemonic = "Zeigefinger und Handrücken zum Gegenüber", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="Menge" where name = "one";</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.35">
@@ -6257,7 +6208,7 @@
       </c>
       <c r="H128" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Orange", mnemonic = "Schalen zeigen und herausbrechen", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "orange"</v>
+        <v>update signs set name_de = "Orange", mnemonic = "Schalen zeigen und herausbrechen", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "orange";</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.35">
@@ -6284,7 +6235,7 @@
       </c>
       <c r="H129" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Draußen", mnemonic = "Nach draußen zeigen", tag1 ="Freizeit", tag2 ="Teil 2", tag3 ="Ort" where name = "outside"</v>
+        <v>update signs set name_de = "Draußen", mnemonic = "Nach draußen zeigen", tag1 ="Freizeit", tag2 ="Teil 2", tag3 ="Ort" where name = "outside";</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.35">
@@ -6311,7 +6262,7 @@
       </c>
       <c r="H130" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "haben/mein", mnemonic = "Handfläche auf Brustkorb legen", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="Verb" where name = "owning"</v>
+        <v>update signs set name_de = "haben/mein", mnemonic = "Handfläche auf Brustkorb legen", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="Verb" where name = "owning";</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.35">
@@ -6334,8 +6285,8 @@
         <v>820</v>
       </c>
       <c r="H131" t="str">
-        <f t="shared" ref="H131:H194" si="2">"update signs set name_de = """&amp;B131&amp;""", mnemonic = """&amp;C131&amp;""", tag1 ="""&amp;D131&amp;""", tag2 ="""&amp;E131&amp;""", tag3 ="""&amp;F131&amp;""" where name = """&amp;A131&amp;""""</f>
-        <v>update signs set name_de = "Schmerzen", mnemonic = "Handfläche vibriert vor Schmerzstelle", tag1 ="Krankheit", tag2 ="Teil 3", tag3 ="" where name = "pain"</v>
+        <f t="shared" ref="H131:H194" si="2">"update signs set name_de = """&amp;B131&amp;""", mnemonic = """&amp;C131&amp;""", tag1 ="""&amp;D131&amp;""", tag2 ="""&amp;E131&amp;""", tag3 ="""&amp;F131&amp;""" where name = """&amp;A131&amp;""";"</f>
+        <v>update signs set name_de = "Schmerzen", mnemonic = "Handfläche vibriert vor Schmerzstelle", tag1 ="Krankheit", tag2 ="Teil 3", tag3 ="" where name = "pain";</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.35">
@@ -6362,7 +6313,7 @@
       </c>
       <c r="H132" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Malen", mnemonic = "Großflächig in Luft malen", tag1 ="Freizeit", tag2 ="Teil 2", tag3 ="Verb" where name = "painting"</v>
+        <v>update signs set name_de = "Malen", mnemonic = "Großflächig in Luft malen", tag1 ="Freizeit", tag2 ="Teil 2", tag3 ="Verb" where name = "painting";</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.35">
@@ -6386,7 +6337,7 @@
       </c>
       <c r="H133" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Papa", mnemonic = "Schnauzbart andeuten", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "papa"</v>
+        <v>update signs set name_de = "Papa", mnemonic = "Schnauzbart andeuten", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "papa";</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.35">
@@ -6413,7 +6364,7 @@
       </c>
       <c r="H134" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Papier", mnemonic = "Fäuste klopfen 2x aneinander", tag1 ="Arbeit", tag2 ="Teil 2", tag3 ="Freizeit" where name = "paper"</v>
+        <v>update signs set name_de = "Papier", mnemonic = "Fäuste klopfen 2x aneinander", tag1 ="Arbeit", tag2 ="Teil 2", tag3 ="Freizeit" where name = "paper";</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.35">
@@ -6440,7 +6391,7 @@
       </c>
       <c r="H135" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Bild", mnemonic = "DIN A4-Blatt in die Luft malen", tag1 ="Freizeit", tag2 ="Teil 2", tag3 ="Haus" where name = "picture"</v>
+        <v>update signs set name_de = "Bild", mnemonic = "DIN A4-Blatt in die Luft malen", tag1 ="Freizeit", tag2 ="Teil 2", tag3 ="Haus" where name = "picture";</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.35">
@@ -6464,7 +6415,7 @@
       </c>
       <c r="H136" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Schwein", mnemonic = "Schnauze nach vorn ziehen", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "pig"</v>
+        <v>update signs set name_de = "Schwein", mnemonic = "Schnauze nach vorn ziehen", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "pig";</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.35">
@@ -6488,7 +6439,7 @@
       </c>
       <c r="H137" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Tablette", mnemonic = "Tablette auf Handfläche malen", tag1 ="Krankheit", tag2 ="Teil 3", tag3 ="" where name = "pill"</v>
+        <v>update signs set name_de = "Tablette", mnemonic = "Tablette auf Handfläche malen", tag1 ="Krankheit", tag2 ="Teil 3", tag3 ="" where name = "pill";</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.35">
@@ -6515,7 +6466,7 @@
       </c>
       <c r="H138" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Rosa/Pink", mnemonic = "Rosa Rose öffnet sich unter Nase", tag1 ="Farbe", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "pink"</v>
+        <v>update signs set name_de = "Rosa/Pink", mnemonic = "Rosa Rose öffnet sich unter Nase", tag1 ="Farbe", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "pink";</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.35">
@@ -6542,7 +6493,7 @@
       </c>
       <c r="H139" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Teller", mnemonic = "Mit Zeigefinger Teller auf Handfläche malen", tag1 ="Ernährung", tag2 ="Teil 2", tag3 ="Geschirr" where name = "plate"</v>
+        <v>update signs set name_de = "Teller", mnemonic = "Mit Zeigefinger Teller auf Handfläche malen", tag1 ="Ernährung", tag2 ="Teil 2", tag3 ="Geschirr" where name = "plate";</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.35">
@@ -6569,7 +6520,7 @@
       </c>
       <c r="H140" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Spielen", mnemonic = "Fächerhände 2x gegengleich auf- und abbewegen", tag1 ="Freizeit", tag2 ="Teil 1", tag3 ="Verb" where name = "playing"</v>
+        <v>update signs set name_de = "Spielen", mnemonic = "Fächerhände 2x gegengleich auf- und abbewegen", tag1 ="Freizeit", tag2 ="Teil 1", tag3 ="Verb" where name = "playing";</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.35">
@@ -6596,7 +6547,7 @@
       </c>
       <c r="H141" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Bitte", mnemonic = "2x Handflächen aneinander", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Kleine Worte" where name = "please"</v>
+        <v>update signs set name_de = "Bitte", mnemonic = "2x Handflächen aneinander", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Kleine Worte" where name = "please";</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.35">
@@ -6623,7 +6574,7 @@
       </c>
       <c r="H142" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Sich übergeben", mnemonic = "Den Weg von unten aus Mund heraus", tag1 ="Krankheit", tag2 ="Teil 3", tag3 ="Verb" where name = "puke"</v>
+        <v>update signs set name_de = "Sich übergeben", mnemonic = "Den Weg von unten aus Mund heraus", tag1 ="Krankheit", tag2 ="Teil 3", tag3 ="Verb" where name = "puke";</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.35">
@@ -6647,7 +6598,7 @@
       </c>
       <c r="H143" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Hase", mnemonic = "Zeige-und Mittelfinger zeigen Ohren", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "rabbit"</v>
+        <v>update signs set name_de = "Hase", mnemonic = "Zeige-und Mittelfinger zeigen Ohren", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "rabbit";</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.35">
@@ -6674,7 +6625,7 @@
       </c>
       <c r="H144" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Lesen", mnemonic = "Auf Handfläche lesen", tag1 ="Freizeit", tag2 ="Teil 2", tag3 ="Verb" where name = "reading"</v>
+        <v>update signs set name_de = "Lesen", mnemonic = "Auf Handfläche lesen", tag1 ="Freizeit", tag2 ="Teil 2", tag3 ="Verb" where name = "reading";</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.35">
@@ -6701,7 +6652,7 @@
       </c>
       <c r="H145" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Rot", mnemonic = "Lippenrot zeigen", tag1 ="Farbe", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "red"</v>
+        <v>update signs set name_de = "Rot", mnemonic = "Lippenrot zeigen", tag1 ="Farbe", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "red";</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.35">
@@ -6725,7 +6676,7 @@
       </c>
       <c r="H146" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Brötchen", mnemonic = "2x Brötchen formen", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "roll"</v>
+        <v>update signs set name_de = "Brötchen", mnemonic = "2x Brötchen formen", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "roll";</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.35">
@@ -6749,7 +6700,7 @@
       </c>
       <c r="H147" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Zimmer", mnemonic = "Zeigefinger ziehen Mauer um Zimmer", tag1 ="Haus", tag2 ="Teil 3", tag3 ="" where name = "room"</v>
+        <v>update signs set name_de = "Zimmer", mnemonic = "Zeigefinger ziehen Mauer um Zimmer", tag1 ="Haus", tag2 ="Teil 3", tag3 ="" where name = "room";</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.35">
@@ -6776,7 +6727,7 @@
       </c>
       <c r="H148" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Rennen/Laufen", mnemonic = "Mit Armen 'rennen'", tag1 ="Freizeit", tag2 ="Teil 3", tag3 ="Verb" where name = "run"</v>
+        <v>update signs set name_de = "Rennen/Laufen", mnemonic = "Mit Armen 'rennen'", tag1 ="Freizeit", tag2 ="Teil 3", tag3 ="Verb" where name = "run";</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.35">
@@ -6800,7 +6751,7 @@
       </c>
       <c r="H149" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Salz", mnemonic = "Prise", tag1 ="Lebensmittel", tag2 ="Teil 3", tag3 ="" where name = "salt"</v>
+        <v>update signs set name_de = "Salz", mnemonic = "Prise", tag1 ="Lebensmittel", tag2 ="Teil 3", tag3 ="" where name = "salt";</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.35">
@@ -6824,7 +6775,7 @@
       </c>
       <c r="H150" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Sand", mnemonic = "Sand aufnehmen und rieseln", tag1 ="Spielen", tag2 ="Teil 2", tag3 ="" where name = "sand"</v>
+        <v>update signs set name_de = "Sand", mnemonic = "Sand aufnehmen und rieseln", tag1 ="Spielen", tag2 ="Teil 2", tag3 ="" where name = "sand";</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.35">
@@ -6851,7 +6802,7 @@
       </c>
       <c r="H151" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Schule", mnemonic = "Kreide an der Tafel", tag1 ="Arbeit", tag2 ="Teil 2", tag3 ="Haus" where name = "school"</v>
+        <v>update signs set name_de = "Schule", mnemonic = "Kreide an der Tafel", tag1 ="Arbeit", tag2 ="Teil 2", tag3 ="Haus" where name = "school";</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.35">
@@ -6878,7 +6829,7 @@
       </c>
       <c r="H152" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Schere/Schneiden", mnemonic = "Scherbewegung mimen", tag1 ="Freizeit", tag2 ="Teil 2", tag3 ="Arbeit" where name = "scissors"</v>
+        <v>update signs set name_de = "Schere/Schneiden", mnemonic = "Scherbewegung mimen", tag1 ="Freizeit", tag2 ="Teil 2", tag3 ="Arbeit" where name = "scissors";</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.35">
@@ -6905,7 +6856,7 @@
       </c>
       <c r="H153" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Schimpfen", mnemonic = "Wie die Geste", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Verb" where name = "scolding"</v>
+        <v>update signs set name_de = "Schimpfen", mnemonic = "Wie die Geste", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Verb" where name = "scolding";</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.35">
@@ -6932,7 +6883,7 @@
       </c>
       <c r="H154" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Rasieren", mnemonic = "Rasierer halten und rasieren mimen", tag1 ="Körperpflege", tag2 ="Teil 3", tag3 ="Verb" where name = "shave"</v>
+        <v>update signs set name_de = "Rasieren", mnemonic = "Rasierer halten und rasieren mimen", tag1 ="Körperpflege", tag2 ="Teil 3", tag3 ="Verb" where name = "shave";</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.35">
@@ -6956,7 +6907,7 @@
       </c>
       <c r="H155" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Schaf", mnemonic = "Wolle am Bauch zeigen", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "sheep"</v>
+        <v>update signs set name_de = "Schaf", mnemonic = "Wolle am Bauch zeigen", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "sheep";</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.35">
@@ -6980,7 +6931,7 @@
       </c>
       <c r="H156" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Schiff/Boot", mnemonic = "Mit Handflächen Bug nach vorn fahren", tag1 ="Fahrzeug", tag2 ="Teil 3", tag3 ="" where name = "ship"</v>
+        <v>update signs set name_de = "Schiff/Boot", mnemonic = "Mit Handflächen Bug nach vorn fahren", tag1 ="Fahrzeug", tag2 ="Teil 3", tag3 ="" where name = "ship";</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.35">
@@ -7007,7 +6958,7 @@
       </c>
       <c r="H157" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Duschen", mnemonic = "Über dem Kopf duschen", tag1 ="Körperpflege", tag2 ="Teil 1", tag3 ="Verb" where name = "showering"</v>
+        <v>update signs set name_de = "Duschen", mnemonic = "Über dem Kopf duschen", tag1 ="Körperpflege", tag2 ="Teil 1", tag3 ="Verb" where name = "showering";</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.35">
@@ -7031,7 +6982,7 @@
       </c>
       <c r="H158" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Bruder/Schwester", mnemonic = "Gestreckte Zeigefinger aneinander führen", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "sibling"</v>
+        <v>update signs set name_de = "Bruder/Schwester", mnemonic = "Gestreckte Zeigefinger aneinander führen", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "sibling";</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.35">
@@ -7058,7 +7009,7 @@
       </c>
       <c r="H159" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Krank", mnemonic = "Krallhand klopft 2x auf Brustkorb", tag1 ="Krankheit", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "sick"</v>
+        <v>update signs set name_de = "Krank", mnemonic = "Krallhand klopft 2x auf Brustkorb", tag1 ="Krankheit", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "sick";</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.35">
@@ -7085,7 +7036,7 @@
       </c>
       <c r="H160" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Waschbecken", mnemonic = "Handschüsseln formen Waschbecken", tag1 ="Haus", tag2 ="Teil 3", tag3 ="Körperpflege" where name = "sink"</v>
+        <v>update signs set name_de = "Waschbecken", mnemonic = "Handschüsseln formen Waschbecken", tag1 ="Haus", tag2 ="Teil 3", tag3 ="Körperpflege" where name = "sink";</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.35">
@@ -7112,7 +7063,7 @@
       </c>
       <c r="H161" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Sitzen", mnemonic = "Häschenhand zieht von oben nach unten", tag1 ="Arbeit", tag2 ="Teil 1", tag3 ="Verb" where name = "sit"</v>
+        <v>update signs set name_de = "Sitzen", mnemonic = "Häschenhand zieht von oben nach unten", tag1 ="Arbeit", tag2 ="Teil 1", tag3 ="Verb" where name = "sit";</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.35">
@@ -7139,7 +7090,7 @@
       </c>
       <c r="H162" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Klein", mnemonic = "Handflächen 20 cm breit auseinander", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "small"</v>
+        <v>update signs set name_de = "Klein", mnemonic = "Handflächen 20 cm breit auseinander", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "small";</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.35">
@@ -7166,7 +7117,7 @@
       </c>
       <c r="H163" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Etw. anderes", mnemonic = "Zeigefinger deuten viele andere Möglichkeiten an", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Kleine Worte" where name = "something_else"</v>
+        <v>update signs set name_de = "Etw. anderes", mnemonic = "Zeigefinger deuten viele andere Möglichkeiten an", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Kleine Worte" where name = "something_else";</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.35">
@@ -7193,7 +7144,7 @@
       </c>
       <c r="H164" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Löffel", mnemonic = "2x in Mund löffeln", tag1 ="Ernährung", tag2 ="Teil 2", tag3 ="Besteck" where name = "spoon"</v>
+        <v>update signs set name_de = "Löffel", mnemonic = "2x in Mund löffeln", tag1 ="Ernährung", tag2 ="Teil 2", tag3 ="Besteck" where name = "spoon";</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.35">
@@ -7220,7 +7171,7 @@
       </c>
       <c r="H165" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Stehen", mnemonic = "Zeige-und Mittelfinger  stehen auf Handfläche", tag1 ="Alltag", tag2 ="Teil 1", tag3 ="Verb" where name = "stand"</v>
+        <v>update signs set name_de = "Stehen", mnemonic = "Zeige-und Mittelfinger  stehen auf Handfläche", tag1 ="Alltag", tag2 ="Teil 1", tag3 ="Verb" where name = "stand";</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.35">
@@ -7247,7 +7198,7 @@
       </c>
       <c r="H166" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Aufstehen", mnemonic = "Wie der Pfarrer in der Kirche", tag1 ="Alltag", tag2 ="Teil 1", tag3 ="Verb" where name = "stand_up"</v>
+        <v>update signs set name_de = "Aufstehen", mnemonic = "Wie der Pfarrer in der Kirche", tag1 ="Alltag", tag2 ="Teil 1", tag3 ="Verb" where name = "stand_up";</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.35">
@@ -7274,7 +7225,7 @@
       </c>
       <c r="H167" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Stopp", mnemonic = "Halt zeigen", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Kleine Worte" where name = "stop"</v>
+        <v>update signs set name_de = "Stopp", mnemonic = "Halt zeigen", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Kleine Worte" where name = "stop";</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.35">
@@ -7298,7 +7249,7 @@
       </c>
       <c r="H168" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Zucker", mnemonic = "Erst 'süß' zeigen, dann mit Fingern streuen", tag1 ="Lebensmittel", tag2 ="Teil 3", tag3 ="" where name = "sugar"</v>
+        <v>update signs set name_de = "Zucker", mnemonic = "Erst 'süß' zeigen, dann mit Fingern streuen", tag1 ="Lebensmittel", tag2 ="Teil 3", tag3 ="" where name = "sugar";</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.35">
@@ -7325,7 +7276,7 @@
       </c>
       <c r="H169" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Schwimmen", mnemonic = "Brustschwimmen mimen", tag1 ="Freizeit", tag2 ="Teil 3", tag3 ="Verb" where name = "swimming"</v>
+        <v>update signs set name_de = "Schwimmen", mnemonic = "Brustschwimmen mimen", tag1 ="Freizeit", tag2 ="Teil 3", tag3 ="Verb" where name = "swimming";</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.35">
@@ -7352,7 +7303,7 @@
       </c>
       <c r="H170" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Etw. ausschalten", mnemonic = "Klappe zu!", tag1 ="Eigenschaften", tag2 ="Teil 1", tag3 ="Verb" where name = "switch_off"</v>
+        <v>update signs set name_de = "Etw. ausschalten", mnemonic = "Klappe zu!", tag1 ="Eigenschaften", tag2 ="Teil 1", tag3 ="Verb" where name = "switch_off";</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.35">
@@ -7379,7 +7330,7 @@
       </c>
       <c r="H171" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Etw. anschalten", mnemonic = "Daumen drückt Schalter", tag1 ="Eigenschaften", tag2 ="Teil 1", tag3 ="Verb" where name = "switch_on"</v>
+        <v>update signs set name_de = "Etw. anschalten", mnemonic = "Daumen drückt Schalter", tag1 ="Eigenschaften", tag2 ="Teil 1", tag3 ="Verb" where name = "switch_on";</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.35">
@@ -7403,7 +7354,7 @@
       </c>
       <c r="H172" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Tisch", mnemonic = "Tischfläche von innen nach außen streichen", tag1 ="Haus", tag2 ="Teil 1", tag3 ="" where name = "table"</v>
+        <v>update signs set name_de = "Tisch", mnemonic = "Tischfläche von innen nach außen streichen", tag1 ="Haus", tag2 ="Teil 1", tag3 ="" where name = "table";</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.35">
@@ -7430,7 +7381,7 @@
       </c>
       <c r="H173" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Tee", mnemonic = "Teebeutel auf-und abschwenken", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="Getränk" where name = "tea"</v>
+        <v>update signs set name_de = "Tee", mnemonic = "Teebeutel auf-und abschwenken", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="Getränk" where name = "tea";</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.35">
@@ -7457,7 +7408,7 @@
       </c>
       <c r="H174" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Telefon", mnemonic = "Y-Hand an Ohr", tag1 ="Interaktion", tag2 ="Teil 2", tag3 ="Alltag" where name = "telephone"</v>
+        <v>update signs set name_de = "Telefon", mnemonic = "Y-Hand an Ohr", tag1 ="Interaktion", tag2 ="Teil 2", tag3 ="Alltag" where name = "telephone";</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.35">
@@ -7481,7 +7432,7 @@
       </c>
       <c r="H175" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Danke", mnemonic = "Wie die Queen; vom Kinn aus nach vorn", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="" where name = "thank_you"</v>
+        <v>update signs set name_de = "Danke", mnemonic = "Wie die Queen; vom Kinn aus nach vorn", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="" where name = "thank_you";</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.35">
@@ -7508,7 +7459,7 @@
       </c>
       <c r="H176" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Da", mnemonic = "Zeigen", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Kleine Worte" where name = "there"</v>
+        <v>update signs set name_de = "Da", mnemonic = "Zeigen", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Kleine Worte" where name = "there";</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.35">
@@ -7535,7 +7486,7 @@
       </c>
       <c r="H177" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Denken/Schlau", mnemonic = "Mit Zeigefinger auf Kopf tippen", tag1 ="Arbeit", tag2 ="Teil 2", tag3 ="Verb" where name = "thinking"</v>
+        <v>update signs set name_de = "Denken/Schlau", mnemonic = "Mit Zeigefinger auf Kopf tippen", tag1 ="Arbeit", tag2 ="Teil 2", tag3 ="Verb" where name = "thinking";</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.35">
@@ -7562,7 +7513,7 @@
       </c>
       <c r="H178" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Aufräumen", mnemonic = "3x einen Stapel zusammenschieben", tag1 ="Spielen", tag2 ="Teil 1", tag3 ="Verb" where name = "tidy_up"</v>
+        <v>update signs set name_de = "Aufräumen", mnemonic = "3x einen Stapel zusammenschieben", tag1 ="Spielen", tag2 ="Teil 1", tag3 ="Verb" where name = "tidy_up";</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.35">
@@ -7589,7 +7540,7 @@
       </c>
       <c r="H179" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Winzig/Wenig", mnemonic = "Zeigefinger und Daumen zeigen 'wenig'", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="Menge" where name = "tiny"</v>
+        <v>update signs set name_de = "Winzig/Wenig", mnemonic = "Zeigefinger und Daumen zeigen 'wenig'", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="Menge" where name = "tiny";</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.35">
@@ -7613,7 +7564,7 @@
       </c>
       <c r="H180" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Heute", mnemonic = "2x langsam vor sich nach unten zeigen", tag1 ="Zeit", tag2 ="Teil 3", tag3 ="" where name = "today"</v>
+        <v>update signs set name_de = "Heute", mnemonic = "2x langsam vor sich nach unten zeigen", tag1 ="Zeit", tag2 ="Teil 3", tag3 ="" where name = "today";</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.35">
@@ -7640,7 +7591,7 @@
       </c>
       <c r="H181" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Toilette", mnemonic = "Y-Hand dreht neben Kopf", tag1 ="Körperpflege", tag2 ="Teil 1", tag3 ="Alltag" where name = "toilet"</v>
+        <v>update signs set name_de = "Toilette", mnemonic = "Y-Hand dreht neben Kopf", tag1 ="Körperpflege", tag2 ="Teil 1", tag3 ="Alltag" where name = "toilet";</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.35">
@@ -7664,7 +7615,7 @@
       </c>
       <c r="H182" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Tomate", mnemonic = "Tomate vom Busch abdrehen", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "tomato"</v>
+        <v>update signs set name_de = "Tomate", mnemonic = "Tomate vom Busch abdrehen", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "tomato";</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.35">
@@ -7688,7 +7639,7 @@
       </c>
       <c r="H183" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Morgen", mnemonic = "Großen Bogen nach vorn zeigen", tag1 ="Zeit", tag2 ="Teil 3", tag3 ="" where name = "tomorrow"</v>
+        <v>update signs set name_de = "Morgen", mnemonic = "Großen Bogen nach vorn zeigen", tag1 ="Zeit", tag2 ="Teil 3", tag3 ="" where name = "tomorrow";</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.35">
@@ -7712,7 +7663,7 @@
       </c>
       <c r="H184" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Handtuch", mnemonic = "Handtuch mit Zeigefinger umfahren", tag1 ="Körperpflege", tag2 ="Teil 3", tag3 ="" where name = "towel"</v>
+        <v>update signs set name_de = "Handtuch", mnemonic = "Handtuch mit Zeigefinger umfahren", tag1 ="Körperpflege", tag2 ="Teil 3", tag3 ="" where name = "towel";</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.35">
@@ -7736,7 +7687,7 @@
       </c>
       <c r="H185" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Kuscheltier", mnemonic = "Kuscheln zeigen", tag1 ="Spielen", tag2 ="Teil 2", tag3 ="" where name = "toy"</v>
+        <v>update signs set name_de = "Kuscheltier", mnemonic = "Kuscheln zeigen", tag1 ="Spielen", tag2 ="Teil 2", tag3 ="" where name = "toy";</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.35">
@@ -7763,7 +7714,7 @@
       </c>
       <c r="H186" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Zug/Eisenbahn", mnemonic = "Neben Körper Räderdrehen zeigen", tag1 ="Fahrzeug", tag2 ="Teil 3", tag3 ="Spielen" where name = "train"</v>
+        <v>update signs set name_de = "Zug/Eisenbahn", mnemonic = "Neben Körper Räderdrehen zeigen", tag1 ="Fahrzeug", tag2 ="Teil 3", tag3 ="Spielen" where name = "train";</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.35">
@@ -7790,7 +7741,7 @@
       </c>
       <c r="H187" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Baum", mnemonic = "Arm=Baumstamm, Finger=Äste", tag1 ="draußen", tag2 ="Teil 2", tag3 ="Pflanzen" where name = "tree"</v>
+        <v>update signs set name_de = "Baum", mnemonic = "Arm=Baumstamm, Finger=Äste", tag1 ="draußen", tag2 ="Teil 2", tag3 ="Pflanzen" where name = "tree";</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.35">
@@ -7817,7 +7768,7 @@
       </c>
       <c r="H188" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Hinfallen", mnemonic = "Nach vorn abstützen", tag1 ="Alltag", tag2 ="Teil 3", tag3 ="Verb" where name = "tumbling"</v>
+        <v>update signs set name_de = "Hinfallen", mnemonic = "Nach vorn abstützen", tag1 ="Alltag", tag2 ="Teil 3", tag3 ="Verb" where name = "tumbling";</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.35">
@@ -7844,7 +7795,7 @@
       </c>
       <c r="H189" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Fernseher/Fernsehen", mnemonic = "Fernbedienung tippen", tag1 ="Haus", tag2 ="Teil 2", tag3 ="Freizeit" where name = "tv"</v>
+        <v>update signs set name_de = "Fernseher/Fernsehen", mnemonic = "Fernbedienung tippen", tag1 ="Haus", tag2 ="Teil 2", tag3 ="Freizeit" where name = "tv";</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.35">
@@ -7871,7 +7822,7 @@
       </c>
       <c r="H190" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Zwei", mnemonic = "Zwei Finger", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="Menge" where name = "two"</v>
+        <v>update signs set name_de = "Zwei", mnemonic = "Zwei Finger", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="Menge" where name = "two";</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.35">
@@ -7895,7 +7846,7 @@
       </c>
       <c r="H191" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Oben/Hoch", mnemonic = "Nach oben zeigen", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="" where name = "up"</v>
+        <v>update signs set name_de = "Oben/Hoch", mnemonic = "Nach oben zeigen", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="" where name = "up";</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.35">
@@ -7922,7 +7873,7 @@
       </c>
       <c r="H192" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Warte/Langsam", mnemonic = "verlangsamende Bewegung", tag1 ="Eigenschaften", tag2 ="Teil 1", tag3 ="Verb" where name = "wait"</v>
+        <v>update signs set name_de = "Warte/Langsam", mnemonic = "verlangsamende Bewegung", tag1 ="Eigenschaften", tag2 ="Teil 1", tag3 ="Verb" where name = "wait";</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.35">
@@ -7949,7 +7900,7 @@
       </c>
       <c r="H193" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Gehen", mnemonic = "Zeige-und Mittelfinger spazieren", tag1 ="Alltag", tag2 ="Teil 3", tag3 ="Verb" where name = "walk"</v>
+        <v>update signs set name_de = "Gehen", mnemonic = "Zeige-und Mittelfinger spazieren", tag1 ="Alltag", tag2 ="Teil 3", tag3 ="Verb" where name = "walk";</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.35">
@@ -7973,7 +7924,7 @@
       </c>
       <c r="H194" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Waschen", mnemonic = "Hände waschen sich", tag1 ="Körperpflege", tag2 ="Teil 1", tag3 ="" where name = "washing"</v>
+        <v>update signs set name_de = "Waschen", mnemonic = "Hände waschen sich", tag1 ="Körperpflege", tag2 ="Teil 1", tag3 ="" where name = "washing";</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.35">
@@ -7999,8 +7950,8 @@
         <v>820</v>
       </c>
       <c r="H195" t="str">
-        <f t="shared" ref="H195:H211" si="3">"update signs set name_de = """&amp;B195&amp;""", mnemonic = """&amp;C195&amp;""", tag1 ="""&amp;D195&amp;""", tag2 ="""&amp;E195&amp;""", tag3 ="""&amp;F195&amp;""" where name = """&amp;A195&amp;""""</f>
-        <v>update signs set name_de = "Wasser", mnemonic = "Steht mir bis zum Hals", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="Getränk" where name = "water"</v>
+        <f t="shared" ref="H195:H211" si="3">"update signs set name_de = """&amp;B195&amp;""", mnemonic = """&amp;C195&amp;""", tag1 ="""&amp;D195&amp;""", tag2 ="""&amp;E195&amp;""", tag3 ="""&amp;F195&amp;""" where name = """&amp;A195&amp;""";"</f>
+        <v>update signs set name_de = "Wasser", mnemonic = "Steht mir bis zum Hals", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="Getränk" where name = "water";</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.35">
@@ -8027,7 +7978,7 @@
       </c>
       <c r="H196" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Wir", mnemonic = "Auf alle und sich selbst zeigen", tag1 ="Personen", tag2 ="Teil 1", tag3 ="Kleine Worte" where name = "we"</v>
+        <v>update signs set name_de = "Wir", mnemonic = "Auf alle und sich selbst zeigen", tag1 ="Personen", tag2 ="Teil 1", tag3 ="Kleine Worte" where name = "we";</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.35">
@@ -8051,7 +8002,7 @@
       </c>
       <c r="H197" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Was?", mnemonic = "Handflächen hin und her schütteln", tag1 ="Frage", tag2 ="Teil 1", tag3 ="" where name = "what"</v>
+        <v>update signs set name_de = "Was?", mnemonic = "Handflächen hin und her schütteln", tag1 ="Frage", tag2 ="Teil 1", tag3 ="" where name = "what";</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.35">
@@ -8075,7 +8026,7 @@
       </c>
       <c r="H198" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Wann?", mnemonic = "Finger klopfen ungeduldig an Wange", tag1 ="Frage", tag2 ="Teil 3", tag3 ="" where name = "when"</v>
+        <v>update signs set name_de = "Wann?", mnemonic = "Finger klopfen ungeduldig an Wange", tag1 ="Frage", tag2 ="Teil 3", tag3 ="" where name = "when";</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.35">
@@ -8099,7 +8050,7 @@
       </c>
       <c r="H199" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Wo?", mnemonic = "Schüssel mit Händen nachahmen", tag1 ="Frage", tag2 ="Teil 1", tag3 ="" where name = "where"</v>
+        <v>update signs set name_de = "Wo?", mnemonic = "Schüssel mit Händen nachahmen", tag1 ="Frage", tag2 ="Teil 1", tag3 ="" where name = "where";</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.35">
@@ -8123,7 +8074,7 @@
       </c>
       <c r="H200" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Wer?", mnemonic = "Fingeralphabet-R wackelt", tag1 ="Frage", tag2 ="Teil 3", tag3 ="" where name = "who"</v>
+        <v>update signs set name_de = "Wer?", mnemonic = "Fingeralphabet-R wackelt", tag1 ="Frage", tag2 ="Teil 3", tag3 ="" where name = "who";</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.35">
@@ -8147,7 +8098,7 @@
       </c>
       <c r="H201" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Fenster", mnemonic = "Mit Zeigefingern Fenster in Luft malen", tag1 ="Haus", tag2 ="Teil 2", tag3 ="" where name = "window"</v>
+        <v>update signs set name_de = "Fenster", mnemonic = "Mit Zeigefingern Fenster in Luft malen", tag1 ="Haus", tag2 ="Teil 2", tag3 ="" where name = "window";</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.35">
@@ -8171,7 +8122,7 @@
       </c>
       <c r="H202" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Mit", mnemonic = "Daumen kommt mit anderen Fingern mit", tag1 ="Kleine Worte", tag2 ="Teil 2", tag3 ="" where name = "with"</v>
+        <v>update signs set name_de = "Mit", mnemonic = "Daumen kommt mit anderen Fingern mit", tag1 ="Kleine Worte", tag2 ="Teil 2", tag3 ="" where name = "with";</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.35">
@@ -8195,7 +8146,7 @@
       </c>
       <c r="H203" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Frau", mnemonic = "Ohrring", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "woman"</v>
+        <v>update signs set name_de = "Frau", mnemonic = "Ohrring", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "woman";</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.35">
@@ -8222,7 +8173,7 @@
       </c>
       <c r="H204" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Stift/Schreiben", mnemonic = "Mit Stift schreiben mimen", tag1 ="Arbeit", tag2 ="Teil 2", tag3 ="Verb" where name = "writing"</v>
+        <v>update signs set name_de = "Stift/Schreiben", mnemonic = "Mit Stift schreiben mimen", tag1 ="Arbeit", tag2 ="Teil 2", tag3 ="Verb" where name = "writing";</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.35">
@@ -8249,7 +8200,7 @@
       </c>
       <c r="H205" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Gelb", mnemonic = "Y-Hand (Yellow) dreht im Handgelenk", tag1 ="Farbe", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "yellow"</v>
+        <v>update signs set name_de = "Gelb", mnemonic = "Y-Hand (Yellow) dreht im Handgelenk", tag1 ="Farbe", tag2 ="Teil 3", tag3 ="Eigenschaften" where name = "yellow";</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.35">
@@ -8276,7 +8227,7 @@
       </c>
       <c r="H206" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Ja", mnemonic = "Nicken", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Kleine Worte" where name = "yes"</v>
+        <v>update signs set name_de = "Ja", mnemonic = "Nicken", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Kleine Worte" where name = "yes";</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.35">
@@ -8300,7 +8251,7 @@
       </c>
       <c r="H207" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Gestern", mnemonic = "Großen Bogen  nach hinten zeigen", tag1 ="Zeit", tag2 ="Teil 3", tag3 ="" where name = "yesterday"</v>
+        <v>update signs set name_de = "Gestern", mnemonic = "Großen Bogen  nach hinten zeigen", tag1 ="Zeit", tag2 ="Teil 3", tag3 ="" where name = "yesterday";</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.35">
@@ -8324,7 +8275,7 @@
       </c>
       <c r="H208" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Joghurt", mnemonic = "Becher auslöffen", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "yoghurt"</v>
+        <v>update signs set name_de = "Joghurt", mnemonic = "Becher auslöffen", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "yoghurt";</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.35">
@@ -8351,7 +8302,7 @@
       </c>
       <c r="H209" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Du", mnemonic = "mit Zeigefinger auf Gegenüber zeigen", tag1 ="Person", tag2 ="Teil 1", tag3 ="Kleine Worte" where name = "you"</v>
+        <v>update signs set name_de = "Du", mnemonic = "mit Zeigefinger auf Gegenüber zeigen", tag1 ="Person", tag2 ="Teil 1", tag3 ="Kleine Worte" where name = "you";</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.35">
@@ -8378,7 +8329,7 @@
       </c>
       <c r="H210" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Du hilfst Mir", mnemonic = "2. Hand hilft der anderen", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Verb" where name = "you_help_me"</v>
+        <v>update signs set name_de = "Du hilfst Mir", mnemonic = "2. Hand hilft der anderen", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="Verb" where name = "you_help_me";</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.35">
@@ -8402,7 +8353,7 @@
       </c>
       <c r="H211" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Dein", mnemonic = "Handfläche zeigt langsam auf Gesprächspartner", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="" where name = "yours"</v>
+        <v>update signs set name_de = "Dein", mnemonic = "Handfläche zeigt langsam auf Gesprächspartner", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="" where name = "yours";</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
#97 Tag3 is only set when it is not null.
</commit_message>
<xml_diff>
--- a/database/VideosUkGebärden.xlsx
+++ b/database/VideosUkGebärden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User-Matthias\Dev\Android\UKGM\src\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2B944E-8B07-44CD-A7FB-D1B076536E84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15592425-DF67-4987-8294-C604F13DB3C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{978A20FD-486C-4CB5-9933-67C562CBE71F}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="834">
   <si>
     <t>afterwards</t>
   </si>
@@ -2489,9 +2489,6 @@
     <t>Behinderung</t>
   </si>
   <si>
-    <t>kleine _Worte</t>
-  </si>
-  <si>
     <t>Krankheit</t>
   </si>
   <si>
@@ -2502,9 +2499,6 @@
   </si>
   <si>
     <t>weg!</t>
-  </si>
-  <si>
-    <t>kleine Wörter</t>
   </si>
   <si>
     <t>Menge</t>
@@ -2969,7 +2963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C22E1E0-4D2F-4ED8-9423-514FCF041C4D}">
   <dimension ref="A1:H264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G197" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G200" workbookViewId="0">
       <selection activeCell="H212" sqref="H212"/>
     </sheetView>
   </sheetViews>
@@ -2983,28 +2977,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>820</v>
+      </c>
+      <c r="B1" t="s">
+        <v>821</v>
+      </c>
+      <c r="C1" t="s">
         <v>822</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>823</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>824</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>825</v>
       </c>
-      <c r="E1" t="s">
-        <v>826</v>
-      </c>
-      <c r="F1" t="s">
-        <v>827</v>
-      </c>
       <c r="G1" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="H1" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -3024,11 +3018,11 @@
         <v>792</v>
       </c>
       <c r="G2" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H2" t="str">
-        <f>"update signs set name_de = """&amp;B2&amp;""", mnemonic = """&amp;C2&amp;""", tag1 ="""&amp;D2&amp;""", tag2 ="""&amp;E2&amp;""", tag3 ="""&amp;F2&amp;""" where name = """&amp;A2&amp;""";"</f>
-        <v>update signs set name_de = "Dann/Danach", mnemonic = "Die Zukunft liegt vor mir", tag1 ="Zeit", tag2 ="Teil 2", tag3 ="" where name = "afterwards";</v>
+        <f>IF(NOT(ISBLANK(F2)),"update signs set name_de = """&amp;B2&amp;""", mnemonic = """&amp;C2&amp;""", tag1 ="""&amp;D2&amp;""", tag2 ="""&amp;E2&amp;""", tag3 ="""&amp;F2&amp;""" where name = """&amp;A2&amp;""";","update signs set name_de = """&amp;B2&amp;""", mnemonic = """&amp;C2&amp;""", tag1 ="""&amp;D2&amp;""", tag2 ="""&amp;E2&amp;""" where name = """&amp;A2&amp;""";")</f>
+        <v>update signs set name_de = "Dann/Danach", mnemonic = "Die Zukunft liegt vor mir", tag1 ="Zeit", tag2 ="Teil 2" where name = "afterwards";</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -3042,17 +3036,17 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E3" t="s">
         <v>793</v>
       </c>
       <c r="G3" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H66" si="0">"update signs set name_de = """&amp;B3&amp;""", mnemonic = """&amp;C3&amp;""", tag1 ="""&amp;D3&amp;""", tag2 ="""&amp;E3&amp;""", tag3 ="""&amp;F3&amp;""" where name = """&amp;A3&amp;""";"</f>
-        <v>update signs set name_de = "Noch mal", mnemonic = "Gebärde 'eins' kommt von hinten nach vorn", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="" where name = "again";</v>
+        <f t="shared" ref="H3:H66" si="0">IF(NOT(ISBLANK(F3)),"update signs set name_de = """&amp;B3&amp;""", mnemonic = """&amp;C3&amp;""", tag1 ="""&amp;D3&amp;""", tag2 ="""&amp;E3&amp;""", tag3 ="""&amp;F3&amp;""" where name = """&amp;A3&amp;""";","update signs set name_de = """&amp;B3&amp;""", mnemonic = """&amp;C3&amp;""", tag1 ="""&amp;D3&amp;""", tag2 ="""&amp;E3&amp;""" where name = """&amp;A3&amp;""";")</f>
+        <v>update signs set name_de = "Noch mal", mnemonic = "Gebärde 'eins' kommt von hinten nach vorn", tag1 ="Kleine Worte", tag2 ="Teil 1" where name = "again";</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -3072,11 +3066,11 @@
         <v>794</v>
       </c>
       <c r="G4" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Flugzeug/Fliegen", mnemonic = "Y-Hand startet vom Boden", tag1 ="Fahrzeug", tag2 ="Teil 3", tag3 ="" where name = "airplane";</v>
+        <v>update signs set name_de = "Flugzeug/Fliegen", mnemonic = "Y-Hand startet vom Boden", tag1 ="Fahrzeug", tag2 ="Teil 3" where name = "airplane";</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -3096,11 +3090,11 @@
         <v>794</v>
       </c>
       <c r="G5" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Allah", mnemonic = "Faust öffnet nach vorn", tag1 ="Religion", tag2 ="Teil 3", tag3 ="" where name = "allah";</v>
+        <v>update signs set name_de = "Allah", mnemonic = "Faust öffnet nach vorn", tag1 ="Religion", tag2 ="Teil 3" where name = "allah";</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -3114,17 +3108,17 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E6" t="s">
         <v>793</v>
       </c>
       <c r="G6" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Alleine", mnemonic = "Erhobenen Zeigefinger von oben nach unten ziehen", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="" where name = "alone";</v>
+        <v>update signs set name_de = "Alleine", mnemonic = "Erhobenen Zeigefinger von oben nach unten ziehen", tag1 ="Kleine Worte", tag2 ="Teil 1" where name = "alone";</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -3144,11 +3138,11 @@
         <v>794</v>
       </c>
       <c r="G7" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Entschuldigung", mnemonic = "Handfläche kreist auf Handrücken", tag1 ="Interaktion", tag2 ="Teil 3", tag3 ="" where name = "apology";</v>
+        <v>update signs set name_de = "Entschuldigung", mnemonic = "Handfläche kreist auf Handrücken", tag1 ="Interaktion", tag2 ="Teil 3" where name = "apology";</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -3168,11 +3162,11 @@
         <v>793</v>
       </c>
       <c r="G8" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Apfel", mnemonic = "Abbeißen", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "apple";</v>
+        <v>update signs set name_de = "Apfel", mnemonic = "Abbeißen", tag1 ="Lebensmittel", tag2 ="Teil 1" where name = "apple";</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -3180,7 +3174,7 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
@@ -3192,11 +3186,11 @@
         <v>792</v>
       </c>
       <c r="G9" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Geht es dir gut?", mnemonic = "Mit fragender Mimik 'du' und 'gut' gebärden", tag1 ="Interaktion", tag2 ="Teil 2", tag3 ="" where name = "are_you_ok";</v>
+        <v>update signs set name_de = "Geht es dir gut?", mnemonic = "Mit fragender Mimik 'du' und 'gut' gebärden", tag1 ="Interaktion", tag2 ="Teil 2" where name = "are_you_ok";</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -3210,7 +3204,7 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E10" t="s">
         <v>793</v>
@@ -3219,7 +3213,7 @@
         <v>683</v>
       </c>
       <c r="G10" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -3243,11 +3237,11 @@
         <v>793</v>
       </c>
       <c r="G11" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Baby", mnemonic = "Baby auf Arm schaukeln", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "baby";</v>
+        <v>update signs set name_de = "Baby", mnemonic = "Baby auf Arm schaukeln", tag1 ="Person", tag2 ="Teil 1" where name = "baby";</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -3267,11 +3261,11 @@
         <v>793</v>
       </c>
       <c r="G12" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Schlecht/Doof", mnemonic = "Daumen runter", tag1 ="Eigenschaften", tag2 ="Teil 1", tag3 ="" where name = "bad";</v>
+        <v>update signs set name_de = "Schlecht/Doof", mnemonic = "Daumen runter", tag1 ="Eigenschaften", tag2 ="Teil 1" where name = "bad";</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -3291,11 +3285,11 @@
         <v>792</v>
       </c>
       <c r="G13" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Tasche", mnemonic = "Taschengriff ergreifen und hochnehmen", tag1 ="Behälter", tag2 ="Teil 2", tag3 ="" where name = "bag";</v>
+        <v>update signs set name_de = "Tasche", mnemonic = "Taschengriff ergreifen und hochnehmen", tag1 ="Behälter", tag2 ="Teil 2" where name = "bag";</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -3318,7 +3312,7 @@
         <v>698</v>
       </c>
       <c r="G14" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -3342,11 +3336,11 @@
         <v>792</v>
       </c>
       <c r="G15" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Ball", mnemonic = "Mit Handflächen Ball umfahren", tag1 ="Spielen", tag2 ="Teil 2", tag3 ="" where name = "ball";</v>
+        <v>update signs set name_de = "Ball", mnemonic = "Mit Handflächen Ball umfahren", tag1 ="Spielen", tag2 ="Teil 2" where name = "ball";</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -3366,11 +3360,11 @@
         <v>793</v>
       </c>
       <c r="G16" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Banane", mnemonic = "Dominante Hand schält", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "banana";</v>
+        <v>update signs set name_de = "Banane", mnemonic = "Dominante Hand schält", tag1 ="Lebensmittel", tag2 ="Teil 1" where name = "banana";</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -3393,7 +3387,7 @@
         <v>698</v>
       </c>
       <c r="G17" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -3417,11 +3411,11 @@
         <v>794</v>
       </c>
       <c r="G18" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Badezimmer", mnemonic = "Erst 'baden' dann 'Zimmer'", tag1 ="Haus", tag2 ="Teil 3", tag3 ="" where name = "bathroom";</v>
+        <v>update signs set name_de = "Badezimmer", mnemonic = "Erst 'baden' dann 'Zimmer'", tag1 ="Haus", tag2 ="Teil 3" where name = "bathroom";</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -3441,11 +3435,11 @@
         <v>793</v>
       </c>
       <c r="G19" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Bett", mnemonic = "Kopf legt sich  schlafen", tag1 ="Haus", tag2 ="Teil 1", tag3 ="" where name = "bed";</v>
+        <v>update signs set name_de = "Bett", mnemonic = "Kopf legt sich  schlafen", tag1 ="Haus", tag2 ="Teil 1" where name = "bed";</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -3468,7 +3462,7 @@
         <v>673</v>
       </c>
       <c r="G20" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -3495,7 +3489,7 @@
         <v>698</v>
       </c>
       <c r="G21" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -3513,7 +3507,7 @@
         <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E22" t="s">
         <v>792</v>
@@ -3522,7 +3516,7 @@
         <v>799</v>
       </c>
       <c r="G22" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -3546,11 +3540,11 @@
         <v>794</v>
       </c>
       <c r="G23" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Groß", mnemonic = "Hände maximal breit auseinander", tag1 ="Eigenschaften", tag2 ="Teil 3", tag3 ="" where name = "big";</v>
+        <v>update signs set name_de = "Groß", mnemonic = "Hände maximal breit auseinander", tag1 ="Eigenschaften", tag2 ="Teil 3" where name = "big";</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -3570,11 +3564,11 @@
         <v>794</v>
       </c>
       <c r="G24" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Fahrrad", mnemonic = "Fäuste fahren", tag1 ="Fahrzeug", tag2 ="Teil 3", tag3 ="" where name = "bike";</v>
+        <v>update signs set name_de = "Fahrrad", mnemonic = "Fäuste fahren", tag1 ="Fahrzeug", tag2 ="Teil 3" where name = "bike";</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -3594,11 +3588,11 @@
         <v>792</v>
       </c>
       <c r="G25" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Vogel", mnemonic = "Schnabel auf und zu", tag1 ="Tier", tag2 ="Teil 2", tag3 ="" where name = "bird";</v>
+        <v>update signs set name_de = "Vogel", mnemonic = "Schnabel auf und zu", tag1 ="Tier", tag2 ="Teil 2" where name = "bird";</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -3618,11 +3612,11 @@
         <v>792</v>
       </c>
       <c r="G26" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Pflanze/blühen", mnemonic = "Pflanze wächst aus Boden/neben Körper", tag1 ="Natur", tag2 ="Teil 2", tag3 ="" where name = "bloom";</v>
+        <v>update signs set name_de = "Pflanze/blühen", mnemonic = "Pflanze wächst aus Boden/neben Körper", tag1 ="Natur", tag2 ="Teil 2" where name = "bloom";</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -3645,7 +3639,7 @@
         <v>677</v>
       </c>
       <c r="G27" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
@@ -3672,7 +3666,7 @@
         <v>804</v>
       </c>
       <c r="G28" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
@@ -3696,11 +3690,11 @@
         <v>792</v>
       </c>
       <c r="G29" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Junge", mnemonic = "2x mit gestreckter Hand grüßen", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "boy";</v>
+        <v>update signs set name_de = "Junge", mnemonic = "2x mit gestreckter Hand grüßen", tag1 ="Person", tag2 ="Teil 2" where name = "boy";</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -3720,11 +3714,11 @@
         <v>792</v>
       </c>
       <c r="G30" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Brot", mnemonic = "Eine Scheibe abschneiden", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "bread";</v>
+        <v>update signs set name_de = "Brot", mnemonic = "Eine Scheibe abschneiden", tag1 ="Lebensmittel", tag2 ="Teil 2" where name = "bread";</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -3744,11 +3738,11 @@
         <v>794</v>
       </c>
       <c r="G31" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Kaputt", mnemonic = "Fäuste zerbrechen etwas", tag1 ="Eigenschaften", tag2 ="Teil 3", tag3 ="" where name = "broken";</v>
+        <v>update signs set name_de = "Kaputt", mnemonic = "Fäuste zerbrechen etwas", tag1 ="Eigenschaften", tag2 ="Teil 3" where name = "broken";</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -3768,11 +3762,11 @@
         <v>794</v>
       </c>
       <c r="G32" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Bürsten/Kämmen", mnemonic = "Faust bürstet über Haare", tag1 ="Körperpflege", tag2 ="Teil 3", tag3 ="" where name = "brush_hair";</v>
+        <v>update signs set name_de = "Bürsten/Kämmen", mnemonic = "Faust bürstet über Haare", tag1 ="Körperpflege", tag2 ="Teil 3" where name = "brush_hair";</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -3792,11 +3786,11 @@
         <v>794</v>
       </c>
       <c r="G33" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Zähne putzen", mnemonic = "Zeigefinger putzt Zähne auf und ab", tag1 ="Körperpflege", tag2 ="Teil 3", tag3 ="" where name = "brush_teeth";</v>
+        <v>update signs set name_de = "Zähne putzen", mnemonic = "Zeigefinger putzt Zähne auf und ab", tag1 ="Körperpflege", tag2 ="Teil 3" where name = "brush_teeth";</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -3816,11 +3810,11 @@
         <v>794</v>
       </c>
       <c r="G34" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Buddha", mnemonic = "O-Hände bewegen sich nach vorn", tag1 ="Religion", tag2 ="Teil 3", tag3 ="" where name = "buddha";</v>
+        <v>update signs set name_de = "Buddha", mnemonic = "O-Hände bewegen sich nach vorn", tag1 ="Religion", tag2 ="Teil 3" where name = "buddha";</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -3840,11 +3834,11 @@
         <v>792</v>
       </c>
       <c r="G35" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Bauen/Bauklötze", mnemonic = "Hände stapeln", tag1 ="Spielen", tag2 ="Teil 2", tag3 ="" where name = "build";</v>
+        <v>update signs set name_de = "Bauen/Bauklötze", mnemonic = "Hände stapeln", tag1 ="Spielen", tag2 ="Teil 2" where name = "build";</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -3864,11 +3858,11 @@
         <v>793</v>
       </c>
       <c r="G36" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Bus", mnemonic = "Buslänge zeigen, diagonal", tag1 ="Fahrzeug", tag2 ="Teil 1", tag3 ="" where name = "bus";</v>
+        <v>update signs set name_de = "Bus", mnemonic = "Buslänge zeigen, diagonal", tag1 ="Fahrzeug", tag2 ="Teil 1" where name = "bus";</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
@@ -3888,11 +3882,11 @@
         <v>794</v>
       </c>
       <c r="G37" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Butter", mnemonic = "Zeigefinger streicht Butter auf Brot", tag1 ="Lebensmittel", tag2 ="Teil 3", tag3 ="" where name = "butter";</v>
+        <v>update signs set name_de = "Butter", mnemonic = "Zeigefinger streicht Butter auf Brot", tag1 ="Lebensmittel", tag2 ="Teil 3" where name = "butter";</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -3912,11 +3906,11 @@
         <v>794</v>
       </c>
       <c r="G38" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Schmetterling", mnemonic = "Hände verhaken und Flügel flattern", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "butterfly";</v>
+        <v>update signs set name_de = "Schmetterling", mnemonic = "Hände verhaken und Flügel flattern", tag1 ="Tier", tag2 ="Teil 3" where name = "butterfly";</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -3939,7 +3933,7 @@
         <v>199</v>
       </c>
       <c r="G39" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="0"/>
@@ -3963,11 +3957,11 @@
         <v>793</v>
       </c>
       <c r="G40" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Bonbon", mnemonic = "Bonbon in Wange", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "candy";</v>
+        <v>update signs set name_de = "Bonbon", mnemonic = "Bonbon in Wange", tag1 ="Lebensmittel", tag2 ="Teil 1" where name = "candy";</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -3987,11 +3981,11 @@
         <v>793</v>
       </c>
       <c r="G41" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Auto", mnemonic = "lenken mimen", tag1 ="Fahrzeug", tag2 ="Teil 1", tag3 ="" where name = "car";</v>
+        <v>update signs set name_de = "Auto", mnemonic = "lenken mimen", tag1 ="Fahrzeug", tag2 ="Teil 1" where name = "car";</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
@@ -4011,11 +4005,11 @@
         <v>794</v>
       </c>
       <c r="G42" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Achtung/Vorsicht", mnemonic = "V-Hände gucken weit zu den Seiten", tag1 ="Interaktion", tag2 ="Teil 3", tag3 ="" where name = "careful";</v>
+        <v>update signs set name_de = "Achtung/Vorsicht", mnemonic = "V-Hände gucken weit zu den Seiten", tag1 ="Interaktion", tag2 ="Teil 3" where name = "careful";</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
@@ -4035,11 +4029,11 @@
         <v>793</v>
       </c>
       <c r="G43" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Möhre", mnemonic = "Schrappen", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "carrot";</v>
+        <v>update signs set name_de = "Möhre", mnemonic = "Schrappen", tag1 ="Lebensmittel", tag2 ="Teil 1" where name = "carrot";</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
@@ -4059,11 +4053,11 @@
         <v>792</v>
       </c>
       <c r="G44" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Katze", mnemonic = "3 Schnurrhaare andeuten", tag1 ="Tier", tag2 ="Teil 2", tag3 ="" where name = "cat";</v>
+        <v>update signs set name_de = "Katze", mnemonic = "3 Schnurrhaare andeuten", tag1 ="Tier", tag2 ="Teil 2" where name = "cat";</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
@@ -4083,11 +4077,11 @@
         <v>793</v>
       </c>
       <c r="G45" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Stuhl", mnemonic = "Gebeugte Finger  als Lehne", tag1 ="Haus", tag2 ="Teil 1", tag3 ="" where name = "chair";</v>
+        <v>update signs set name_de = "Stuhl", mnemonic = "Gebeugte Finger  als Lehne", tag1 ="Haus", tag2 ="Teil 1" where name = "chair";</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
@@ -4107,11 +4101,11 @@
         <v>794</v>
       </c>
       <c r="G46" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Huhn", mnemonic = "Mit Zeigefinger und Daumen picken", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "chicken";</v>
+        <v>update signs set name_de = "Huhn", mnemonic = "Mit Zeigefinger und Daumen picken", tag1 ="Tier", tag2 ="Teil 3" where name = "chicken";</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
@@ -4131,11 +4125,11 @@
         <v>793</v>
       </c>
       <c r="G47" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Kinder", mnemonic = "Köpfe wie Orgelpfeifen zeigen", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "children";</v>
+        <v>update signs set name_de = "Kinder", mnemonic = "Köpfe wie Orgelpfeifen zeigen", tag1 ="Person", tag2 ="Teil 1" where name = "children";</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
@@ -4155,11 +4149,11 @@
         <v>793</v>
       </c>
       <c r="G48" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Schokolade", mnemonic = "Tafel zeigen", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "chocolade";</v>
+        <v>update signs set name_de = "Schokolade", mnemonic = "Tafel zeigen", tag1 ="Lebensmittel", tag2 ="Teil 1" where name = "chocolade";</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
@@ -4179,11 +4173,11 @@
         <v>792</v>
       </c>
       <c r="G49" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Sauber", mnemonic = "Hand sauber wischen", tag1 ="Eigenschaften", tag2 ="Teil 2", tag3 ="" where name = "clean";</v>
+        <v>update signs set name_de = "Sauber", mnemonic = "Hand sauber wischen", tag1 ="Eigenschaften", tag2 ="Teil 2" where name = "clean";</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
@@ -4206,7 +4200,7 @@
         <v>698</v>
       </c>
       <c r="G50" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
@@ -4233,7 +4227,7 @@
         <v>698</v>
       </c>
       <c r="G51" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
@@ -4257,11 +4251,11 @@
         <v>792</v>
       </c>
       <c r="G52" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Kaffee", mnemonic = "Kaffee mahlen", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "coffee";</v>
+        <v>update signs set name_de = "Kaffee", mnemonic = "Kaffee mahlen", tag1 ="Lebensmittel", tag2 ="Teil 2" where name = "coffee";</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
@@ -4281,11 +4275,11 @@
         <v>792</v>
       </c>
       <c r="G53" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Kalt/Frieren", mnemonic = "Vor Kälte zittern", tag1 ="Eigenschaften", tag2 ="Teil 2", tag3 ="" where name = "cold";</v>
+        <v>update signs set name_de = "Kalt/Frieren", mnemonic = "Vor Kälte zittern", tag1 ="Eigenschaften", tag2 ="Teil 2" where name = "cold";</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
@@ -4308,7 +4302,7 @@
         <v>698</v>
       </c>
       <c r="G54" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="0"/>
@@ -4332,11 +4326,11 @@
         <v>793</v>
       </c>
       <c r="G55" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Keks", mnemonic = "Abbeißen", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "cookie";</v>
+        <v>update signs set name_de = "Keks", mnemonic = "Abbeißen", tag1 ="Lebensmittel", tag2 ="Teil 1" where name = "cookie";</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
@@ -4359,7 +4353,7 @@
         <v>698</v>
       </c>
       <c r="G56" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="0"/>
@@ -4383,11 +4377,11 @@
         <v>794</v>
       </c>
       <c r="G57" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Kuh", mnemonic = "Hörner nachahmen", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "cow";</v>
+        <v>update signs set name_de = "Kuh", mnemonic = "Hörner nachahmen", tag1 ="Tier", tag2 ="Teil 3" where name = "cow";</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
@@ -4407,11 +4401,11 @@
         <v>792</v>
       </c>
       <c r="G58" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Gurke", mnemonic = "Gurke nachformen", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "cucumber";</v>
+        <v>update signs set name_de = "Gurke", mnemonic = "Gurke nachformen", tag1 ="Lebensmittel", tag2 ="Teil 2" where name = "cucumber";</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
@@ -4431,11 +4425,11 @@
         <v>792</v>
       </c>
       <c r="G59" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H59" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Schrank", mnemonic = "Mit Handflächen Schrank umreißen", tag1 ="Haus", tag2 ="Teil 2", tag3 ="" where name = "cupboard";</v>
+        <v>update signs set name_de = "Schrank", mnemonic = "Mit Handflächen Schrank umreißen", tag1 ="Haus", tag2 ="Teil 2" where name = "cupboard";</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.35">
@@ -4455,11 +4449,11 @@
         <v>794</v>
       </c>
       <c r="G60" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Hörgerät", mnemonic = "Hörgerät hinter Ohr mimen", tag1 ="Behinderung", tag2 ="Teil 3", tag3 ="" where name = "deaf_aid";</v>
+        <v>update signs set name_de = "Hörgerät", mnemonic = "Hörgerät hinter Ohr mimen", tag1 ="Behinderung", tag2 ="Teil 3" where name = "deaf_aid";</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
@@ -4479,11 +4473,11 @@
         <v>794</v>
       </c>
       <c r="G61" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H61" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Windel", mnemonic = "Handflächen kletten Windel zu", tag1 ="Körperpflege", tag2 ="Teil 3", tag3 ="" where name = "diaper";</v>
+        <v>update signs set name_de = "Windel", mnemonic = "Handflächen kletten Windel zu", tag1 ="Körperpflege", tag2 ="Teil 3" where name = "diaper";</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
@@ -4506,7 +4500,7 @@
         <v>677</v>
       </c>
       <c r="G62" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="0"/>
@@ -4530,11 +4524,11 @@
         <v>792</v>
       </c>
       <c r="G63" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H63" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Arzt/Doktor", mnemonic = "Auf Handrücken pieksen", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "doctor";</v>
+        <v>update signs set name_de = "Arzt/Doktor", mnemonic = "Auf Handrücken pieksen", tag1 ="Person", tag2 ="Teil 2" where name = "doctor";</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
@@ -4554,11 +4548,11 @@
         <v>792</v>
       </c>
       <c r="G64" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Hund", mnemonic = "Hund zu sich 'heranklopfen'", tag1 ="Tier", tag2 ="Teil 2", tag3 ="" where name = "dog";</v>
+        <v>update signs set name_de = "Hund", mnemonic = "Hund zu sich 'heranklopfen'", tag1 ="Tier", tag2 ="Teil 2" where name = "dog";</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
@@ -4578,11 +4572,11 @@
         <v>793</v>
       </c>
       <c r="G65" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H65" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Puppe", mnemonic = "Baby still auf Arm halten", tag1 ="Spielen", tag2 ="Teil 1", tag3 ="" where name = "doll";</v>
+        <v>update signs set name_de = "Puppe", mnemonic = "Baby still auf Arm halten", tag1 ="Spielen", tag2 ="Teil 1" where name = "doll";</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
@@ -4602,14 +4596,14 @@
         <v>793</v>
       </c>
       <c r="F66" t="s">
-        <v>806</v>
+        <v>819</v>
       </c>
       <c r="G66" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H66" t="str">
         <f t="shared" si="0"/>
-        <v>update signs set name_de = "Fertig", mnemonic = "Handkante auf Handfläche 'schlagen'", tag1 ="Eigenschaften", tag2 ="Teil 1", tag3 ="kleine _Worte" where name = "done";</v>
+        <v>update signs set name_de = "Fertig", mnemonic = "Handkante auf Handfläche 'schlagen'", tag1 ="Eigenschaften", tag2 ="Teil 1", tag3 ="Kleine Worte" where name = "done";</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
@@ -4629,11 +4623,11 @@
         <v>792</v>
       </c>
       <c r="G67" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H67" t="str">
-        <f t="shared" ref="H67:H130" si="1">"update signs set name_de = """&amp;B67&amp;""", mnemonic = """&amp;C67&amp;""", tag1 ="""&amp;D67&amp;""", tag2 ="""&amp;E67&amp;""", tag3 ="""&amp;F67&amp;""" where name = """&amp;A67&amp;""";"</f>
-        <v>update signs set name_de = "Tür/Tor", mnemonic = "Mit gestreckter Hand 'Türöffnen' zeigen", tag1 ="Haus", tag2 ="Teil 2", tag3 ="" where name = "door";</v>
+        <f t="shared" ref="H67:H130" si="1">IF(NOT(ISBLANK(F67)),"update signs set name_de = """&amp;B67&amp;""", mnemonic = """&amp;C67&amp;""", tag1 ="""&amp;D67&amp;""", tag2 ="""&amp;E67&amp;""", tag3 ="""&amp;F67&amp;""" where name = """&amp;A67&amp;""";","update signs set name_de = """&amp;B67&amp;""", mnemonic = """&amp;C67&amp;""", tag1 ="""&amp;D67&amp;""", tag2 ="""&amp;E67&amp;""" where name = """&amp;A67&amp;""";")</f>
+        <v>update signs set name_de = "Tür/Tor", mnemonic = "Mit gestreckter Hand 'Türöffnen' zeigen", tag1 ="Haus", tag2 ="Teil 2" where name = "door";</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
@@ -4647,7 +4641,7 @@
         <v>197</v>
       </c>
       <c r="D68" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E68" t="s">
         <v>794</v>
@@ -4656,7 +4650,7 @@
         <v>677</v>
       </c>
       <c r="G68" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H68" t="str">
         <f t="shared" si="1"/>
@@ -4683,7 +4677,7 @@
         <v>199</v>
       </c>
       <c r="G69" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H69" t="str">
         <f t="shared" si="1"/>
@@ -4710,7 +4704,7 @@
         <v>698</v>
       </c>
       <c r="G70" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H70" t="str">
         <f t="shared" si="1"/>
@@ -4728,17 +4722,17 @@
         <v>206</v>
       </c>
       <c r="D71" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E71" t="s">
         <v>794</v>
       </c>
       <c r="G71" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H71" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Tropfen", mnemonic = "Zeigefinger tropft (tippen)", tag1 ="Krankheit", tag2 ="Teil 3", tag3 ="" where name = "drop";</v>
+        <v>update signs set name_de = "Tropfen", mnemonic = "Zeigefinger tropft (tippen)", tag1 ="Krankheit", tag2 ="Teil 3" where name = "drop";</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.35">
@@ -4761,7 +4755,7 @@
         <v>698</v>
       </c>
       <c r="G72" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H72" t="str">
         <f t="shared" si="1"/>
@@ -4785,11 +4779,11 @@
         <v>794</v>
       </c>
       <c r="G73" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H73" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Ei", mnemonic = "Eigröße zeigen", tag1 ="Lebensmittel", tag2 ="Teil 3", tag3 ="" where name = "egg";</v>
+        <v>update signs set name_de = "Ei", mnemonic = "Eigröße zeigen", tag1 ="Lebensmittel", tag2 ="Teil 3" where name = "egg";</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
@@ -4803,7 +4797,7 @@
         <v>215</v>
       </c>
       <c r="D74" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E74" t="s">
         <v>794</v>
@@ -4812,7 +4806,7 @@
         <v>677</v>
       </c>
       <c r="G74" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H74" t="str">
         <f t="shared" si="1"/>
@@ -4839,7 +4833,7 @@
         <v>698</v>
       </c>
       <c r="G75" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H75" t="str">
         <f t="shared" si="1"/>
@@ -4857,7 +4851,7 @@
         <v>221</v>
       </c>
       <c r="D76" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E76" t="s">
         <v>792</v>
@@ -4866,7 +4860,7 @@
         <v>673</v>
       </c>
       <c r="G76" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H76" t="str">
         <f t="shared" si="1"/>
@@ -4890,11 +4884,11 @@
         <v>794</v>
       </c>
       <c r="G77" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H77" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Fisch", mnemonic = "Hand schlängelt sich durch's Wasser", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "fish";</v>
+        <v>update signs set name_de = "Fisch", mnemonic = "Hand schlängelt sich durch's Wasser", tag1 ="Tier", tag2 ="Teil 3" where name = "fish";</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.35">
@@ -4908,16 +4902,16 @@
         <v>227</v>
       </c>
       <c r="D78" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E78" t="s">
         <v>792</v>
       </c>
       <c r="F78" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="G78" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H78" t="str">
         <f t="shared" si="1"/>
@@ -4944,7 +4938,7 @@
         <v>677</v>
       </c>
       <c r="G79" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H79" t="str">
         <f t="shared" si="1"/>
@@ -4956,7 +4950,7 @@
         <v>231</v>
       </c>
       <c r="B80" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="C80" t="s">
         <v>232</v>
@@ -4971,7 +4965,7 @@
         <v>698</v>
       </c>
       <c r="G80" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H80" t="str">
         <f t="shared" si="1"/>
@@ -4995,11 +4989,11 @@
         <v>792</v>
       </c>
       <c r="G81" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H81" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Gabel", mnemonic = "Gabel piekt in Handfläche", tag1 ="Ernährung", tag2 ="Teil 2", tag3 ="" where name = "fork";</v>
+        <v>update signs set name_de = "Gabel", mnemonic = "Gabel piekt in Handfläche", tag1 ="Ernährung", tag2 ="Teil 2" where name = "fork";</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.35">
@@ -5019,11 +5013,11 @@
         <v>793</v>
       </c>
       <c r="G82" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H82" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Freund/In", mnemonic = "2x Hände schütteln", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "friend";</v>
+        <v>update signs set name_de = "Freund/In", mnemonic = "2x Hände schütteln", tag1 ="Person", tag2 ="Teil 1" where name = "friend";</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.35">
@@ -5037,7 +5031,7 @@
         <v>241</v>
       </c>
       <c r="D83" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E83" t="s">
         <v>794</v>
@@ -5046,7 +5040,7 @@
         <v>677</v>
       </c>
       <c r="G83" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H83" t="str">
         <f t="shared" si="1"/>
@@ -5073,7 +5067,7 @@
         <v>714</v>
       </c>
       <c r="G84" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H84" t="str">
         <f t="shared" si="1"/>
@@ -5097,11 +5091,11 @@
         <v>792</v>
       </c>
       <c r="G85" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H85" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Mädchen", mnemonic = "Mit Daumen 2x Trägerkleid andeuten", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "girl";</v>
+        <v>update signs set name_de = "Mädchen", mnemonic = "Mit Daumen 2x Trägerkleid andeuten", tag1 ="Person", tag2 ="Teil 2" where name = "girl";</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.35">
@@ -5124,7 +5118,7 @@
         <v>698</v>
       </c>
       <c r="G86" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H86" t="str">
         <f t="shared" si="1"/>
@@ -5148,11 +5142,11 @@
         <v>794</v>
       </c>
       <c r="G87" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H87" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Brille", mnemonic = "Zeigefinger und Daumen formen Brille", tag1 ="Behinderung", tag2 ="Teil 3", tag3 ="" where name = "glasses";</v>
+        <v>update signs set name_de = "Brille", mnemonic = "Zeigefinger und Daumen formen Brille", tag1 ="Behinderung", tag2 ="Teil 3" where name = "glasses";</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.35">
@@ -5160,13 +5154,13 @@
         <v>254</v>
       </c>
       <c r="B88" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C88" t="s">
         <v>255</v>
       </c>
       <c r="D88" t="s">
-        <v>811</v>
+        <v>819</v>
       </c>
       <c r="E88" t="s">
         <v>793</v>
@@ -5175,11 +5169,11 @@
         <v>677</v>
       </c>
       <c r="G88" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H88" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "weg!", mnemonic = "Wegwerf-Bewegung", tag1 ="kleine Wörter", tag2 ="Teil 1", tag3 ="Eigenschaften" where name = "go_away";</v>
+        <v>update signs set name_de = "weg!", mnemonic = "Wegwerf-Bewegung", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="Eigenschaften" where name = "go_away";</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.35">
@@ -5187,7 +5181,7 @@
         <v>256</v>
       </c>
       <c r="B89" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="C89" t="s">
         <v>257</v>
@@ -5199,11 +5193,11 @@
         <v>793</v>
       </c>
       <c r="G89" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H89" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Geh da hin", mnemonic = "Richtung zeigen", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="" where name = "go_there";</v>
+        <v>update signs set name_de = "Geh da hin", mnemonic = "Richtung zeigen", tag1 ="Interaktion", tag2 ="Teil 1" where name = "go_there";</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.35">
@@ -5223,11 +5217,11 @@
         <v>794</v>
       </c>
       <c r="G90" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H90" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Gott", mnemonic = "Dreieinigkeit fährt in den Himmel", tag1 ="Religion", tag2 ="Teil 3", tag3 ="" where name = "god";</v>
+        <v>update signs set name_de = "Gott", mnemonic = "Dreieinigkeit fährt in den Himmel", tag1 ="Religion", tag2 ="Teil 3" where name = "god";</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.35">
@@ -5241,7 +5235,7 @@
         <v>263</v>
       </c>
       <c r="D91" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E91" t="s">
         <v>793</v>
@@ -5250,7 +5244,7 @@
         <v>677</v>
       </c>
       <c r="G91" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H91" t="str">
         <f t="shared" si="1"/>
@@ -5274,11 +5268,11 @@
         <v>792</v>
       </c>
       <c r="G92" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H92" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Oma", mnemonic = "Dutt andeuten", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "grandma";</v>
+        <v>update signs set name_de = "Oma", mnemonic = "Dutt andeuten", tag1 ="Person", tag2 ="Teil 2" where name = "grandma";</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.35">
@@ -5298,11 +5292,11 @@
         <v>792</v>
       </c>
       <c r="G93" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H93" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Opa", mnemonic = "Zwirbelbart andeuten", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "grandpa";</v>
+        <v>update signs set name_de = "Opa", mnemonic = "Zwirbelbart andeuten", tag1 ="Person", tag2 ="Teil 2" where name = "grandpa";</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.35">
@@ -5325,7 +5319,7 @@
         <v>677</v>
       </c>
       <c r="G94" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H94" t="str">
         <f t="shared" si="1"/>
@@ -5349,10 +5343,10 @@
         <v>793</v>
       </c>
       <c r="F95" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="G95" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H95" t="str">
         <f t="shared" si="1"/>
@@ -5379,7 +5373,7 @@
         <v>698</v>
       </c>
       <c r="G96" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H96" t="str">
         <f t="shared" si="1"/>
@@ -5397,17 +5391,17 @@
         <v>281</v>
       </c>
       <c r="D97" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E97" t="s">
         <v>793</v>
       </c>
       <c r="G97" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H97" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Hier", mnemonic = "Punkt zeigen", tag1 ="Kleine Worte", tag2 ="Teil 1", tag3 ="" where name = "here";</v>
+        <v>update signs set name_de = "Hier", mnemonic = "Punkt zeigen", tag1 ="Kleine Worte", tag2 ="Teil 1" where name = "here";</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.35">
@@ -5427,11 +5421,11 @@
         <v>794</v>
       </c>
       <c r="G98" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H98" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Pferd", mnemonic = "Mit Zügeln reiten", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "horse";</v>
+        <v>update signs set name_de = "Pferd", mnemonic = "Mit Zügeln reiten", tag1 ="Tier", tag2 ="Teil 3" where name = "horse";</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.35">
@@ -5445,7 +5439,7 @@
         <v>287</v>
       </c>
       <c r="D99" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E99" t="s">
         <v>792</v>
@@ -5454,7 +5448,7 @@
         <v>677</v>
       </c>
       <c r="G99" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H99" t="str">
         <f t="shared" si="1"/>
@@ -5478,11 +5472,11 @@
         <v>793</v>
       </c>
       <c r="G100" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H100" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Haus", mnemonic = "Dach andeuten", tag1 ="Haus", tag2 ="Teil 1", tag3 ="" where name = "house";</v>
+        <v>update signs set name_de = "Haus", mnemonic = "Dach andeuten", tag1 ="Haus", tag2 ="Teil 1" where name = "house";</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.35">
@@ -5502,11 +5496,11 @@
         <v>793</v>
       </c>
       <c r="G101" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H101" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Ich", mnemonic = "Mit Zeigefinger auf sich zeigen", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "i";</v>
+        <v>update signs set name_de = "Ich", mnemonic = "Mit Zeigefinger auf sich zeigen", tag1 ="Person", tag2 ="Teil 1" where name = "i";</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.35">
@@ -5526,11 +5520,11 @@
         <v>792</v>
       </c>
       <c r="G102" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H102" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Eis", mnemonic = "Eis lecken", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "ice";</v>
+        <v>update signs set name_de = "Eis", mnemonic = "Eis lecken", tag1 ="Lebensmittel", tag2 ="Teil 2" where name = "ice";</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.35">
@@ -5544,7 +5538,7 @@
         <v>299</v>
       </c>
       <c r="D103" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E103" t="s">
         <v>792</v>
@@ -5553,7 +5547,7 @@
         <v>799</v>
       </c>
       <c r="G103" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H103" t="str">
         <f t="shared" si="1"/>
@@ -5580,7 +5574,7 @@
         <v>686</v>
       </c>
       <c r="G104" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H104" t="str">
         <f t="shared" si="1"/>
@@ -5607,7 +5601,7 @@
         <v>199</v>
       </c>
       <c r="G105" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H105" t="str">
         <f t="shared" si="1"/>
@@ -5634,7 +5628,7 @@
         <v>698</v>
       </c>
       <c r="G106" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H106" t="str">
         <f t="shared" si="1"/>
@@ -5661,7 +5655,7 @@
         <v>408</v>
       </c>
       <c r="G107" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H107" t="str">
         <f t="shared" si="1"/>
@@ -5685,11 +5679,11 @@
         <v>794</v>
       </c>
       <c r="G108" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H108" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Küche", mnemonic = "Erst 'kochen' dann 'Zimmer'", tag1 ="Haus", tag2 ="Teil 3", tag3 ="" where name = "kitchen";</v>
+        <v>update signs set name_de = "Küche", mnemonic = "Erst 'kochen' dann 'Zimmer'", tag1 ="Haus", tag2 ="Teil 3" where name = "kitchen";</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.35">
@@ -5712,7 +5706,7 @@
         <v>698</v>
       </c>
       <c r="G109" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H109" t="str">
         <f t="shared" si="1"/>
@@ -5736,11 +5730,11 @@
         <v>792</v>
       </c>
       <c r="G110" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H110" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Licht/Lampe", mnemonic = "Strahlende Lampe seitlich oben neben Kopf", tag1 ="Haus", tag2 ="Teil 2", tag3 ="" where name = "lamp";</v>
+        <v>update signs set name_de = "Licht/Lampe", mnemonic = "Strahlende Lampe seitlich oben neben Kopf", tag1 ="Haus", tag2 ="Teil 2" where name = "lamp";</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.35">
@@ -5754,7 +5748,7 @@
         <v>323</v>
       </c>
       <c r="D111" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E111" t="s">
         <v>792</v>
@@ -5763,7 +5757,7 @@
         <v>673</v>
       </c>
       <c r="G111" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H111" t="str">
         <f t="shared" si="1"/>
@@ -5790,7 +5784,7 @@
         <v>698</v>
       </c>
       <c r="G112" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H112" t="str">
         <f t="shared" si="1"/>
@@ -5817,7 +5811,7 @@
         <v>698</v>
       </c>
       <c r="G113" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H113" t="str">
         <f t="shared" si="1"/>
@@ -5844,7 +5838,7 @@
         <v>698</v>
       </c>
       <c r="G114" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H114" t="str">
         <f t="shared" si="1"/>
@@ -5868,11 +5862,11 @@
         <v>793</v>
       </c>
       <c r="G115" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H115" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Mama", mnemonic = "Wange kreisend streicheln", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "mama";</v>
+        <v>update signs set name_de = "Mama", mnemonic = "Wange kreisend streicheln", tag1 ="Person", tag2 ="Teil 1" where name = "mama";</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.35">
@@ -5892,11 +5886,11 @@
         <v>792</v>
       </c>
       <c r="G116" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H116" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Mann", mnemonic = "Hut an Krempe fassen", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "man";</v>
+        <v>update signs set name_de = "Mann", mnemonic = "Hut an Krempe fassen", tag1 ="Person", tag2 ="Teil 2" where name = "man";</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.35">
@@ -5910,16 +5904,16 @@
         <v>341</v>
       </c>
       <c r="D117" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E117" t="s">
         <v>794</v>
       </c>
       <c r="F117" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="G117" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H117" t="str">
         <f t="shared" si="1"/>
@@ -5943,11 +5937,11 @@
         <v>794</v>
       </c>
       <c r="G118" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H118" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Marmelade", mnemonic = "Hand streicht flächig auf Brotscheibe", tag1 ="Lebensmittel", tag2 ="Teil 3", tag3 ="" where name = "marmelade";</v>
+        <v>update signs set name_de = "Marmelade", mnemonic = "Hand streicht flächig auf Brotscheibe", tag1 ="Lebensmittel", tag2 ="Teil 3" where name = "marmelade";</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.35">
@@ -5970,7 +5964,7 @@
         <v>199</v>
       </c>
       <c r="G119" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H119" t="str">
         <f t="shared" si="1"/>
@@ -5988,16 +5982,16 @@
         <v>350</v>
       </c>
       <c r="D120" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E120" t="s">
         <v>794</v>
       </c>
       <c r="F120" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="G120" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H120" t="str">
         <f t="shared" si="1"/>
@@ -6021,11 +6015,11 @@
         <v>794</v>
       </c>
       <c r="G121" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H121" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Motorrad/Mofa", mnemonic = "An Lenker gibt eine Faust Gas", tag1 ="Fahrzeug", tag2 ="Teil 3", tag3 ="" where name = "motorcycle";</v>
+        <v>update signs set name_de = "Motorrad/Mofa", mnemonic = "An Lenker gibt eine Faust Gas", tag1 ="Fahrzeug", tag2 ="Teil 3" where name = "motorcycle";</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.35">
@@ -6048,7 +6042,7 @@
         <v>698</v>
       </c>
       <c r="G122" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H122" t="str">
         <f t="shared" si="1"/>
@@ -6066,7 +6060,7 @@
         <v>359</v>
       </c>
       <c r="D123" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E123" t="s">
         <v>793</v>
@@ -6075,7 +6069,7 @@
         <v>683</v>
       </c>
       <c r="G123" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H123" t="str">
         <f t="shared" si="1"/>
@@ -6099,11 +6093,11 @@
         <v>794</v>
       </c>
       <c r="G124" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H124" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Nudeln", mnemonic = "Spaghetti aufwickeln", tag1 ="Lebensmittel", tag2 ="Teil 3", tag3 ="" where name = "noodles";</v>
+        <v>update signs set name_de = "Nudeln", mnemonic = "Spaghetti aufwickeln", tag1 ="Lebensmittel", tag2 ="Teil 3" where name = "noodles";</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.35">
@@ -6117,7 +6111,7 @@
         <v>365</v>
       </c>
       <c r="D125" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E125" t="s">
         <v>792</v>
@@ -6126,7 +6120,7 @@
         <v>673</v>
       </c>
       <c r="G125" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H125" t="str">
         <f t="shared" si="1"/>
@@ -6144,7 +6138,7 @@
         <v>368</v>
       </c>
       <c r="D126" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E126" t="s">
         <v>792</v>
@@ -6153,7 +6147,7 @@
         <v>799</v>
       </c>
       <c r="G126" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H126" t="str">
         <f t="shared" si="1"/>
@@ -6171,16 +6165,16 @@
         <v>371</v>
       </c>
       <c r="D127" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E127" t="s">
         <v>793</v>
       </c>
       <c r="F127" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="G127" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H127" t="str">
         <f t="shared" si="1"/>
@@ -6204,11 +6198,11 @@
         <v>793</v>
       </c>
       <c r="G128" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H128" t="str">
         <f t="shared" si="1"/>
-        <v>update signs set name_de = "Orange", mnemonic = "Schalen zeigen und herausbrechen", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="" where name = "orange";</v>
+        <v>update signs set name_de = "Orange", mnemonic = "Schalen zeigen und herausbrechen", tag1 ="Lebensmittel", tag2 ="Teil 1" where name = "orange";</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.35">
@@ -6228,10 +6222,10 @@
         <v>792</v>
       </c>
       <c r="F129" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="G129" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H129" t="str">
         <f t="shared" si="1"/>
@@ -6243,13 +6237,13 @@
         <v>378</v>
       </c>
       <c r="B130" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="C130" t="s">
         <v>379</v>
       </c>
       <c r="D130" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E130" t="s">
         <v>794</v>
@@ -6258,7 +6252,7 @@
         <v>698</v>
       </c>
       <c r="G130" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H130" t="str">
         <f t="shared" si="1"/>
@@ -6276,17 +6270,17 @@
         <v>382</v>
       </c>
       <c r="D131" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E131" t="s">
         <v>794</v>
       </c>
       <c r="G131" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H131" t="str">
-        <f t="shared" ref="H131:H194" si="2">"update signs set name_de = """&amp;B131&amp;""", mnemonic = """&amp;C131&amp;""", tag1 ="""&amp;D131&amp;""", tag2 ="""&amp;E131&amp;""", tag3 ="""&amp;F131&amp;""" where name = """&amp;A131&amp;""";"</f>
-        <v>update signs set name_de = "Schmerzen", mnemonic = "Handfläche vibriert vor Schmerzstelle", tag1 ="Krankheit", tag2 ="Teil 3", tag3 ="" where name = "pain";</v>
+        <f t="shared" ref="H131:H194" si="2">IF(NOT(ISBLANK(F131)),"update signs set name_de = """&amp;B131&amp;""", mnemonic = """&amp;C131&amp;""", tag1 ="""&amp;D131&amp;""", tag2 ="""&amp;E131&amp;""", tag3 ="""&amp;F131&amp;""" where name = """&amp;A131&amp;""";","update signs set name_de = """&amp;B131&amp;""", mnemonic = """&amp;C131&amp;""", tag1 ="""&amp;D131&amp;""", tag2 ="""&amp;E131&amp;""" where name = """&amp;A131&amp;""";")</f>
+        <v>update signs set name_de = "Schmerzen", mnemonic = "Handfläche vibriert vor Schmerzstelle", tag1 ="Krankheit", tag2 ="Teil 3" where name = "pain";</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.35">
@@ -6309,7 +6303,7 @@
         <v>698</v>
       </c>
       <c r="G132" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H132" t="str">
         <f t="shared" si="2"/>
@@ -6333,11 +6327,11 @@
         <v>793</v>
       </c>
       <c r="G133" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H133" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Papa", mnemonic = "Schnauzbart andeuten", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "papa";</v>
+        <v>update signs set name_de = "Papa", mnemonic = "Schnauzbart andeuten", tag1 ="Person", tag2 ="Teil 1" where name = "papa";</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.35">
@@ -6360,7 +6354,7 @@
         <v>714</v>
       </c>
       <c r="G134" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H134" t="str">
         <f t="shared" si="2"/>
@@ -6387,7 +6381,7 @@
         <v>289</v>
       </c>
       <c r="G135" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H135" t="str">
         <f t="shared" si="2"/>
@@ -6411,11 +6405,11 @@
         <v>794</v>
       </c>
       <c r="G136" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H136" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Schwein", mnemonic = "Schnauze nach vorn ziehen", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "pig";</v>
+        <v>update signs set name_de = "Schwein", mnemonic = "Schnauze nach vorn ziehen", tag1 ="Tier", tag2 ="Teil 3" where name = "pig";</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.35">
@@ -6429,17 +6423,17 @@
         <v>400</v>
       </c>
       <c r="D137" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E137" t="s">
         <v>794</v>
       </c>
       <c r="G137" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H137" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Tablette", mnemonic = "Tablette auf Handfläche malen", tag1 ="Krankheit", tag2 ="Teil 3", tag3 ="" where name = "pill";</v>
+        <v>update signs set name_de = "Tablette", mnemonic = "Tablette auf Handfläche malen", tag1 ="Krankheit", tag2 ="Teil 3" where name = "pill";</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.35">
@@ -6462,7 +6456,7 @@
         <v>677</v>
       </c>
       <c r="G138" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H138" t="str">
         <f t="shared" si="2"/>
@@ -6486,10 +6480,10 @@
         <v>792</v>
       </c>
       <c r="F139" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="G139" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H139" t="str">
         <f t="shared" si="2"/>
@@ -6516,7 +6510,7 @@
         <v>698</v>
       </c>
       <c r="G140" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H140" t="str">
         <f t="shared" si="2"/>
@@ -6540,10 +6534,10 @@
         <v>793</v>
       </c>
       <c r="F141" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="G141" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H141" t="str">
         <f t="shared" si="2"/>
@@ -6561,7 +6555,7 @@
         <v>415</v>
       </c>
       <c r="D142" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E142" t="s">
         <v>794</v>
@@ -6570,7 +6564,7 @@
         <v>698</v>
       </c>
       <c r="G142" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H142" t="str">
         <f t="shared" si="2"/>
@@ -6594,11 +6588,11 @@
         <v>794</v>
       </c>
       <c r="G143" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H143" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Hase", mnemonic = "Zeige-und Mittelfinger zeigen Ohren", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "rabbit";</v>
+        <v>update signs set name_de = "Hase", mnemonic = "Zeige-und Mittelfinger zeigen Ohren", tag1 ="Tier", tag2 ="Teil 3" where name = "rabbit";</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.35">
@@ -6621,7 +6615,7 @@
         <v>698</v>
       </c>
       <c r="G144" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H144" t="str">
         <f t="shared" si="2"/>
@@ -6648,7 +6642,7 @@
         <v>677</v>
       </c>
       <c r="G145" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H145" t="str">
         <f t="shared" si="2"/>
@@ -6672,11 +6666,11 @@
         <v>792</v>
       </c>
       <c r="G146" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H146" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Brötchen", mnemonic = "2x Brötchen formen", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "roll";</v>
+        <v>update signs set name_de = "Brötchen", mnemonic = "2x Brötchen formen", tag1 ="Lebensmittel", tag2 ="Teil 2" where name = "roll";</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.35">
@@ -6696,11 +6690,11 @@
         <v>794</v>
       </c>
       <c r="G147" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H147" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Zimmer", mnemonic = "Zeigefinger ziehen Mauer um Zimmer", tag1 ="Haus", tag2 ="Teil 3", tag3 ="" where name = "room";</v>
+        <v>update signs set name_de = "Zimmer", mnemonic = "Zeigefinger ziehen Mauer um Zimmer", tag1 ="Haus", tag2 ="Teil 3" where name = "room";</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.35">
@@ -6723,7 +6717,7 @@
         <v>698</v>
       </c>
       <c r="G148" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H148" t="str">
         <f t="shared" si="2"/>
@@ -6747,11 +6741,11 @@
         <v>794</v>
       </c>
       <c r="G149" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H149" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Salz", mnemonic = "Prise", tag1 ="Lebensmittel", tag2 ="Teil 3", tag3 ="" where name = "salt";</v>
+        <v>update signs set name_de = "Salz", mnemonic = "Prise", tag1 ="Lebensmittel", tag2 ="Teil 3" where name = "salt";</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.35">
@@ -6771,11 +6765,11 @@
         <v>792</v>
       </c>
       <c r="G150" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H150" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Sand", mnemonic = "Sand aufnehmen und rieseln", tag1 ="Spielen", tag2 ="Teil 2", tag3 ="" where name = "sand";</v>
+        <v>update signs set name_de = "Sand", mnemonic = "Sand aufnehmen und rieseln", tag1 ="Spielen", tag2 ="Teil 2" where name = "sand";</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.35">
@@ -6798,7 +6792,7 @@
         <v>289</v>
       </c>
       <c r="G151" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H151" t="str">
         <f t="shared" si="2"/>
@@ -6825,7 +6819,7 @@
         <v>689</v>
       </c>
       <c r="G152" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H152" t="str">
         <f t="shared" si="2"/>
@@ -6852,7 +6846,7 @@
         <v>698</v>
       </c>
       <c r="G153" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H153" t="str">
         <f t="shared" si="2"/>
@@ -6879,7 +6873,7 @@
         <v>698</v>
       </c>
       <c r="G154" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H154" t="str">
         <f t="shared" si="2"/>
@@ -6903,11 +6897,11 @@
         <v>794</v>
       </c>
       <c r="G155" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H155" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Schaf", mnemonic = "Wolle am Bauch zeigen", tag1 ="Tier", tag2 ="Teil 3", tag3 ="" where name = "sheep";</v>
+        <v>update signs set name_de = "Schaf", mnemonic = "Wolle am Bauch zeigen", tag1 ="Tier", tag2 ="Teil 3" where name = "sheep";</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.35">
@@ -6927,11 +6921,11 @@
         <v>794</v>
       </c>
       <c r="G156" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H156" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Schiff/Boot", mnemonic = "Mit Handflächen Bug nach vorn fahren", tag1 ="Fahrzeug", tag2 ="Teil 3", tag3 ="" where name = "ship";</v>
+        <v>update signs set name_de = "Schiff/Boot", mnemonic = "Mit Handflächen Bug nach vorn fahren", tag1 ="Fahrzeug", tag2 ="Teil 3" where name = "ship";</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.35">
@@ -6954,7 +6948,7 @@
         <v>698</v>
       </c>
       <c r="G157" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H157" t="str">
         <f t="shared" si="2"/>
@@ -6978,11 +6972,11 @@
         <v>793</v>
       </c>
       <c r="G158" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H158" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Bruder/Schwester", mnemonic = "Gestreckte Zeigefinger aneinander führen", tag1 ="Person", tag2 ="Teil 1", tag3 ="" where name = "sibling";</v>
+        <v>update signs set name_de = "Bruder/Schwester", mnemonic = "Gestreckte Zeigefinger aneinander führen", tag1 ="Person", tag2 ="Teil 1" where name = "sibling";</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.35">
@@ -6996,7 +6990,7 @@
         <v>466</v>
       </c>
       <c r="D159" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E159" t="s">
         <v>794</v>
@@ -7005,7 +6999,7 @@
         <v>677</v>
       </c>
       <c r="G159" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H159" t="str">
         <f t="shared" si="2"/>
@@ -7032,7 +7026,7 @@
         <v>798</v>
       </c>
       <c r="G160" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H160" t="str">
         <f t="shared" si="2"/>
@@ -7059,7 +7053,7 @@
         <v>698</v>
       </c>
       <c r="G161" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H161" t="str">
         <f t="shared" si="2"/>
@@ -7077,7 +7071,7 @@
         <v>475</v>
       </c>
       <c r="D162" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E162" t="s">
         <v>794</v>
@@ -7086,7 +7080,7 @@
         <v>677</v>
       </c>
       <c r="G162" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H162" t="str">
         <f t="shared" si="2"/>
@@ -7098,7 +7092,7 @@
         <v>476</v>
       </c>
       <c r="B163" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="C163" t="s">
         <v>477</v>
@@ -7110,10 +7104,10 @@
         <v>793</v>
       </c>
       <c r="F163" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="G163" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H163" t="str">
         <f t="shared" si="2"/>
@@ -7137,10 +7131,10 @@
         <v>792</v>
       </c>
       <c r="F164" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="G164" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H164" t="str">
         <f t="shared" si="2"/>
@@ -7167,7 +7161,7 @@
         <v>698</v>
       </c>
       <c r="G165" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H165" t="str">
         <f t="shared" si="2"/>
@@ -7194,7 +7188,7 @@
         <v>698</v>
       </c>
       <c r="G166" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H166" t="str">
         <f t="shared" si="2"/>
@@ -7218,10 +7212,10 @@
         <v>793</v>
       </c>
       <c r="F167" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="G167" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H167" t="str">
         <f t="shared" si="2"/>
@@ -7245,11 +7239,11 @@
         <v>794</v>
       </c>
       <c r="G168" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H168" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Zucker", mnemonic = "Erst 'süß' zeigen, dann mit Fingern streuen", tag1 ="Lebensmittel", tag2 ="Teil 3", tag3 ="" where name = "sugar";</v>
+        <v>update signs set name_de = "Zucker", mnemonic = "Erst 'süß' zeigen, dann mit Fingern streuen", tag1 ="Lebensmittel", tag2 ="Teil 3" where name = "sugar";</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.35">
@@ -7272,7 +7266,7 @@
         <v>698</v>
       </c>
       <c r="G169" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H169" t="str">
         <f t="shared" si="2"/>
@@ -7284,7 +7278,7 @@
         <v>496</v>
       </c>
       <c r="B170" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="C170" t="s">
         <v>497</v>
@@ -7299,7 +7293,7 @@
         <v>698</v>
       </c>
       <c r="G170" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H170" t="str">
         <f t="shared" si="2"/>
@@ -7311,7 +7305,7 @@
         <v>498</v>
       </c>
       <c r="B171" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="C171" t="s">
         <v>499</v>
@@ -7326,7 +7320,7 @@
         <v>698</v>
       </c>
       <c r="G171" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H171" t="str">
         <f t="shared" si="2"/>
@@ -7350,11 +7344,11 @@
         <v>793</v>
       </c>
       <c r="G172" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H172" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Tisch", mnemonic = "Tischfläche von innen nach außen streichen", tag1 ="Haus", tag2 ="Teil 1", tag3 ="" where name = "table";</v>
+        <v>update signs set name_de = "Tisch", mnemonic = "Tischfläche von innen nach außen streichen", tag1 ="Haus", tag2 ="Teil 1" where name = "table";</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.35">
@@ -7377,7 +7371,7 @@
         <v>199</v>
       </c>
       <c r="G173" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H173" t="str">
         <f t="shared" si="2"/>
@@ -7404,7 +7398,7 @@
         <v>722</v>
       </c>
       <c r="G174" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H174" t="str">
         <f t="shared" si="2"/>
@@ -7428,11 +7422,11 @@
         <v>793</v>
       </c>
       <c r="G175" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H175" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Danke", mnemonic = "Wie die Queen; vom Kinn aus nach vorn", tag1 ="Interaktion", tag2 ="Teil 1", tag3 ="" where name = "thank_you";</v>
+        <v>update signs set name_de = "Danke", mnemonic = "Wie die Queen; vom Kinn aus nach vorn", tag1 ="Interaktion", tag2 ="Teil 1" where name = "thank_you";</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.35">
@@ -7452,10 +7446,10 @@
         <v>793</v>
       </c>
       <c r="F176" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="G176" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H176" t="str">
         <f t="shared" si="2"/>
@@ -7482,7 +7476,7 @@
         <v>698</v>
       </c>
       <c r="G177" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H177" t="str">
         <f t="shared" si="2"/>
@@ -7509,7 +7503,7 @@
         <v>698</v>
       </c>
       <c r="G178" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H178" t="str">
         <f t="shared" si="2"/>
@@ -7527,16 +7521,16 @@
         <v>523</v>
       </c>
       <c r="D179" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E179" t="s">
         <v>794</v>
       </c>
       <c r="F179" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="G179" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H179" t="str">
         <f t="shared" si="2"/>
@@ -7560,11 +7554,11 @@
         <v>794</v>
       </c>
       <c r="G180" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H180" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Heute", mnemonic = "2x langsam vor sich nach unten zeigen", tag1 ="Zeit", tag2 ="Teil 3", tag3 ="" where name = "today";</v>
+        <v>update signs set name_de = "Heute", mnemonic = "2x langsam vor sich nach unten zeigen", tag1 ="Zeit", tag2 ="Teil 3" where name = "today";</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.35">
@@ -7587,7 +7581,7 @@
         <v>722</v>
       </c>
       <c r="G181" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H181" t="str">
         <f t="shared" si="2"/>
@@ -7611,11 +7605,11 @@
         <v>792</v>
       </c>
       <c r="G182" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H182" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Tomate", mnemonic = "Tomate vom Busch abdrehen", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "tomato";</v>
+        <v>update signs set name_de = "Tomate", mnemonic = "Tomate vom Busch abdrehen", tag1 ="Lebensmittel", tag2 ="Teil 2" where name = "tomato";</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.35">
@@ -7635,11 +7629,11 @@
         <v>794</v>
       </c>
       <c r="G183" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H183" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Morgen", mnemonic = "Großen Bogen nach vorn zeigen", tag1 ="Zeit", tag2 ="Teil 3", tag3 ="" where name = "tomorrow";</v>
+        <v>update signs set name_de = "Morgen", mnemonic = "Großen Bogen nach vorn zeigen", tag1 ="Zeit", tag2 ="Teil 3" where name = "tomorrow";</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.35">
@@ -7659,11 +7653,11 @@
         <v>794</v>
       </c>
       <c r="G184" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H184" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Handtuch", mnemonic = "Handtuch mit Zeigefinger umfahren", tag1 ="Körperpflege", tag2 ="Teil 3", tag3 ="" where name = "towel";</v>
+        <v>update signs set name_de = "Handtuch", mnemonic = "Handtuch mit Zeigefinger umfahren", tag1 ="Körperpflege", tag2 ="Teil 3" where name = "towel";</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.35">
@@ -7683,11 +7677,11 @@
         <v>792</v>
       </c>
       <c r="G185" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H185" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Kuscheltier", mnemonic = "Kuscheln zeigen", tag1 ="Spielen", tag2 ="Teil 2", tag3 ="" where name = "toy";</v>
+        <v>update signs set name_de = "Kuscheltier", mnemonic = "Kuscheln zeigen", tag1 ="Spielen", tag2 ="Teil 2" where name = "toy";</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.35">
@@ -7710,7 +7704,7 @@
         <v>408</v>
       </c>
       <c r="G186" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H186" t="str">
         <f t="shared" si="2"/>
@@ -7728,16 +7722,16 @@
         <v>547</v>
       </c>
       <c r="D187" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E187" t="s">
         <v>792</v>
       </c>
       <c r="F187" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="G187" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H187" t="str">
         <f t="shared" si="2"/>
@@ -7764,7 +7758,7 @@
         <v>698</v>
       </c>
       <c r="G188" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H188" t="str">
         <f t="shared" si="2"/>
@@ -7791,7 +7785,7 @@
         <v>714</v>
       </c>
       <c r="G189" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H189" t="str">
         <f t="shared" si="2"/>
@@ -7809,16 +7803,16 @@
         <v>556</v>
       </c>
       <c r="D190" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E190" t="s">
         <v>793</v>
       </c>
       <c r="F190" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="G190" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H190" t="str">
         <f t="shared" si="2"/>
@@ -7836,17 +7830,17 @@
         <v>559</v>
       </c>
       <c r="D191" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E191" t="s">
         <v>794</v>
       </c>
       <c r="G191" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H191" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Oben/Hoch", mnemonic = "Nach oben zeigen", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="" where name = "up";</v>
+        <v>update signs set name_de = "Oben/Hoch", mnemonic = "Nach oben zeigen", tag1 ="Kleine Worte", tag2 ="Teil 3" where name = "up";</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.35">
@@ -7869,7 +7863,7 @@
         <v>698</v>
       </c>
       <c r="G192" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H192" t="str">
         <f t="shared" si="2"/>
@@ -7896,7 +7890,7 @@
         <v>698</v>
       </c>
       <c r="G193" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H193" t="str">
         <f t="shared" si="2"/>
@@ -7920,11 +7914,11 @@
         <v>793</v>
       </c>
       <c r="G194" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H194" t="str">
         <f t="shared" si="2"/>
-        <v>update signs set name_de = "Waschen", mnemonic = "Hände waschen sich", tag1 ="Körperpflege", tag2 ="Teil 1", tag3 ="" where name = "washing";</v>
+        <v>update signs set name_de = "Waschen", mnemonic = "Hände waschen sich", tag1 ="Körperpflege", tag2 ="Teil 1" where name = "washing";</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.35">
@@ -7947,10 +7941,10 @@
         <v>199</v>
       </c>
       <c r="G195" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H195" t="str">
-        <f t="shared" ref="H195:H211" si="3">"update signs set name_de = """&amp;B195&amp;""", mnemonic = """&amp;C195&amp;""", tag1 ="""&amp;D195&amp;""", tag2 ="""&amp;E195&amp;""", tag3 ="""&amp;F195&amp;""" where name = """&amp;A195&amp;""";"</f>
+        <f t="shared" ref="H195:H211" si="3">IF(NOT(ISBLANK(F195)),"update signs set name_de = """&amp;B195&amp;""", mnemonic = """&amp;C195&amp;""", tag1 ="""&amp;D195&amp;""", tag2 ="""&amp;E195&amp;""", tag3 ="""&amp;F195&amp;""" where name = """&amp;A195&amp;""";","update signs set name_de = """&amp;B195&amp;""", mnemonic = """&amp;C195&amp;""", tag1 ="""&amp;D195&amp;""", tag2 ="""&amp;E195&amp;""" where name = """&amp;A195&amp;""";")</f>
         <v>update signs set name_de = "Wasser", mnemonic = "Steht mir bis zum Hals", tag1 ="Lebensmittel", tag2 ="Teil 1", tag3 ="Getränk" where name = "water";</v>
       </c>
     </row>
@@ -7965,16 +7959,16 @@
         <v>574</v>
       </c>
       <c r="D196" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="E196" t="s">
         <v>793</v>
       </c>
       <c r="F196" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="G196" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H196" t="str">
         <f t="shared" si="3"/>
@@ -7998,11 +7992,11 @@
         <v>793</v>
       </c>
       <c r="G197" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H197" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Was?", mnemonic = "Handflächen hin und her schütteln", tag1 ="Frage", tag2 ="Teil 1", tag3 ="" where name = "what";</v>
+        <v>update signs set name_de = "Was?", mnemonic = "Handflächen hin und her schütteln", tag1 ="Frage", tag2 ="Teil 1" where name = "what";</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.35">
@@ -8022,11 +8016,11 @@
         <v>794</v>
       </c>
       <c r="G198" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H198" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Wann?", mnemonic = "Finger klopfen ungeduldig an Wange", tag1 ="Frage", tag2 ="Teil 3", tag3 ="" where name = "when";</v>
+        <v>update signs set name_de = "Wann?", mnemonic = "Finger klopfen ungeduldig an Wange", tag1 ="Frage", tag2 ="Teil 3" where name = "when";</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.35">
@@ -8046,11 +8040,11 @@
         <v>793</v>
       </c>
       <c r="G199" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H199" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Wo?", mnemonic = "Schüssel mit Händen nachahmen", tag1 ="Frage", tag2 ="Teil 1", tag3 ="" where name = "where";</v>
+        <v>update signs set name_de = "Wo?", mnemonic = "Schüssel mit Händen nachahmen", tag1 ="Frage", tag2 ="Teil 1" where name = "where";</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.35">
@@ -8070,11 +8064,11 @@
         <v>794</v>
       </c>
       <c r="G200" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H200" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Wer?", mnemonic = "Fingeralphabet-R wackelt", tag1 ="Frage", tag2 ="Teil 3", tag3 ="" where name = "who";</v>
+        <v>update signs set name_de = "Wer?", mnemonic = "Fingeralphabet-R wackelt", tag1 ="Frage", tag2 ="Teil 3" where name = "who";</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.35">
@@ -8094,11 +8088,11 @@
         <v>792</v>
       </c>
       <c r="G201" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H201" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Fenster", mnemonic = "Mit Zeigefingern Fenster in Luft malen", tag1 ="Haus", tag2 ="Teil 2", tag3 ="" where name = "window";</v>
+        <v>update signs set name_de = "Fenster", mnemonic = "Mit Zeigefingern Fenster in Luft malen", tag1 ="Haus", tag2 ="Teil 2" where name = "window";</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.35">
@@ -8112,17 +8106,17 @@
         <v>592</v>
       </c>
       <c r="D202" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E202" t="s">
         <v>792</v>
       </c>
       <c r="G202" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H202" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Mit", mnemonic = "Daumen kommt mit anderen Fingern mit", tag1 ="Kleine Worte", tag2 ="Teil 2", tag3 ="" where name = "with";</v>
+        <v>update signs set name_de = "Mit", mnemonic = "Daumen kommt mit anderen Fingern mit", tag1 ="Kleine Worte", tag2 ="Teil 2" where name = "with";</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.35">
@@ -8142,11 +8136,11 @@
         <v>792</v>
       </c>
       <c r="G203" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H203" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Frau", mnemonic = "Ohrring", tag1 ="Person", tag2 ="Teil 2", tag3 ="" where name = "woman";</v>
+        <v>update signs set name_de = "Frau", mnemonic = "Ohrring", tag1 ="Person", tag2 ="Teil 2" where name = "woman";</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.35">
@@ -8169,7 +8163,7 @@
         <v>698</v>
       </c>
       <c r="G204" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H204" t="str">
         <f t="shared" si="3"/>
@@ -8196,7 +8190,7 @@
         <v>677</v>
       </c>
       <c r="G205" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H205" t="str">
         <f t="shared" si="3"/>
@@ -8220,10 +8214,10 @@
         <v>793</v>
       </c>
       <c r="F206" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="G206" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H206" t="str">
         <f t="shared" si="3"/>
@@ -8247,11 +8241,11 @@
         <v>794</v>
       </c>
       <c r="G207" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H207" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Gestern", mnemonic = "Großen Bogen  nach hinten zeigen", tag1 ="Zeit", tag2 ="Teil 3", tag3 ="" where name = "yesterday";</v>
+        <v>update signs set name_de = "Gestern", mnemonic = "Großen Bogen  nach hinten zeigen", tag1 ="Zeit", tag2 ="Teil 3" where name = "yesterday";</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.35">
@@ -8271,11 +8265,11 @@
         <v>792</v>
       </c>
       <c r="G208" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H208" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Joghurt", mnemonic = "Becher auslöffen", tag1 ="Lebensmittel", tag2 ="Teil 2", tag3 ="" where name = "yoghurt";</v>
+        <v>update signs set name_de = "Joghurt", mnemonic = "Becher auslöffen", tag1 ="Lebensmittel", tag2 ="Teil 2" where name = "yoghurt";</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.35">
@@ -8295,10 +8289,10 @@
         <v>793</v>
       </c>
       <c r="F209" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="G209" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H209" t="str">
         <f t="shared" si="3"/>
@@ -8310,7 +8304,7 @@
         <v>614</v>
       </c>
       <c r="B210" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="C210" t="s">
         <v>278</v>
@@ -8325,7 +8319,7 @@
         <v>698</v>
       </c>
       <c r="G210" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H210" t="str">
         <f t="shared" si="3"/>
@@ -8343,17 +8337,17 @@
         <v>617</v>
       </c>
       <c r="D211" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E211" t="s">
         <v>794</v>
       </c>
       <c r="G211" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="H211" t="str">
         <f t="shared" si="3"/>
-        <v>update signs set name_de = "Dein", mnemonic = "Handfläche zeigt langsam auf Gesprächspartner", tag1 ="Kleine Worte", tag2 ="Teil 3", tag3 ="" where name = "yours";</v>
+        <v>update signs set name_de = "Dein", mnemonic = "Handfläche zeigt langsam auf Gesprächspartner", tag1 ="Kleine Worte", tag2 ="Teil 3" where name = "yours";</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.35">
@@ -8373,8 +8367,8 @@
         <v>674</v>
       </c>
       <c r="H212" t="str">
-        <f>"insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("""&amp;$A212&amp;""","""&amp;$B212&amp;""","""&amp;$C212&amp;""","""&amp;$D212&amp;""","""&amp;$E212&amp;""","""&amp;$F212&amp;""");"</f>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("evening","Abend","Handflächen legen sich von außen kommend übereinander","Zeit","Zusatz","");</v>
+        <f>IF(NOT(ISBLANK(F212)),"insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("""&amp;$A212&amp;""","""&amp;$B212&amp;""","""&amp;$C212&amp;""","""&amp;$D212&amp;""","""&amp;$E212&amp;""","""&amp;$F212&amp;""");","insert into signs (name, name_de, mnemonic, tag1, tag2) values ("""&amp;$A212&amp;""","""&amp;$B212&amp;""","""&amp;$C212&amp;""","""&amp;$D212&amp;""","""&amp;$E212&amp;""");")</f>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("evening","Abend","Handflächen legen sich von außen kommend übereinander","Zeit","Zusatz");</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.35">
@@ -8394,8 +8388,8 @@
         <v>674</v>
       </c>
       <c r="H213" t="str">
-        <f t="shared" ref="H213:H264" si="4">"insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("""&amp;$A213&amp;""","""&amp;$B213&amp;""","""&amp;$C213&amp;""","""&amp;$D213&amp;""","""&amp;$E213&amp;""","""&amp;$F213&amp;""");"</f>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("old","alt","mit Zügelhand kleines Stück an Wange runtersteichen","Eigenschaften","Zusatz","");</v>
+        <f t="shared" ref="H213:H264" si="4">IF(NOT(ISBLANK(F213)),"insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("""&amp;$A213&amp;""","""&amp;$B213&amp;""","""&amp;$C213&amp;""","""&amp;$D213&amp;""","""&amp;$E213&amp;""","""&amp;$F213&amp;""");","insert into signs (name, name_de, mnemonic, tag1, tag2) values ("""&amp;$A213&amp;""","""&amp;$B213&amp;""","""&amp;$C213&amp;""","""&amp;$D213&amp;""","""&amp;$E213&amp;""");")</f>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("old","alt","mit Zügelhand kleines Stück an Wange runtersteichen","Eigenschaften","Zusatz");</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.35">
@@ -8416,7 +8410,7 @@
       </c>
       <c r="H214" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("anxiety","Angst","Faust klopft an Herz; Herzklopfen vor Angst","Gefühl","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("anxiety","Angst","Faust klopft an Herz; Herzklopfen vor Angst","Gefühl","Zusatz");</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.35">
@@ -8436,7 +8430,7 @@
         <v>674</v>
       </c>
       <c r="F215" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="H215" t="str">
         <f t="shared" si="4"/>
@@ -8461,7 +8455,7 @@
       </c>
       <c r="H216" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("bossmang","Chef","Gut'-Faust steigt von anderem Handrücken auf","Person","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("bossmang","Chef","Gut'-Faust steigt von anderem Handrücken auf","Person","Zusatz");</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.35">
@@ -8482,7 +8476,7 @@
       </c>
       <c r="H217" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("computer","Computer","Zehn Finger tippen auf Tastatur","Arbeit","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("computer","Computer","Zehn Finger tippen auf Tastatur","Arbeit","Zusatz");</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.35">
@@ -8503,7 +8497,7 @@
       </c>
       <c r="H218" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("morning","der Morgen","es wird hell'","Zeit","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("morning","der Morgen","es wird hell'","Zeit","Zusatz");</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.35">
@@ -8538,7 +8532,7 @@
         <v>625</v>
       </c>
       <c r="C220" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="D220" t="s">
         <v>694</v>
@@ -8572,7 +8566,7 @@
       </c>
       <c r="H221" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("allowed","dürfen","Flachhand kippt nach vorn","Verb","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("allowed","dürfen","Flachhand kippt nach vorn","Verb","Zusatz");</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.35">
@@ -8641,7 +8635,7 @@
       </c>
       <c r="H224" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("friday","Freitag","Zeigefinger von Nasenspitze an Stirn drehen","Wochentag","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("friday","Freitag","Zeigefinger von Nasenspitze an Stirn drehen","Wochentag","Zusatz");</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.35">
@@ -8662,7 +8656,7 @@
       </c>
       <c r="H225" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("happiness","Freude","Handflächen wedeln aufsteigende Freude vor dem Bauch","Gefühl","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("happiness","Freude","Handflächen wedeln aufsteigende Freude vor dem Bauch","Gefühl","Zusatz");</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.35">
@@ -8683,7 +8677,7 @@
       </c>
       <c r="H226" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("happy","fröhlich","Handflächen wedeln aufsteigende Freude vor dem Bauch","Gefühl","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("happy","fröhlich","Handflächen wedeln aufsteigende Freude vor dem Bauch","Gefühl","Zusatz");</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.35">
@@ -8704,7 +8698,7 @@
       </c>
       <c r="H227" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("spring","Frühling","sich öffnende Blume seitlich auf Schulterhöhe","Jahreszeit","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("spring","Frühling","sich öffnende Blume seitlich auf Schulterhöhe","Jahreszeit","Zusatz");</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.35">
@@ -8742,7 +8736,7 @@
         <v>717</v>
       </c>
       <c r="D229" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E229" t="s">
         <v>674</v>
@@ -8773,7 +8767,7 @@
       </c>
       <c r="H230" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("autumn","Herbst","Gegenbewegung zu Frühling: Pflanzen verschwinden wieder in Erde (Blumenzwiebeln, Stauden..)","Jahreszeit","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("autumn","Herbst","Gegenbewegung zu Frühling: Pflanzen verschwinden wieder in Erde (Blumenzwiebeln, Stauden..)","Jahreszeit","Zusatz");</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.35">
@@ -8817,7 +8811,7 @@
         <v>674</v>
       </c>
       <c r="F232" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="H232" t="str">
         <f t="shared" si="4"/>
@@ -8835,7 +8829,7 @@
         <v>725</v>
       </c>
       <c r="D233" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E233" t="s">
         <v>674</v>
@@ -8890,7 +8884,7 @@
       </c>
       <c r="H235" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("slow","langsam","flache Hände 2x langsam vor Körper senken","Eigenschaften","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("slow","langsam","flache Hände 2x langsam vor Körper senken","Eigenschaften","Zusatz");</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.35">
@@ -8983,7 +8977,7 @@
       </c>
       <c r="H239" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("wednesday","Mittwoch","Pistolenhand 2x an Kinn tupfen","Wochentag","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("wednesday","Mittwoch","Pistolenhand 2x an Kinn tupfen","Wochentag","Zusatz");</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.35">
@@ -9004,7 +8998,7 @@
       </c>
       <c r="H240" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("monday","Montag","Daumennagel streicht an Wange runter","Wochentag","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("monday","Montag","Daumennagel streicht an Wange runter","Wochentag","Zusatz");</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.35">
@@ -9025,7 +9019,7 @@
       </c>
       <c r="H241" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("night","Nacht","Handflächen schließen zu Fäusten","Zeit","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("night","Nacht","Handflächen schließen zu Fäusten","Zeit","Zusatz");</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.35">
@@ -9046,7 +9040,7 @@
       </c>
       <c r="H242" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("name","Name","Zeige-und Mittelfinger 3x an Wange  klopfen","Person","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("name","Name","Zeige-und Mittelfinger 3x an Wange  klopfen","Person","Zusatz");</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.35">
@@ -9060,7 +9054,7 @@
         <v>747</v>
       </c>
       <c r="D243" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E243" t="s">
         <v>674</v>
@@ -9084,14 +9078,14 @@
         <v>749</v>
       </c>
       <c r="D244" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E244" t="s">
         <v>674</v>
       </c>
       <c r="H244" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("never","nie","Zeigefinger-X schnell auseinanderziehen","Kleine Worte","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("never","nie","Zeigefinger-X schnell auseinanderziehen","Kleine Worte","Zusatz");</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.35">
@@ -9160,7 +9154,7 @@
       </c>
       <c r="H247" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("saturday","Samstag","mit Handrücken 'Lächeln' unter Kinn zeigen","Wochentag","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("saturday","Samstag","mit Handrücken 'Lächeln' unter Kinn zeigen","Wochentag","Zusatz");</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.35">
@@ -9174,7 +9168,7 @@
         <v>757</v>
       </c>
       <c r="D248" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E248" t="s">
         <v>674</v>
@@ -9205,7 +9199,7 @@
       </c>
       <c r="H249" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("summer","Sommer","wie 'warm'","Jahreszeit","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("summer","Sommer","wie 'warm'","Jahreszeit","Zusatz");</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.35">
@@ -9226,7 +9220,7 @@
       </c>
       <c r="H250" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("sunday","Sonntag","'schicke Kleidung' mit Handstreichen über Oberkörper zeigen","Wochentag","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("sunday","Sonntag","'schicke Kleidung' mit Handstreichen über Oberkörper zeigen","Wochentag","Zusatz");</v>
       </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.35">
@@ -9271,7 +9265,7 @@
       </c>
       <c r="H252" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("day","Tag","beide Pinzettengriffe ziehen Tag wie Kaugummi auseinander","Zeit","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("day","Tag","beide Pinzettengriffe ziehen Tag wie Kaugummi auseinander","Zeit","Zusatz");</v>
       </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.35">
@@ -9333,7 +9327,7 @@
         <v>771</v>
       </c>
       <c r="D255" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E255" t="s">
         <v>674</v>
@@ -9364,7 +9358,7 @@
       </c>
       <c r="H256" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("why","warum","bohrender Zeigefinger (bohrende Frage)","Frage","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("why","warum","bohrender Zeigefinger (bohrende Frage)","Frage","Zusatz");</v>
       </c>
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.35">
@@ -9385,7 +9379,7 @@
       </c>
       <c r="H257" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("which","welche","eine Flugzeug-Hand 3x wackeln","Frage","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("which","welche","eine Flugzeug-Hand 3x wackeln","Frage","Zusatz");</v>
       </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.35">
@@ -9406,7 +9400,7 @@
       </c>
       <c r="H258" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("how_many","wie viele","zappelnde Finger einer Hand neben Schulter","Frage","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("how_many","wie viele","zappelnde Finger einer Hand neben Schulter","Frage","Zusatz");</v>
       </c>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.35">
@@ -9427,7 +9421,7 @@
       </c>
       <c r="H259" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("how","wie","Flugzeug-Hände; kleine Finger überkreuz auseinanderziehen","Frage","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("how","wie","Flugzeug-Hände; kleine Finger überkreuz auseinanderziehen","Frage","Zusatz");</v>
       </c>
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.35">
@@ -9448,7 +9442,7 @@
       </c>
       <c r="H260" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("winter","Winter","wie 'kalt'","Jahreszeit","Zusatz","");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2) values ("winter","Winter","wie 'kalt'","Jahreszeit","Zusatz");</v>
       </c>
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.35">
@@ -9534,7 +9528,7 @@
         <v>791</v>
       </c>
       <c r="D264" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E264" t="s">
         <v>674</v>

</xml_diff>

<commit_message>
#97 Fixing a typo
</commit_message>
<xml_diff>
--- a/database/VideosUkGebärden.xlsx
+++ b/database/VideosUkGebärden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User-Matthias\Dev\Android\UKGM\src\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15592425-DF67-4987-8294-C604F13DB3C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AAD3F4-CD2E-46CD-A4F8-43F0DF123D82}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{978A20FD-486C-4CB5-9933-67C562CBE71F}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="834">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1662" uniqueCount="835">
   <si>
     <t>afterwards</t>
   </si>
@@ -2444,9 +2444,6 @@
     <t>together</t>
   </si>
   <si>
-    <t>von außen mit ffenen Handflächen alles zusammenballen</t>
-  </si>
-  <si>
     <t>Teil 2</t>
   </si>
   <si>
@@ -2571,6 +2568,12 @@
   </si>
   <si>
     <t>Geht es dir gut?</t>
+  </si>
+  <si>
+    <t>you_plural</t>
+  </si>
+  <si>
+    <t>von außen mit offenen Handflächen alles zusammenballen</t>
   </si>
 </sst>
 </file>
@@ -2963,8 +2966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C22E1E0-4D2F-4ED8-9423-514FCF041C4D}">
   <dimension ref="A1:H264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G200" workbookViewId="0">
-      <selection activeCell="H212" sqref="H212"/>
+    <sheetView tabSelected="1" topLeftCell="C249" workbookViewId="0">
+      <selection activeCell="C265" sqref="C265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2977,28 +2980,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>819</v>
+      </c>
+      <c r="B1" t="s">
         <v>820</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>821</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>822</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>823</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>824</v>
       </c>
-      <c r="F1" t="s">
-        <v>825</v>
-      </c>
       <c r="G1" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -3015,10 +3018,10 @@
         <v>673</v>
       </c>
       <c r="E2" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G2" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H2" t="str">
         <f>IF(NOT(ISBLANK(F2)),"update signs set name_de = """&amp;B2&amp;""", mnemonic = """&amp;C2&amp;""", tag1 ="""&amp;D2&amp;""", tag2 ="""&amp;E2&amp;""", tag3 ="""&amp;F2&amp;""" where name = """&amp;A2&amp;""";","update signs set name_de = """&amp;B2&amp;""", mnemonic = """&amp;C2&amp;""", tag1 ="""&amp;D2&amp;""", tag2 ="""&amp;E2&amp;""" where name = """&amp;A2&amp;""";")</f>
@@ -3036,13 +3039,13 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E3" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H66" si="0">IF(NOT(ISBLANK(F3)),"update signs set name_de = """&amp;B3&amp;""", mnemonic = """&amp;C3&amp;""", tag1 ="""&amp;D3&amp;""", tag2 ="""&amp;E3&amp;""", tag3 ="""&amp;F3&amp;""" where name = """&amp;A3&amp;""";","update signs set name_de = """&amp;B3&amp;""", mnemonic = """&amp;C3&amp;""", tag1 ="""&amp;D3&amp;""", tag2 ="""&amp;E3&amp;""" where name = """&amp;A3&amp;""";")</f>
@@ -3063,10 +3066,10 @@
         <v>703</v>
       </c>
       <c r="E4" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G4" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -3084,13 +3087,13 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E5" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G5" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -3108,13 +3111,13 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E6" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G6" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -3135,10 +3138,10 @@
         <v>683</v>
       </c>
       <c r="E7" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G7" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -3159,10 +3162,10 @@
         <v>728</v>
       </c>
       <c r="E8" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G8" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -3174,7 +3177,7 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
@@ -3183,10 +3186,10 @@
         <v>683</v>
       </c>
       <c r="E9" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G9" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -3204,16 +3207,16 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E10" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F10" t="s">
         <v>683</v>
       </c>
       <c r="G10" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -3234,10 +3237,10 @@
         <v>686</v>
       </c>
       <c r="E11" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G11" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -3258,10 +3261,10 @@
         <v>677</v>
       </c>
       <c r="E12" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G12" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -3279,13 +3282,13 @@
         <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E13" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G13" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -3303,16 +3306,16 @@
         <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E14" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F14" t="s">
         <v>698</v>
       </c>
       <c r="G14" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -3333,10 +3336,10 @@
         <v>408</v>
       </c>
       <c r="E15" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G15" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -3357,10 +3360,10 @@
         <v>728</v>
       </c>
       <c r="E16" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G16" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -3378,16 +3381,16 @@
         <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E17" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F17" t="s">
         <v>698</v>
       </c>
       <c r="G17" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -3408,10 +3411,10 @@
         <v>289</v>
       </c>
       <c r="E18" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G18" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -3432,10 +3435,10 @@
         <v>289</v>
       </c>
       <c r="E19" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G19" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -3456,13 +3459,13 @@
         <v>673</v>
       </c>
       <c r="E20" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F20" t="s">
         <v>673</v>
       </c>
       <c r="G20" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -3483,13 +3486,13 @@
         <v>689</v>
       </c>
       <c r="E21" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F21" t="s">
         <v>698</v>
       </c>
       <c r="G21" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -3507,16 +3510,16 @@
         <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E22" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F22" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="G22" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -3537,10 +3540,10 @@
         <v>677</v>
       </c>
       <c r="E23" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G23" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -3561,10 +3564,10 @@
         <v>703</v>
       </c>
       <c r="E24" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G24" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
@@ -3582,13 +3585,13 @@
         <v>70</v>
       </c>
       <c r="D25" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E25" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G25" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
@@ -3600,19 +3603,19 @@
         <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C26" t="s">
         <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E26" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G26" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
@@ -3630,16 +3633,16 @@
         <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E27" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F27" t="s">
         <v>677</v>
       </c>
       <c r="G27" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
@@ -3660,13 +3663,13 @@
         <v>408</v>
       </c>
       <c r="E28" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F28" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="G28" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
@@ -3687,10 +3690,10 @@
         <v>686</v>
       </c>
       <c r="E29" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G29" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
@@ -3711,10 +3714,10 @@
         <v>728</v>
       </c>
       <c r="E30" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G30" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
@@ -3735,10 +3738,10 @@
         <v>677</v>
       </c>
       <c r="E31" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G31" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
@@ -3756,13 +3759,13 @@
         <v>90</v>
       </c>
       <c r="D32" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E32" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G32" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
@@ -3780,13 +3783,13 @@
         <v>93</v>
       </c>
       <c r="D33" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E33" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G33" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
@@ -3804,13 +3807,13 @@
         <v>96</v>
       </c>
       <c r="D34" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E34" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G34" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="0"/>
@@ -3831,10 +3834,10 @@
         <v>408</v>
       </c>
       <c r="E35" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G35" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="0"/>
@@ -3855,10 +3858,10 @@
         <v>703</v>
       </c>
       <c r="E36" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G36" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="0"/>
@@ -3879,10 +3882,10 @@
         <v>728</v>
       </c>
       <c r="E37" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G37" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="0"/>
@@ -3900,13 +3903,13 @@
         <v>108</v>
       </c>
       <c r="D38" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E38" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G38" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="0"/>
@@ -3927,13 +3930,13 @@
         <v>728</v>
       </c>
       <c r="E39" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F39" t="s">
         <v>199</v>
       </c>
       <c r="G39" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="0"/>
@@ -3954,10 +3957,10 @@
         <v>728</v>
       </c>
       <c r="E40" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G40" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="0"/>
@@ -3978,10 +3981,10 @@
         <v>703</v>
       </c>
       <c r="E41" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G41" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="0"/>
@@ -4002,10 +4005,10 @@
         <v>683</v>
       </c>
       <c r="E42" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G42" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="0"/>
@@ -4026,10 +4029,10 @@
         <v>728</v>
       </c>
       <c r="E43" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G43" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="0"/>
@@ -4047,13 +4050,13 @@
         <v>126</v>
       </c>
       <c r="D44" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E44" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G44" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
@@ -4074,10 +4077,10 @@
         <v>289</v>
       </c>
       <c r="E45" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G45" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="0"/>
@@ -4095,13 +4098,13 @@
         <v>132</v>
       </c>
       <c r="D46" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E46" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G46" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
@@ -4122,10 +4125,10 @@
         <v>686</v>
       </c>
       <c r="E47" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G47" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
@@ -4146,10 +4149,10 @@
         <v>728</v>
       </c>
       <c r="E48" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G48" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
@@ -4170,10 +4173,10 @@
         <v>677</v>
       </c>
       <c r="E49" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G49" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
@@ -4194,13 +4197,13 @@
         <v>714</v>
       </c>
       <c r="E50" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F50" t="s">
         <v>698</v>
       </c>
       <c r="G50" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
@@ -4221,13 +4224,13 @@
         <v>289</v>
       </c>
       <c r="E51" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F51" t="s">
         <v>698</v>
       </c>
       <c r="G51" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
@@ -4248,10 +4251,10 @@
         <v>728</v>
       </c>
       <c r="E52" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G52" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
@@ -4272,10 +4275,10 @@
         <v>677</v>
       </c>
       <c r="E53" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G53" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="0"/>
@@ -4296,13 +4299,13 @@
         <v>683</v>
       </c>
       <c r="E54" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F54" t="s">
         <v>698</v>
       </c>
       <c r="G54" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="0"/>
@@ -4323,10 +4326,10 @@
         <v>728</v>
       </c>
       <c r="E55" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G55" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
@@ -4344,16 +4347,16 @@
         <v>161</v>
       </c>
       <c r="D56" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E56" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F56" t="s">
         <v>698</v>
       </c>
       <c r="G56" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="0"/>
@@ -4371,13 +4374,13 @@
         <v>164</v>
       </c>
       <c r="D57" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E57" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G57" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="0"/>
@@ -4398,10 +4401,10 @@
         <v>728</v>
       </c>
       <c r="E58" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G58" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="0"/>
@@ -4422,10 +4425,10 @@
         <v>289</v>
       </c>
       <c r="E59" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G59" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H59" t="str">
         <f t="shared" si="0"/>
@@ -4443,13 +4446,13 @@
         <v>173</v>
       </c>
       <c r="D60" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E60" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G60" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" si="0"/>
@@ -4467,13 +4470,13 @@
         <v>176</v>
       </c>
       <c r="D61" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E61" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G61" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H61" t="str">
         <f t="shared" si="0"/>
@@ -4491,16 +4494,16 @@
         <v>179</v>
       </c>
       <c r="D62" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E62" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F62" t="s">
         <v>677</v>
       </c>
       <c r="G62" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="0"/>
@@ -4521,10 +4524,10 @@
         <v>686</v>
       </c>
       <c r="E63" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G63" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H63" t="str">
         <f t="shared" si="0"/>
@@ -4542,13 +4545,13 @@
         <v>185</v>
       </c>
       <c r="D64" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E64" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G64" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="0"/>
@@ -4569,10 +4572,10 @@
         <v>408</v>
       </c>
       <c r="E65" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G65" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H65" t="str">
         <f t="shared" si="0"/>
@@ -4593,13 +4596,13 @@
         <v>677</v>
       </c>
       <c r="E66" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F66" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G66" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H66" t="str">
         <f t="shared" si="0"/>
@@ -4620,10 +4623,10 @@
         <v>289</v>
       </c>
       <c r="E67" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G67" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H67" t="str">
         <f t="shared" ref="H67:H130" si="1">IF(NOT(ISBLANK(F67)),"update signs set name_de = """&amp;B67&amp;""", mnemonic = """&amp;C67&amp;""", tag1 ="""&amp;D67&amp;""", tag2 ="""&amp;E67&amp;""", tag3 ="""&amp;F67&amp;""" where name = """&amp;A67&amp;""";","update signs set name_de = """&amp;B67&amp;""", mnemonic = """&amp;C67&amp;""", tag1 ="""&amp;D67&amp;""", tag2 ="""&amp;E67&amp;""" where name = """&amp;A67&amp;""";")</f>
@@ -4641,16 +4644,16 @@
         <v>197</v>
       </c>
       <c r="D68" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E68" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F68" t="s">
         <v>677</v>
       </c>
       <c r="G68" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H68" t="str">
         <f t="shared" si="1"/>
@@ -4671,13 +4674,13 @@
         <v>728</v>
       </c>
       <c r="E69" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F69" t="s">
         <v>199</v>
       </c>
       <c r="G69" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H69" t="str">
         <f t="shared" si="1"/>
@@ -4695,16 +4698,16 @@
         <v>203</v>
       </c>
       <c r="D70" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E70" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F70" t="s">
         <v>698</v>
       </c>
       <c r="G70" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H70" t="str">
         <f t="shared" si="1"/>
@@ -4722,13 +4725,13 @@
         <v>206</v>
       </c>
       <c r="D71" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E71" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G71" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H71" t="str">
         <f t="shared" si="1"/>
@@ -4746,16 +4749,16 @@
         <v>209</v>
       </c>
       <c r="D72" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E72" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F72" t="s">
         <v>698</v>
       </c>
       <c r="G72" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H72" t="str">
         <f t="shared" si="1"/>
@@ -4776,10 +4779,10 @@
         <v>728</v>
       </c>
       <c r="E73" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G73" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H73" t="str">
         <f t="shared" si="1"/>
@@ -4797,16 +4800,16 @@
         <v>215</v>
       </c>
       <c r="D74" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E74" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F74" t="s">
         <v>677</v>
       </c>
       <c r="G74" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H74" t="str">
         <f t="shared" si="1"/>
@@ -4827,13 +4830,13 @@
         <v>714</v>
       </c>
       <c r="E75" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F75" t="s">
         <v>698</v>
       </c>
       <c r="G75" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H75" t="str">
         <f t="shared" si="1"/>
@@ -4851,16 +4854,16 @@
         <v>221</v>
       </c>
       <c r="D76" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E76" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F76" t="s">
         <v>673</v>
       </c>
       <c r="G76" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H76" t="str">
         <f t="shared" si="1"/>
@@ -4878,13 +4881,13 @@
         <v>224</v>
       </c>
       <c r="D77" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E77" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G77" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H77" t="str">
         <f t="shared" si="1"/>
@@ -4902,16 +4905,16 @@
         <v>227</v>
       </c>
       <c r="D78" t="s">
+        <v>806</v>
+      </c>
+      <c r="E78" t="s">
+        <v>791</v>
+      </c>
+      <c r="F78" t="s">
         <v>807</v>
       </c>
-      <c r="E78" t="s">
-        <v>792</v>
-      </c>
-      <c r="F78" t="s">
-        <v>808</v>
-      </c>
       <c r="G78" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H78" t="str">
         <f t="shared" si="1"/>
@@ -4932,13 +4935,13 @@
         <v>683</v>
       </c>
       <c r="E79" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F79" t="s">
         <v>677</v>
       </c>
       <c r="G79" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H79" t="str">
         <f t="shared" si="1"/>
@@ -4950,7 +4953,7 @@
         <v>231</v>
       </c>
       <c r="B80" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C80" t="s">
         <v>232</v>
@@ -4959,13 +4962,13 @@
         <v>714</v>
       </c>
       <c r="E80" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F80" t="s">
         <v>698</v>
       </c>
       <c r="G80" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H80" t="str">
         <f t="shared" si="1"/>
@@ -4983,13 +4986,13 @@
         <v>235</v>
       </c>
       <c r="D81" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E81" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G81" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H81" t="str">
         <f t="shared" si="1"/>
@@ -5010,10 +5013,10 @@
         <v>686</v>
       </c>
       <c r="E82" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G82" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H82" t="str">
         <f t="shared" si="1"/>
@@ -5031,16 +5034,16 @@
         <v>241</v>
       </c>
       <c r="D83" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E83" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F83" t="s">
         <v>677</v>
       </c>
       <c r="G83" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H83" t="str">
         <f t="shared" si="1"/>
@@ -5061,13 +5064,13 @@
         <v>683</v>
       </c>
       <c r="E84" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F84" t="s">
         <v>714</v>
       </c>
       <c r="G84" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H84" t="str">
         <f t="shared" si="1"/>
@@ -5088,10 +5091,10 @@
         <v>686</v>
       </c>
       <c r="E85" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G85" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H85" t="str">
         <f t="shared" si="1"/>
@@ -5112,13 +5115,13 @@
         <v>683</v>
       </c>
       <c r="E86" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F86" t="s">
         <v>698</v>
       </c>
       <c r="G86" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H86" t="str">
         <f t="shared" si="1"/>
@@ -5136,13 +5139,13 @@
         <v>253</v>
       </c>
       <c r="D87" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E87" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G87" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H87" t="str">
         <f t="shared" si="1"/>
@@ -5154,22 +5157,22 @@
         <v>254</v>
       </c>
       <c r="B88" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C88" t="s">
         <v>255</v>
       </c>
       <c r="D88" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E88" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F88" t="s">
         <v>677</v>
       </c>
       <c r="G88" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H88" t="str">
         <f t="shared" si="1"/>
@@ -5181,7 +5184,7 @@
         <v>256</v>
       </c>
       <c r="B89" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C89" t="s">
         <v>257</v>
@@ -5190,10 +5193,10 @@
         <v>683</v>
       </c>
       <c r="E89" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G89" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H89" t="str">
         <f t="shared" si="1"/>
@@ -5211,13 +5214,13 @@
         <v>260</v>
       </c>
       <c r="D90" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E90" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G90" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H90" t="str">
         <f t="shared" si="1"/>
@@ -5235,16 +5238,16 @@
         <v>263</v>
       </c>
       <c r="D91" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E91" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F91" t="s">
         <v>677</v>
       </c>
       <c r="G91" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H91" t="str">
         <f t="shared" si="1"/>
@@ -5265,10 +5268,10 @@
         <v>686</v>
       </c>
       <c r="E92" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G92" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H92" t="str">
         <f t="shared" si="1"/>
@@ -5289,10 +5292,10 @@
         <v>686</v>
       </c>
       <c r="E93" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G93" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H93" t="str">
         <f t="shared" si="1"/>
@@ -5310,16 +5313,16 @@
         <v>272</v>
       </c>
       <c r="D94" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E94" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F94" t="s">
         <v>677</v>
       </c>
       <c r="G94" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H94" t="str">
         <f t="shared" si="1"/>
@@ -5340,13 +5343,13 @@
         <v>683</v>
       </c>
       <c r="E95" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F95" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G95" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H95" t="str">
         <f t="shared" si="1"/>
@@ -5367,13 +5370,13 @@
         <v>683</v>
       </c>
       <c r="E96" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F96" t="s">
         <v>698</v>
       </c>
       <c r="G96" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H96" t="str">
         <f t="shared" si="1"/>
@@ -5391,13 +5394,13 @@
         <v>281</v>
       </c>
       <c r="D97" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E97" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G97" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H97" t="str">
         <f t="shared" si="1"/>
@@ -5415,13 +5418,13 @@
         <v>284</v>
       </c>
       <c r="D98" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E98" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G98" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H98" t="str">
         <f t="shared" si="1"/>
@@ -5439,16 +5442,16 @@
         <v>287</v>
       </c>
       <c r="D99" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E99" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F99" t="s">
         <v>677</v>
       </c>
       <c r="G99" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H99" t="str">
         <f t="shared" si="1"/>
@@ -5469,10 +5472,10 @@
         <v>289</v>
       </c>
       <c r="E100" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G100" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H100" t="str">
         <f t="shared" si="1"/>
@@ -5493,10 +5496,10 @@
         <v>686</v>
       </c>
       <c r="E101" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G101" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H101" t="str">
         <f t="shared" si="1"/>
@@ -5517,10 +5520,10 @@
         <v>728</v>
       </c>
       <c r="E102" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G102" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H102" t="str">
         <f t="shared" si="1"/>
@@ -5538,16 +5541,16 @@
         <v>299</v>
       </c>
       <c r="D103" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E103" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F103" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="G103" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H103" t="str">
         <f t="shared" si="1"/>
@@ -5565,16 +5568,16 @@
         <v>302</v>
       </c>
       <c r="D104" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E104" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F104" t="s">
         <v>686</v>
       </c>
       <c r="G104" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H104" t="str">
         <f t="shared" si="1"/>
@@ -5595,13 +5598,13 @@
         <v>728</v>
       </c>
       <c r="E105" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F105" t="s">
         <v>199</v>
       </c>
       <c r="G105" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H105" t="str">
         <f t="shared" si="1"/>
@@ -5622,13 +5625,13 @@
         <v>714</v>
       </c>
       <c r="E106" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F106" t="s">
         <v>698</v>
       </c>
       <c r="G106" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H106" t="str">
         <f t="shared" si="1"/>
@@ -5649,13 +5652,13 @@
         <v>289</v>
       </c>
       <c r="E107" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F107" t="s">
         <v>408</v>
       </c>
       <c r="G107" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H107" t="str">
         <f t="shared" si="1"/>
@@ -5676,10 +5679,10 @@
         <v>289</v>
       </c>
       <c r="E108" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G108" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H108" t="str">
         <f t="shared" si="1"/>
@@ -5697,16 +5700,16 @@
         <v>317</v>
       </c>
       <c r="D109" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E109" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F109" t="s">
         <v>698</v>
       </c>
       <c r="G109" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H109" t="str">
         <f t="shared" si="1"/>
@@ -5727,10 +5730,10 @@
         <v>289</v>
       </c>
       <c r="E110" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G110" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H110" t="str">
         <f t="shared" si="1"/>
@@ -5748,16 +5751,16 @@
         <v>323</v>
       </c>
       <c r="D111" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E111" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F111" t="s">
         <v>673</v>
       </c>
       <c r="G111" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H111" t="str">
         <f t="shared" si="1"/>
@@ -5778,13 +5781,13 @@
         <v>683</v>
       </c>
       <c r="E112" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F112" t="s">
         <v>698</v>
       </c>
       <c r="G112" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H112" t="str">
         <f t="shared" si="1"/>
@@ -5805,13 +5808,13 @@
         <v>683</v>
       </c>
       <c r="E113" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F113" t="s">
         <v>698</v>
       </c>
       <c r="G113" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H113" t="str">
         <f t="shared" si="1"/>
@@ -5832,13 +5835,13 @@
         <v>689</v>
       </c>
       <c r="E114" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F114" t="s">
         <v>698</v>
       </c>
       <c r="G114" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H114" t="str">
         <f t="shared" si="1"/>
@@ -5859,10 +5862,10 @@
         <v>686</v>
       </c>
       <c r="E115" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G115" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H115" t="str">
         <f t="shared" si="1"/>
@@ -5883,10 +5886,10 @@
         <v>686</v>
       </c>
       <c r="E116" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G116" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H116" t="str">
         <f t="shared" si="1"/>
@@ -5904,16 +5907,16 @@
         <v>341</v>
       </c>
       <c r="D117" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E117" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F117" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="G117" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H117" t="str">
         <f t="shared" si="1"/>
@@ -5934,10 +5937,10 @@
         <v>728</v>
       </c>
       <c r="E118" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G118" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H118" t="str">
         <f t="shared" si="1"/>
@@ -5958,13 +5961,13 @@
         <v>728</v>
       </c>
       <c r="E119" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F119" t="s">
         <v>199</v>
       </c>
       <c r="G119" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H119" t="str">
         <f t="shared" si="1"/>
@@ -5982,16 +5985,16 @@
         <v>350</v>
       </c>
       <c r="D120" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E120" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F120" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="G120" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H120" t="str">
         <f t="shared" si="1"/>
@@ -6012,10 +6015,10 @@
         <v>703</v>
       </c>
       <c r="E121" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G121" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H121" t="str">
         <f t="shared" si="1"/>
@@ -6036,13 +6039,13 @@
         <v>408</v>
       </c>
       <c r="E122" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F122" t="s">
         <v>698</v>
       </c>
       <c r="G122" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H122" t="str">
         <f t="shared" si="1"/>
@@ -6060,16 +6063,16 @@
         <v>359</v>
       </c>
       <c r="D123" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E123" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F123" t="s">
         <v>683</v>
       </c>
       <c r="G123" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H123" t="str">
         <f t="shared" si="1"/>
@@ -6090,10 +6093,10 @@
         <v>728</v>
       </c>
       <c r="E124" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G124" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H124" t="str">
         <f t="shared" si="1"/>
@@ -6111,16 +6114,16 @@
         <v>365</v>
       </c>
       <c r="D125" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E125" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F125" t="s">
         <v>673</v>
       </c>
       <c r="G125" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H125" t="str">
         <f t="shared" si="1"/>
@@ -6138,16 +6141,16 @@
         <v>368</v>
       </c>
       <c r="D126" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E126" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F126" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="G126" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H126" t="str">
         <f t="shared" si="1"/>
@@ -6165,16 +6168,16 @@
         <v>371</v>
       </c>
       <c r="D127" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E127" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F127" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="G127" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H127" t="str">
         <f t="shared" si="1"/>
@@ -6195,10 +6198,10 @@
         <v>728</v>
       </c>
       <c r="E128" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G128" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H128" t="str">
         <f t="shared" si="1"/>
@@ -6219,13 +6222,13 @@
         <v>714</v>
       </c>
       <c r="E129" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F129" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="G129" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H129" t="str">
         <f t="shared" si="1"/>
@@ -6237,22 +6240,22 @@
         <v>378</v>
       </c>
       <c r="B130" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C130" t="s">
         <v>379</v>
       </c>
       <c r="D130" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E130" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F130" t="s">
         <v>698</v>
       </c>
       <c r="G130" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H130" t="str">
         <f t="shared" si="1"/>
@@ -6270,13 +6273,13 @@
         <v>382</v>
       </c>
       <c r="D131" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E131" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G131" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H131" t="str">
         <f t="shared" ref="H131:H194" si="2">IF(NOT(ISBLANK(F131)),"update signs set name_de = """&amp;B131&amp;""", mnemonic = """&amp;C131&amp;""", tag1 ="""&amp;D131&amp;""", tag2 ="""&amp;E131&amp;""", tag3 ="""&amp;F131&amp;""" where name = """&amp;A131&amp;""";","update signs set name_de = """&amp;B131&amp;""", mnemonic = """&amp;C131&amp;""", tag1 ="""&amp;D131&amp;""", tag2 ="""&amp;E131&amp;""" where name = """&amp;A131&amp;""";")</f>
@@ -6297,13 +6300,13 @@
         <v>714</v>
       </c>
       <c r="E132" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F132" t="s">
         <v>698</v>
       </c>
       <c r="G132" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H132" t="str">
         <f t="shared" si="2"/>
@@ -6324,10 +6327,10 @@
         <v>686</v>
       </c>
       <c r="E133" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G133" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H133" t="str">
         <f t="shared" si="2"/>
@@ -6348,13 +6351,13 @@
         <v>689</v>
       </c>
       <c r="E134" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F134" t="s">
         <v>714</v>
       </c>
       <c r="G134" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H134" t="str">
         <f t="shared" si="2"/>
@@ -6375,13 +6378,13 @@
         <v>714</v>
       </c>
       <c r="E135" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F135" t="s">
         <v>289</v>
       </c>
       <c r="G135" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H135" t="str">
         <f t="shared" si="2"/>
@@ -6399,13 +6402,13 @@
         <v>397</v>
       </c>
       <c r="D136" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E136" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G136" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H136" t="str">
         <f t="shared" si="2"/>
@@ -6423,13 +6426,13 @@
         <v>400</v>
       </c>
       <c r="D137" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E137" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G137" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H137" t="str">
         <f t="shared" si="2"/>
@@ -6447,16 +6450,16 @@
         <v>403</v>
       </c>
       <c r="D138" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E138" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F138" t="s">
         <v>677</v>
       </c>
       <c r="G138" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H138" t="str">
         <f t="shared" si="2"/>
@@ -6474,16 +6477,16 @@
         <v>406</v>
       </c>
       <c r="D139" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E139" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F139" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="G139" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H139" t="str">
         <f t="shared" si="2"/>
@@ -6504,13 +6507,13 @@
         <v>714</v>
       </c>
       <c r="E140" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F140" t="s">
         <v>698</v>
       </c>
       <c r="G140" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H140" t="str">
         <f t="shared" si="2"/>
@@ -6531,13 +6534,13 @@
         <v>683</v>
       </c>
       <c r="E141" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F141" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G141" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H141" t="str">
         <f t="shared" si="2"/>
@@ -6555,16 +6558,16 @@
         <v>415</v>
       </c>
       <c r="D142" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E142" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F142" t="s">
         <v>698</v>
       </c>
       <c r="G142" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H142" t="str">
         <f t="shared" si="2"/>
@@ -6582,13 +6585,13 @@
         <v>418</v>
       </c>
       <c r="D143" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E143" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G143" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H143" t="str">
         <f t="shared" si="2"/>
@@ -6609,13 +6612,13 @@
         <v>714</v>
       </c>
       <c r="E144" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F144" t="s">
         <v>698</v>
       </c>
       <c r="G144" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H144" t="str">
         <f t="shared" si="2"/>
@@ -6633,16 +6636,16 @@
         <v>424</v>
       </c>
       <c r="D145" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E145" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F145" t="s">
         <v>677</v>
       </c>
       <c r="G145" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H145" t="str">
         <f t="shared" si="2"/>
@@ -6663,10 +6666,10 @@
         <v>728</v>
       </c>
       <c r="E146" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G146" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H146" t="str">
         <f t="shared" si="2"/>
@@ -6687,10 +6690,10 @@
         <v>289</v>
       </c>
       <c r="E147" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G147" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H147" t="str">
         <f t="shared" si="2"/>
@@ -6711,13 +6714,13 @@
         <v>714</v>
       </c>
       <c r="E148" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F148" t="s">
         <v>698</v>
       </c>
       <c r="G148" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H148" t="str">
         <f t="shared" si="2"/>
@@ -6738,10 +6741,10 @@
         <v>728</v>
       </c>
       <c r="E149" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G149" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H149" t="str">
         <f t="shared" si="2"/>
@@ -6762,10 +6765,10 @@
         <v>408</v>
       </c>
       <c r="E150" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G150" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H150" t="str">
         <f t="shared" si="2"/>
@@ -6786,13 +6789,13 @@
         <v>689</v>
       </c>
       <c r="E151" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F151" t="s">
         <v>289</v>
       </c>
       <c r="G151" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H151" t="str">
         <f t="shared" si="2"/>
@@ -6813,13 +6816,13 @@
         <v>714</v>
       </c>
       <c r="E152" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F152" t="s">
         <v>689</v>
       </c>
       <c r="G152" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H152" t="str">
         <f t="shared" si="2"/>
@@ -6840,13 +6843,13 @@
         <v>683</v>
       </c>
       <c r="E153" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F153" t="s">
         <v>698</v>
       </c>
       <c r="G153" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H153" t="str">
         <f t="shared" si="2"/>
@@ -6864,16 +6867,16 @@
         <v>451</v>
       </c>
       <c r="D154" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E154" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F154" t="s">
         <v>698</v>
       </c>
       <c r="G154" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H154" t="str">
         <f t="shared" si="2"/>
@@ -6891,13 +6894,13 @@
         <v>454</v>
       </c>
       <c r="D155" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E155" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G155" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H155" t="str">
         <f t="shared" si="2"/>
@@ -6918,10 +6921,10 @@
         <v>703</v>
       </c>
       <c r="E156" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G156" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H156" t="str">
         <f t="shared" si="2"/>
@@ -6939,16 +6942,16 @@
         <v>460</v>
       </c>
       <c r="D157" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E157" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F157" t="s">
         <v>698</v>
       </c>
       <c r="G157" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H157" t="str">
         <f t="shared" si="2"/>
@@ -6969,10 +6972,10 @@
         <v>686</v>
       </c>
       <c r="E158" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G158" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H158" t="str">
         <f t="shared" si="2"/>
@@ -6990,16 +6993,16 @@
         <v>466</v>
       </c>
       <c r="D159" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E159" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F159" t="s">
         <v>677</v>
       </c>
       <c r="G159" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H159" t="str">
         <f t="shared" si="2"/>
@@ -7020,13 +7023,13 @@
         <v>289</v>
       </c>
       <c r="E160" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F160" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="G160" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H160" t="str">
         <f t="shared" si="2"/>
@@ -7047,13 +7050,13 @@
         <v>689</v>
       </c>
       <c r="E161" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F161" t="s">
         <v>698</v>
       </c>
       <c r="G161" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H161" t="str">
         <f t="shared" si="2"/>
@@ -7071,16 +7074,16 @@
         <v>475</v>
       </c>
       <c r="D162" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E162" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F162" t="s">
         <v>677</v>
       </c>
       <c r="G162" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H162" t="str">
         <f t="shared" si="2"/>
@@ -7092,7 +7095,7 @@
         <v>476</v>
       </c>
       <c r="B163" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C163" t="s">
         <v>477</v>
@@ -7101,13 +7104,13 @@
         <v>683</v>
       </c>
       <c r="E163" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F163" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G163" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H163" t="str">
         <f t="shared" si="2"/>
@@ -7125,16 +7128,16 @@
         <v>480</v>
       </c>
       <c r="D164" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E164" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F164" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="G164" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H164" t="str">
         <f t="shared" si="2"/>
@@ -7155,13 +7158,13 @@
         <v>722</v>
       </c>
       <c r="E165" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F165" t="s">
         <v>698</v>
       </c>
       <c r="G165" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H165" t="str">
         <f t="shared" si="2"/>
@@ -7182,13 +7185,13 @@
         <v>722</v>
       </c>
       <c r="E166" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F166" t="s">
         <v>698</v>
       </c>
       <c r="G166" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H166" t="str">
         <f t="shared" si="2"/>
@@ -7209,13 +7212,13 @@
         <v>683</v>
       </c>
       <c r="E167" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F167" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G167" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H167" t="str">
         <f t="shared" si="2"/>
@@ -7236,10 +7239,10 @@
         <v>728</v>
       </c>
       <c r="E168" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G168" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H168" t="str">
         <f t="shared" si="2"/>
@@ -7260,13 +7263,13 @@
         <v>714</v>
       </c>
       <c r="E169" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F169" t="s">
         <v>698</v>
       </c>
       <c r="G169" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H169" t="str">
         <f t="shared" si="2"/>
@@ -7278,7 +7281,7 @@
         <v>496</v>
       </c>
       <c r="B170" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C170" t="s">
         <v>497</v>
@@ -7287,13 +7290,13 @@
         <v>677</v>
       </c>
       <c r="E170" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F170" t="s">
         <v>698</v>
       </c>
       <c r="G170" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H170" t="str">
         <f t="shared" si="2"/>
@@ -7305,7 +7308,7 @@
         <v>498</v>
       </c>
       <c r="B171" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C171" t="s">
         <v>499</v>
@@ -7314,13 +7317,13 @@
         <v>677</v>
       </c>
       <c r="E171" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F171" t="s">
         <v>698</v>
       </c>
       <c r="G171" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H171" t="str">
         <f t="shared" si="2"/>
@@ -7341,10 +7344,10 @@
         <v>289</v>
       </c>
       <c r="E172" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G172" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H172" t="str">
         <f t="shared" si="2"/>
@@ -7365,13 +7368,13 @@
         <v>728</v>
       </c>
       <c r="E173" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F173" t="s">
         <v>199</v>
       </c>
       <c r="G173" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H173" t="str">
         <f t="shared" si="2"/>
@@ -7392,13 +7395,13 @@
         <v>683</v>
       </c>
       <c r="E174" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F174" t="s">
         <v>722</v>
       </c>
       <c r="G174" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H174" t="str">
         <f t="shared" si="2"/>
@@ -7419,10 +7422,10 @@
         <v>683</v>
       </c>
       <c r="E175" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G175" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H175" t="str">
         <f t="shared" si="2"/>
@@ -7443,13 +7446,13 @@
         <v>683</v>
       </c>
       <c r="E176" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F176" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G176" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H176" t="str">
         <f t="shared" si="2"/>
@@ -7470,13 +7473,13 @@
         <v>689</v>
       </c>
       <c r="E177" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F177" t="s">
         <v>698</v>
       </c>
       <c r="G177" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H177" t="str">
         <f t="shared" si="2"/>
@@ -7497,13 +7500,13 @@
         <v>408</v>
       </c>
       <c r="E178" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F178" t="s">
         <v>698</v>
       </c>
       <c r="G178" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H178" t="str">
         <f t="shared" si="2"/>
@@ -7521,16 +7524,16 @@
         <v>523</v>
       </c>
       <c r="D179" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E179" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F179" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="G179" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H179" t="str">
         <f t="shared" si="2"/>
@@ -7551,10 +7554,10 @@
         <v>673</v>
       </c>
       <c r="E180" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G180" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H180" t="str">
         <f t="shared" si="2"/>
@@ -7572,16 +7575,16 @@
         <v>529</v>
       </c>
       <c r="D181" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E181" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F181" t="s">
         <v>722</v>
       </c>
       <c r="G181" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H181" t="str">
         <f t="shared" si="2"/>
@@ -7602,10 +7605,10 @@
         <v>728</v>
       </c>
       <c r="E182" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G182" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H182" t="str">
         <f t="shared" si="2"/>
@@ -7626,10 +7629,10 @@
         <v>673</v>
       </c>
       <c r="E183" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G183" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H183" t="str">
         <f t="shared" si="2"/>
@@ -7647,13 +7650,13 @@
         <v>538</v>
       </c>
       <c r="D184" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E184" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G184" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H184" t="str">
         <f t="shared" si="2"/>
@@ -7674,10 +7677,10 @@
         <v>408</v>
       </c>
       <c r="E185" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G185" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H185" t="str">
         <f t="shared" si="2"/>
@@ -7698,13 +7701,13 @@
         <v>703</v>
       </c>
       <c r="E186" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F186" t="s">
         <v>408</v>
       </c>
       <c r="G186" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H186" t="str">
         <f t="shared" si="2"/>
@@ -7722,16 +7725,16 @@
         <v>547</v>
       </c>
       <c r="D187" t="s">
+        <v>806</v>
+      </c>
+      <c r="E187" t="s">
+        <v>791</v>
+      </c>
+      <c r="F187" t="s">
         <v>807</v>
       </c>
-      <c r="E187" t="s">
-        <v>792</v>
-      </c>
-      <c r="F187" t="s">
-        <v>808</v>
-      </c>
       <c r="G187" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H187" t="str">
         <f t="shared" si="2"/>
@@ -7752,13 +7755,13 @@
         <v>722</v>
       </c>
       <c r="E188" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F188" t="s">
         <v>698</v>
       </c>
       <c r="G188" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H188" t="str">
         <f t="shared" si="2"/>
@@ -7779,13 +7782,13 @@
         <v>289</v>
       </c>
       <c r="E189" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F189" t="s">
         <v>714</v>
       </c>
       <c r="G189" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H189" t="str">
         <f t="shared" si="2"/>
@@ -7803,16 +7806,16 @@
         <v>556</v>
       </c>
       <c r="D190" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E190" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F190" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="G190" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H190" t="str">
         <f t="shared" si="2"/>
@@ -7830,13 +7833,13 @@
         <v>559</v>
       </c>
       <c r="D191" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E191" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G191" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H191" t="str">
         <f t="shared" si="2"/>
@@ -7857,13 +7860,13 @@
         <v>677</v>
       </c>
       <c r="E192" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F192" t="s">
         <v>698</v>
       </c>
       <c r="G192" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H192" t="str">
         <f t="shared" si="2"/>
@@ -7884,13 +7887,13 @@
         <v>722</v>
       </c>
       <c r="E193" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F193" t="s">
         <v>698</v>
       </c>
       <c r="G193" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H193" t="str">
         <f t="shared" si="2"/>
@@ -7908,13 +7911,13 @@
         <v>568</v>
       </c>
       <c r="D194" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E194" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G194" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H194" t="str">
         <f t="shared" si="2"/>
@@ -7935,13 +7938,13 @@
         <v>728</v>
       </c>
       <c r="E195" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F195" t="s">
         <v>199</v>
       </c>
       <c r="G195" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H195" t="str">
         <f t="shared" ref="H195:H211" si="3">IF(NOT(ISBLANK(F195)),"update signs set name_de = """&amp;B195&amp;""", mnemonic = """&amp;C195&amp;""", tag1 ="""&amp;D195&amp;""", tag2 ="""&amp;E195&amp;""", tag3 ="""&amp;F195&amp;""" where name = """&amp;A195&amp;""";","update signs set name_de = """&amp;B195&amp;""", mnemonic = """&amp;C195&amp;""", tag1 ="""&amp;D195&amp;""", tag2 ="""&amp;E195&amp;""" where name = """&amp;A195&amp;""";")</f>
@@ -7959,16 +7962,16 @@
         <v>574</v>
       </c>
       <c r="D196" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E196" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F196" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G196" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H196" t="str">
         <f t="shared" si="3"/>
@@ -7989,10 +7992,10 @@
         <v>774</v>
       </c>
       <c r="E197" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G197" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H197" t="str">
         <f t="shared" si="3"/>
@@ -8013,10 +8016,10 @@
         <v>774</v>
       </c>
       <c r="E198" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G198" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H198" t="str">
         <f t="shared" si="3"/>
@@ -8037,10 +8040,10 @@
         <v>774</v>
       </c>
       <c r="E199" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G199" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H199" t="str">
         <f t="shared" si="3"/>
@@ -8061,10 +8064,10 @@
         <v>774</v>
       </c>
       <c r="E200" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G200" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H200" t="str">
         <f t="shared" si="3"/>
@@ -8085,10 +8088,10 @@
         <v>289</v>
       </c>
       <c r="E201" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G201" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H201" t="str">
         <f t="shared" si="3"/>
@@ -8106,13 +8109,13 @@
         <v>592</v>
       </c>
       <c r="D202" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E202" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G202" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H202" t="str">
         <f t="shared" si="3"/>
@@ -8133,10 +8136,10 @@
         <v>686</v>
       </c>
       <c r="E203" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G203" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H203" t="str">
         <f t="shared" si="3"/>
@@ -8157,13 +8160,13 @@
         <v>689</v>
       </c>
       <c r="E204" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F204" t="s">
         <v>698</v>
       </c>
       <c r="G204" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H204" t="str">
         <f t="shared" si="3"/>
@@ -8181,16 +8184,16 @@
         <v>601</v>
       </c>
       <c r="D205" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E205" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F205" t="s">
         <v>677</v>
       </c>
       <c r="G205" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H205" t="str">
         <f t="shared" si="3"/>
@@ -8211,13 +8214,13 @@
         <v>683</v>
       </c>
       <c r="E206" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F206" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G206" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H206" t="str">
         <f t="shared" si="3"/>
@@ -8238,10 +8241,10 @@
         <v>673</v>
       </c>
       <c r="E207" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G207" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H207" t="str">
         <f t="shared" si="3"/>
@@ -8262,10 +8265,10 @@
         <v>728</v>
       </c>
       <c r="E208" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G208" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H208" t="str">
         <f t="shared" si="3"/>
@@ -8286,13 +8289,13 @@
         <v>686</v>
       </c>
       <c r="E209" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F209" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G209" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H209" t="str">
         <f t="shared" si="3"/>
@@ -8304,7 +8307,7 @@
         <v>614</v>
       </c>
       <c r="B210" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C210" t="s">
         <v>278</v>
@@ -8313,13 +8316,13 @@
         <v>683</v>
       </c>
       <c r="E210" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F210" t="s">
         <v>698</v>
       </c>
       <c r="G210" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H210" t="str">
         <f t="shared" si="3"/>
@@ -8337,13 +8340,13 @@
         <v>617</v>
       </c>
       <c r="D211" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E211" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G211" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H211" t="str">
         <f t="shared" si="3"/>
@@ -8430,7 +8433,7 @@
         <v>674</v>
       </c>
       <c r="F215" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="H215" t="str">
         <f t="shared" si="4"/>
@@ -8532,7 +8535,7 @@
         <v>625</v>
       </c>
       <c r="C220" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D220" t="s">
         <v>694</v>
@@ -8736,7 +8739,7 @@
         <v>717</v>
       </c>
       <c r="D229" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E229" t="s">
         <v>674</v>
@@ -8796,7 +8799,7 @@
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>611</v>
+        <v>833</v>
       </c>
       <c r="B232" t="s">
         <v>634</v>
@@ -8811,11 +8814,11 @@
         <v>674</v>
       </c>
       <c r="F232" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="H232" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("you","ihr","in Bogen auf die anderen zeigen","Person","Zusatz","Kleine Worte");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("you_plural","ihr","in Bogen auf die anderen zeigen","Person","Zusatz","Kleine Worte");</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.35">
@@ -8829,7 +8832,7 @@
         <v>725</v>
       </c>
       <c r="D233" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E233" t="s">
         <v>674</v>
@@ -9054,7 +9057,7 @@
         <v>747</v>
       </c>
       <c r="D243" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E243" t="s">
         <v>674</v>
@@ -9078,7 +9081,7 @@
         <v>749</v>
       </c>
       <c r="D244" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E244" t="s">
         <v>674</v>
@@ -9168,7 +9171,7 @@
         <v>757</v>
       </c>
       <c r="D248" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E248" t="s">
         <v>674</v>
@@ -9327,7 +9330,7 @@
         <v>771</v>
       </c>
       <c r="D255" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E255" t="s">
         <v>674</v>
@@ -9525,10 +9528,10 @@
         <v>665</v>
       </c>
       <c r="C264" t="s">
-        <v>791</v>
+        <v>834</v>
       </c>
       <c r="D264" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E264" t="s">
         <v>674</v>
@@ -9538,7 +9541,7 @@
       </c>
       <c r="H264" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("together","zusammen","von außen mit ffenen Handflächen alles zusammenballen","Kleine Worte","Zusatz","Eigenschaften");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("together","zusammen","von außen mit offenen Handflächen alles zusammenballen","Kleine Worte","Zusatz","Eigenschaften");</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#97 Adding 53 new videos to the app. Migrating the database by using signs.db_upgrade_1-2.sql and increasing the database version in DbContract. The sql files can be found in VideosUkGebärden.xlsx
</commit_message>
<xml_diff>
--- a/database/VideosUkGebärden.xlsx
+++ b/database/VideosUkGebärden.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User-Matthias\Dev\Android\UKGM\src\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\UK-Gebaerden_Muensterland\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AAD3F4-CD2E-46CD-A4F8-43F0DF123D82}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496AF1F0-6E7B-4DBF-9B56-6E7F6623C283}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{978A20FD-486C-4CB5-9933-67C562CBE71F}"/>
   </bookViews>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2309,9 +2311,6 @@
     <t>Zeige-und Mittelfinger 3x an Wange  klopfen</t>
   </si>
   <si>
-    <t>new</t>
-  </si>
-  <si>
     <t>dominante Hand schiebt sich langsam hinter anderer Hand hervor: 'neu erscheinen'</t>
   </si>
   <si>
@@ -2574,6 +2573,9 @@
   </si>
   <si>
     <t>von außen mit offenen Handflächen alles zusammenballen</t>
+  </si>
+  <si>
+    <t>brand_new</t>
   </si>
 </sst>
 </file>
@@ -2966,8 +2968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C22E1E0-4D2F-4ED8-9423-514FCF041C4D}">
   <dimension ref="A1:H264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C249" workbookViewId="0">
-      <selection activeCell="C265" sqref="C265"/>
+    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
+      <selection activeCell="A244" sqref="A244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2980,28 +2982,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>818</v>
+      </c>
+      <c r="B1" t="s">
         <v>819</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>820</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>821</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>822</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>823</v>
       </c>
-      <c r="F1" t="s">
-        <v>824</v>
-      </c>
       <c r="G1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="H1" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -3018,10 +3020,10 @@
         <v>673</v>
       </c>
       <c r="E2" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H2" t="str">
         <f>IF(NOT(ISBLANK(F2)),"update signs set name_de = """&amp;B2&amp;""", mnemonic = """&amp;C2&amp;""", tag1 ="""&amp;D2&amp;""", tag2 ="""&amp;E2&amp;""", tag3 ="""&amp;F2&amp;""" where name = """&amp;A2&amp;""";","update signs set name_de = """&amp;B2&amp;""", mnemonic = """&amp;C2&amp;""", tag1 ="""&amp;D2&amp;""", tag2 ="""&amp;E2&amp;""" where name = """&amp;A2&amp;""";")</f>
@@ -3039,13 +3041,13 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E3" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H66" si="0">IF(NOT(ISBLANK(F3)),"update signs set name_de = """&amp;B3&amp;""", mnemonic = """&amp;C3&amp;""", tag1 ="""&amp;D3&amp;""", tag2 ="""&amp;E3&amp;""", tag3 ="""&amp;F3&amp;""" where name = """&amp;A3&amp;""";","update signs set name_de = """&amp;B3&amp;""", mnemonic = """&amp;C3&amp;""", tag1 ="""&amp;D3&amp;""", tag2 ="""&amp;E3&amp;""" where name = """&amp;A3&amp;""";")</f>
@@ -3066,10 +3068,10 @@
         <v>703</v>
       </c>
       <c r="E4" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G4" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -3087,13 +3089,13 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E5" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G5" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -3111,13 +3113,13 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E6" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G6" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -3138,10 +3140,10 @@
         <v>683</v>
       </c>
       <c r="E7" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G7" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -3162,10 +3164,10 @@
         <v>728</v>
       </c>
       <c r="E8" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G8" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -3177,7 +3179,7 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
@@ -3186,10 +3188,10 @@
         <v>683</v>
       </c>
       <c r="E9" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G9" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -3207,16 +3209,16 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E10" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F10" t="s">
         <v>683</v>
       </c>
       <c r="G10" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -3237,10 +3239,10 @@
         <v>686</v>
       </c>
       <c r="E11" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G11" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -3261,10 +3263,10 @@
         <v>677</v>
       </c>
       <c r="E12" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G12" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -3282,13 +3284,13 @@
         <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E13" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G13" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -3306,16 +3308,16 @@
         <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E14" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F14" t="s">
         <v>698</v>
       </c>
       <c r="G14" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -3336,10 +3338,10 @@
         <v>408</v>
       </c>
       <c r="E15" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G15" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -3360,10 +3362,10 @@
         <v>728</v>
       </c>
       <c r="E16" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G16" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -3381,16 +3383,16 @@
         <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E17" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F17" t="s">
         <v>698</v>
       </c>
       <c r="G17" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -3411,10 +3413,10 @@
         <v>289</v>
       </c>
       <c r="E18" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G18" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -3435,10 +3437,10 @@
         <v>289</v>
       </c>
       <c r="E19" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G19" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -3459,13 +3461,13 @@
         <v>673</v>
       </c>
       <c r="E20" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F20" t="s">
         <v>673</v>
       </c>
       <c r="G20" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -3486,13 +3488,13 @@
         <v>689</v>
       </c>
       <c r="E21" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F21" t="s">
         <v>698</v>
       </c>
       <c r="G21" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -3510,16 +3512,16 @@
         <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E22" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F22" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="G22" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -3540,10 +3542,10 @@
         <v>677</v>
       </c>
       <c r="E23" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G23" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -3564,10 +3566,10 @@
         <v>703</v>
       </c>
       <c r="E24" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G24" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
@@ -3585,13 +3587,13 @@
         <v>70</v>
       </c>
       <c r="D25" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E25" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G25" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
@@ -3603,19 +3605,19 @@
         <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C26" t="s">
         <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E26" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G26" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
@@ -3633,16 +3635,16 @@
         <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E27" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F27" t="s">
         <v>677</v>
       </c>
       <c r="G27" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
@@ -3663,13 +3665,13 @@
         <v>408</v>
       </c>
       <c r="E28" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F28" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="G28" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
@@ -3690,10 +3692,10 @@
         <v>686</v>
       </c>
       <c r="E29" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G29" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
@@ -3714,10 +3716,10 @@
         <v>728</v>
       </c>
       <c r="E30" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G30" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
@@ -3738,10 +3740,10 @@
         <v>677</v>
       </c>
       <c r="E31" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G31" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
@@ -3759,13 +3761,13 @@
         <v>90</v>
       </c>
       <c r="D32" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E32" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G32" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
@@ -3783,13 +3785,13 @@
         <v>93</v>
       </c>
       <c r="D33" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E33" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G33" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
@@ -3807,13 +3809,13 @@
         <v>96</v>
       </c>
       <c r="D34" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E34" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G34" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="0"/>
@@ -3834,10 +3836,10 @@
         <v>408</v>
       </c>
       <c r="E35" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G35" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="0"/>
@@ -3858,10 +3860,10 @@
         <v>703</v>
       </c>
       <c r="E36" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G36" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="0"/>
@@ -3882,10 +3884,10 @@
         <v>728</v>
       </c>
       <c r="E37" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G37" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="0"/>
@@ -3903,13 +3905,13 @@
         <v>108</v>
       </c>
       <c r="D38" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E38" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G38" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="0"/>
@@ -3930,13 +3932,13 @@
         <v>728</v>
       </c>
       <c r="E39" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F39" t="s">
         <v>199</v>
       </c>
       <c r="G39" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="0"/>
@@ -3957,10 +3959,10 @@
         <v>728</v>
       </c>
       <c r="E40" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G40" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="0"/>
@@ -3981,10 +3983,10 @@
         <v>703</v>
       </c>
       <c r="E41" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G41" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="0"/>
@@ -4005,10 +4007,10 @@
         <v>683</v>
       </c>
       <c r="E42" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G42" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="0"/>
@@ -4029,10 +4031,10 @@
         <v>728</v>
       </c>
       <c r="E43" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G43" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="0"/>
@@ -4050,13 +4052,13 @@
         <v>126</v>
       </c>
       <c r="D44" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E44" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G44" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
@@ -4077,10 +4079,10 @@
         <v>289</v>
       </c>
       <c r="E45" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G45" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="0"/>
@@ -4098,13 +4100,13 @@
         <v>132</v>
       </c>
       <c r="D46" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E46" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G46" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
@@ -4125,10 +4127,10 @@
         <v>686</v>
       </c>
       <c r="E47" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G47" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
@@ -4149,10 +4151,10 @@
         <v>728</v>
       </c>
       <c r="E48" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G48" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
@@ -4173,10 +4175,10 @@
         <v>677</v>
       </c>
       <c r="E49" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G49" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
@@ -4197,13 +4199,13 @@
         <v>714</v>
       </c>
       <c r="E50" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F50" t="s">
         <v>698</v>
       </c>
       <c r="G50" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
@@ -4224,13 +4226,13 @@
         <v>289</v>
       </c>
       <c r="E51" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F51" t="s">
         <v>698</v>
       </c>
       <c r="G51" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
@@ -4251,10 +4253,10 @@
         <v>728</v>
       </c>
       <c r="E52" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G52" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
@@ -4275,10 +4277,10 @@
         <v>677</v>
       </c>
       <c r="E53" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G53" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="0"/>
@@ -4299,13 +4301,13 @@
         <v>683</v>
       </c>
       <c r="E54" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F54" t="s">
         <v>698</v>
       </c>
       <c r="G54" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="0"/>
@@ -4326,10 +4328,10 @@
         <v>728</v>
       </c>
       <c r="E55" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G55" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
@@ -4347,16 +4349,16 @@
         <v>161</v>
       </c>
       <c r="D56" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E56" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F56" t="s">
         <v>698</v>
       </c>
       <c r="G56" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="0"/>
@@ -4374,13 +4376,13 @@
         <v>164</v>
       </c>
       <c r="D57" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E57" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G57" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="0"/>
@@ -4401,10 +4403,10 @@
         <v>728</v>
       </c>
       <c r="E58" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G58" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="0"/>
@@ -4425,10 +4427,10 @@
         <v>289</v>
       </c>
       <c r="E59" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G59" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H59" t="str">
         <f t="shared" si="0"/>
@@ -4446,13 +4448,13 @@
         <v>173</v>
       </c>
       <c r="D60" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E60" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G60" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" si="0"/>
@@ -4470,13 +4472,13 @@
         <v>176</v>
       </c>
       <c r="D61" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E61" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G61" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H61" t="str">
         <f t="shared" si="0"/>
@@ -4494,16 +4496,16 @@
         <v>179</v>
       </c>
       <c r="D62" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E62" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F62" t="s">
         <v>677</v>
       </c>
       <c r="G62" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="0"/>
@@ -4524,10 +4526,10 @@
         <v>686</v>
       </c>
       <c r="E63" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G63" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H63" t="str">
         <f t="shared" si="0"/>
@@ -4545,13 +4547,13 @@
         <v>185</v>
       </c>
       <c r="D64" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E64" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G64" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="0"/>
@@ -4572,10 +4574,10 @@
         <v>408</v>
       </c>
       <c r="E65" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G65" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H65" t="str">
         <f t="shared" si="0"/>
@@ -4596,13 +4598,13 @@
         <v>677</v>
       </c>
       <c r="E66" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F66" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="G66" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H66" t="str">
         <f t="shared" si="0"/>
@@ -4623,10 +4625,10 @@
         <v>289</v>
       </c>
       <c r="E67" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G67" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H67" t="str">
         <f t="shared" ref="H67:H130" si="1">IF(NOT(ISBLANK(F67)),"update signs set name_de = """&amp;B67&amp;""", mnemonic = """&amp;C67&amp;""", tag1 ="""&amp;D67&amp;""", tag2 ="""&amp;E67&amp;""", tag3 ="""&amp;F67&amp;""" where name = """&amp;A67&amp;""";","update signs set name_de = """&amp;B67&amp;""", mnemonic = """&amp;C67&amp;""", tag1 ="""&amp;D67&amp;""", tag2 ="""&amp;E67&amp;""" where name = """&amp;A67&amp;""";")</f>
@@ -4644,16 +4646,16 @@
         <v>197</v>
       </c>
       <c r="D68" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E68" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F68" t="s">
         <v>677</v>
       </c>
       <c r="G68" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H68" t="str">
         <f t="shared" si="1"/>
@@ -4674,13 +4676,13 @@
         <v>728</v>
       </c>
       <c r="E69" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F69" t="s">
         <v>199</v>
       </c>
       <c r="G69" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H69" t="str">
         <f t="shared" si="1"/>
@@ -4698,16 +4700,16 @@
         <v>203</v>
       </c>
       <c r="D70" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E70" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F70" t="s">
         <v>698</v>
       </c>
       <c r="G70" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H70" t="str">
         <f t="shared" si="1"/>
@@ -4725,13 +4727,13 @@
         <v>206</v>
       </c>
       <c r="D71" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E71" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G71" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H71" t="str">
         <f t="shared" si="1"/>
@@ -4749,16 +4751,16 @@
         <v>209</v>
       </c>
       <c r="D72" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E72" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F72" t="s">
         <v>698</v>
       </c>
       <c r="G72" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H72" t="str">
         <f t="shared" si="1"/>
@@ -4779,10 +4781,10 @@
         <v>728</v>
       </c>
       <c r="E73" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G73" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H73" t="str">
         <f t="shared" si="1"/>
@@ -4800,16 +4802,16 @@
         <v>215</v>
       </c>
       <c r="D74" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E74" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F74" t="s">
         <v>677</v>
       </c>
       <c r="G74" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H74" t="str">
         <f t="shared" si="1"/>
@@ -4830,13 +4832,13 @@
         <v>714</v>
       </c>
       <c r="E75" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F75" t="s">
         <v>698</v>
       </c>
       <c r="G75" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H75" t="str">
         <f t="shared" si="1"/>
@@ -4854,16 +4856,16 @@
         <v>221</v>
       </c>
       <c r="D76" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E76" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F76" t="s">
         <v>673</v>
       </c>
       <c r="G76" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H76" t="str">
         <f t="shared" si="1"/>
@@ -4881,13 +4883,13 @@
         <v>224</v>
       </c>
       <c r="D77" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E77" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G77" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H77" t="str">
         <f t="shared" si="1"/>
@@ -4905,16 +4907,16 @@
         <v>227</v>
       </c>
       <c r="D78" t="s">
+        <v>805</v>
+      </c>
+      <c r="E78" t="s">
+        <v>790</v>
+      </c>
+      <c r="F78" t="s">
         <v>806</v>
       </c>
-      <c r="E78" t="s">
-        <v>791</v>
-      </c>
-      <c r="F78" t="s">
-        <v>807</v>
-      </c>
       <c r="G78" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H78" t="str">
         <f t="shared" si="1"/>
@@ -4935,13 +4937,13 @@
         <v>683</v>
       </c>
       <c r="E79" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F79" t="s">
         <v>677</v>
       </c>
       <c r="G79" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H79" t="str">
         <f t="shared" si="1"/>
@@ -4953,7 +4955,7 @@
         <v>231</v>
       </c>
       <c r="B80" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C80" t="s">
         <v>232</v>
@@ -4962,13 +4964,13 @@
         <v>714</v>
       </c>
       <c r="E80" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F80" t="s">
         <v>698</v>
       </c>
       <c r="G80" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H80" t="str">
         <f t="shared" si="1"/>
@@ -4986,13 +4988,13 @@
         <v>235</v>
       </c>
       <c r="D81" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E81" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G81" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H81" t="str">
         <f t="shared" si="1"/>
@@ -5013,10 +5015,10 @@
         <v>686</v>
       </c>
       <c r="E82" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G82" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H82" t="str">
         <f t="shared" si="1"/>
@@ -5034,16 +5036,16 @@
         <v>241</v>
       </c>
       <c r="D83" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E83" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F83" t="s">
         <v>677</v>
       </c>
       <c r="G83" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H83" t="str">
         <f t="shared" si="1"/>
@@ -5064,13 +5066,13 @@
         <v>683</v>
       </c>
       <c r="E84" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F84" t="s">
         <v>714</v>
       </c>
       <c r="G84" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H84" t="str">
         <f t="shared" si="1"/>
@@ -5091,10 +5093,10 @@
         <v>686</v>
       </c>
       <c r="E85" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G85" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H85" t="str">
         <f t="shared" si="1"/>
@@ -5115,13 +5117,13 @@
         <v>683</v>
       </c>
       <c r="E86" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F86" t="s">
         <v>698</v>
       </c>
       <c r="G86" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H86" t="str">
         <f t="shared" si="1"/>
@@ -5139,13 +5141,13 @@
         <v>253</v>
       </c>
       <c r="D87" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E87" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G87" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H87" t="str">
         <f t="shared" si="1"/>
@@ -5157,22 +5159,22 @@
         <v>254</v>
       </c>
       <c r="B88" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C88" t="s">
         <v>255</v>
       </c>
       <c r="D88" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E88" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F88" t="s">
         <v>677</v>
       </c>
       <c r="G88" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H88" t="str">
         <f t="shared" si="1"/>
@@ -5184,7 +5186,7 @@
         <v>256</v>
       </c>
       <c r="B89" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C89" t="s">
         <v>257</v>
@@ -5193,10 +5195,10 @@
         <v>683</v>
       </c>
       <c r="E89" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G89" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H89" t="str">
         <f t="shared" si="1"/>
@@ -5214,13 +5216,13 @@
         <v>260</v>
       </c>
       <c r="D90" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E90" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G90" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H90" t="str">
         <f t="shared" si="1"/>
@@ -5238,16 +5240,16 @@
         <v>263</v>
       </c>
       <c r="D91" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E91" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F91" t="s">
         <v>677</v>
       </c>
       <c r="G91" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H91" t="str">
         <f t="shared" si="1"/>
@@ -5268,10 +5270,10 @@
         <v>686</v>
       </c>
       <c r="E92" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G92" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H92" t="str">
         <f t="shared" si="1"/>
@@ -5292,10 +5294,10 @@
         <v>686</v>
       </c>
       <c r="E93" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G93" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H93" t="str">
         <f t="shared" si="1"/>
@@ -5313,16 +5315,16 @@
         <v>272</v>
       </c>
       <c r="D94" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E94" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F94" t="s">
         <v>677</v>
       </c>
       <c r="G94" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H94" t="str">
         <f t="shared" si="1"/>
@@ -5343,13 +5345,13 @@
         <v>683</v>
       </c>
       <c r="E95" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F95" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="G95" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H95" t="str">
         <f t="shared" si="1"/>
@@ -5370,13 +5372,13 @@
         <v>683</v>
       </c>
       <c r="E96" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F96" t="s">
         <v>698</v>
       </c>
       <c r="G96" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H96" t="str">
         <f t="shared" si="1"/>
@@ -5394,13 +5396,13 @@
         <v>281</v>
       </c>
       <c r="D97" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E97" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G97" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H97" t="str">
         <f t="shared" si="1"/>
@@ -5418,13 +5420,13 @@
         <v>284</v>
       </c>
       <c r="D98" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E98" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G98" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H98" t="str">
         <f t="shared" si="1"/>
@@ -5442,16 +5444,16 @@
         <v>287</v>
       </c>
       <c r="D99" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E99" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F99" t="s">
         <v>677</v>
       </c>
       <c r="G99" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H99" t="str">
         <f t="shared" si="1"/>
@@ -5472,10 +5474,10 @@
         <v>289</v>
       </c>
       <c r="E100" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G100" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H100" t="str">
         <f t="shared" si="1"/>
@@ -5496,10 +5498,10 @@
         <v>686</v>
       </c>
       <c r="E101" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G101" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H101" t="str">
         <f t="shared" si="1"/>
@@ -5520,10 +5522,10 @@
         <v>728</v>
       </c>
       <c r="E102" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G102" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H102" t="str">
         <f t="shared" si="1"/>
@@ -5541,16 +5543,16 @@
         <v>299</v>
       </c>
       <c r="D103" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E103" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F103" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="G103" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H103" t="str">
         <f t="shared" si="1"/>
@@ -5568,16 +5570,16 @@
         <v>302</v>
       </c>
       <c r="D104" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E104" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F104" t="s">
         <v>686</v>
       </c>
       <c r="G104" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H104" t="str">
         <f t="shared" si="1"/>
@@ -5598,13 +5600,13 @@
         <v>728</v>
       </c>
       <c r="E105" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F105" t="s">
         <v>199</v>
       </c>
       <c r="G105" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H105" t="str">
         <f t="shared" si="1"/>
@@ -5625,13 +5627,13 @@
         <v>714</v>
       </c>
       <c r="E106" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F106" t="s">
         <v>698</v>
       </c>
       <c r="G106" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H106" t="str">
         <f t="shared" si="1"/>
@@ -5652,13 +5654,13 @@
         <v>289</v>
       </c>
       <c r="E107" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F107" t="s">
         <v>408</v>
       </c>
       <c r="G107" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H107" t="str">
         <f t="shared" si="1"/>
@@ -5679,10 +5681,10 @@
         <v>289</v>
       </c>
       <c r="E108" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G108" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H108" t="str">
         <f t="shared" si="1"/>
@@ -5700,16 +5702,16 @@
         <v>317</v>
       </c>
       <c r="D109" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E109" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F109" t="s">
         <v>698</v>
       </c>
       <c r="G109" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H109" t="str">
         <f t="shared" si="1"/>
@@ -5730,10 +5732,10 @@
         <v>289</v>
       </c>
       <c r="E110" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G110" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H110" t="str">
         <f t="shared" si="1"/>
@@ -5751,16 +5753,16 @@
         <v>323</v>
       </c>
       <c r="D111" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E111" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F111" t="s">
         <v>673</v>
       </c>
       <c r="G111" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H111" t="str">
         <f t="shared" si="1"/>
@@ -5781,13 +5783,13 @@
         <v>683</v>
       </c>
       <c r="E112" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F112" t="s">
         <v>698</v>
       </c>
       <c r="G112" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H112" t="str">
         <f t="shared" si="1"/>
@@ -5808,13 +5810,13 @@
         <v>683</v>
       </c>
       <c r="E113" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F113" t="s">
         <v>698</v>
       </c>
       <c r="G113" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H113" t="str">
         <f t="shared" si="1"/>
@@ -5835,13 +5837,13 @@
         <v>689</v>
       </c>
       <c r="E114" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F114" t="s">
         <v>698</v>
       </c>
       <c r="G114" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H114" t="str">
         <f t="shared" si="1"/>
@@ -5862,10 +5864,10 @@
         <v>686</v>
       </c>
       <c r="E115" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G115" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H115" t="str">
         <f t="shared" si="1"/>
@@ -5886,10 +5888,10 @@
         <v>686</v>
       </c>
       <c r="E116" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G116" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H116" t="str">
         <f t="shared" si="1"/>
@@ -5907,16 +5909,16 @@
         <v>341</v>
       </c>
       <c r="D117" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E117" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F117" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="G117" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H117" t="str">
         <f t="shared" si="1"/>
@@ -5937,10 +5939,10 @@
         <v>728</v>
       </c>
       <c r="E118" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G118" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H118" t="str">
         <f t="shared" si="1"/>
@@ -5961,13 +5963,13 @@
         <v>728</v>
       </c>
       <c r="E119" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F119" t="s">
         <v>199</v>
       </c>
       <c r="G119" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H119" t="str">
         <f t="shared" si="1"/>
@@ -5985,16 +5987,16 @@
         <v>350</v>
       </c>
       <c r="D120" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E120" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F120" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="G120" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H120" t="str">
         <f t="shared" si="1"/>
@@ -6015,10 +6017,10 @@
         <v>703</v>
       </c>
       <c r="E121" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G121" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H121" t="str">
         <f t="shared" si="1"/>
@@ -6039,13 +6041,13 @@
         <v>408</v>
       </c>
       <c r="E122" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F122" t="s">
         <v>698</v>
       </c>
       <c r="G122" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H122" t="str">
         <f t="shared" si="1"/>
@@ -6063,16 +6065,16 @@
         <v>359</v>
       </c>
       <c r="D123" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E123" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F123" t="s">
         <v>683</v>
       </c>
       <c r="G123" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H123" t="str">
         <f t="shared" si="1"/>
@@ -6093,10 +6095,10 @@
         <v>728</v>
       </c>
       <c r="E124" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G124" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H124" t="str">
         <f t="shared" si="1"/>
@@ -6114,16 +6116,16 @@
         <v>365</v>
       </c>
       <c r="D125" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E125" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F125" t="s">
         <v>673</v>
       </c>
       <c r="G125" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H125" t="str">
         <f t="shared" si="1"/>
@@ -6141,16 +6143,16 @@
         <v>368</v>
       </c>
       <c r="D126" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E126" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F126" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="G126" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H126" t="str">
         <f t="shared" si="1"/>
@@ -6168,16 +6170,16 @@
         <v>371</v>
       </c>
       <c r="D127" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E127" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F127" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="G127" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H127" t="str">
         <f t="shared" si="1"/>
@@ -6198,10 +6200,10 @@
         <v>728</v>
       </c>
       <c r="E128" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G128" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H128" t="str">
         <f t="shared" si="1"/>
@@ -6222,13 +6224,13 @@
         <v>714</v>
       </c>
       <c r="E129" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F129" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="G129" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H129" t="str">
         <f t="shared" si="1"/>
@@ -6240,22 +6242,22 @@
         <v>378</v>
       </c>
       <c r="B130" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C130" t="s">
         <v>379</v>
       </c>
       <c r="D130" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E130" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F130" t="s">
         <v>698</v>
       </c>
       <c r="G130" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H130" t="str">
         <f t="shared" si="1"/>
@@ -6273,13 +6275,13 @@
         <v>382</v>
       </c>
       <c r="D131" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E131" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G131" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H131" t="str">
         <f t="shared" ref="H131:H194" si="2">IF(NOT(ISBLANK(F131)),"update signs set name_de = """&amp;B131&amp;""", mnemonic = """&amp;C131&amp;""", tag1 ="""&amp;D131&amp;""", tag2 ="""&amp;E131&amp;""", tag3 ="""&amp;F131&amp;""" where name = """&amp;A131&amp;""";","update signs set name_de = """&amp;B131&amp;""", mnemonic = """&amp;C131&amp;""", tag1 ="""&amp;D131&amp;""", tag2 ="""&amp;E131&amp;""" where name = """&amp;A131&amp;""";")</f>
@@ -6300,13 +6302,13 @@
         <v>714</v>
       </c>
       <c r="E132" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F132" t="s">
         <v>698</v>
       </c>
       <c r="G132" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H132" t="str">
         <f t="shared" si="2"/>
@@ -6327,10 +6329,10 @@
         <v>686</v>
       </c>
       <c r="E133" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G133" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H133" t="str">
         <f t="shared" si="2"/>
@@ -6351,13 +6353,13 @@
         <v>689</v>
       </c>
       <c r="E134" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F134" t="s">
         <v>714</v>
       </c>
       <c r="G134" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H134" t="str">
         <f t="shared" si="2"/>
@@ -6378,13 +6380,13 @@
         <v>714</v>
       </c>
       <c r="E135" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F135" t="s">
         <v>289</v>
       </c>
       <c r="G135" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H135" t="str">
         <f t="shared" si="2"/>
@@ -6402,13 +6404,13 @@
         <v>397</v>
       </c>
       <c r="D136" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E136" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G136" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H136" t="str">
         <f t="shared" si="2"/>
@@ -6426,13 +6428,13 @@
         <v>400</v>
       </c>
       <c r="D137" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E137" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G137" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H137" t="str">
         <f t="shared" si="2"/>
@@ -6450,16 +6452,16 @@
         <v>403</v>
       </c>
       <c r="D138" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E138" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F138" t="s">
         <v>677</v>
       </c>
       <c r="G138" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H138" t="str">
         <f t="shared" si="2"/>
@@ -6477,16 +6479,16 @@
         <v>406</v>
       </c>
       <c r="D139" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E139" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F139" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="G139" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H139" t="str">
         <f t="shared" si="2"/>
@@ -6507,13 +6509,13 @@
         <v>714</v>
       </c>
       <c r="E140" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F140" t="s">
         <v>698</v>
       </c>
       <c r="G140" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H140" t="str">
         <f t="shared" si="2"/>
@@ -6534,13 +6536,13 @@
         <v>683</v>
       </c>
       <c r="E141" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F141" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="G141" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H141" t="str">
         <f t="shared" si="2"/>
@@ -6558,16 +6560,16 @@
         <v>415</v>
       </c>
       <c r="D142" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E142" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F142" t="s">
         <v>698</v>
       </c>
       <c r="G142" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H142" t="str">
         <f t="shared" si="2"/>
@@ -6585,13 +6587,13 @@
         <v>418</v>
       </c>
       <c r="D143" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E143" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G143" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H143" t="str">
         <f t="shared" si="2"/>
@@ -6612,13 +6614,13 @@
         <v>714</v>
       </c>
       <c r="E144" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F144" t="s">
         <v>698</v>
       </c>
       <c r="G144" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H144" t="str">
         <f t="shared" si="2"/>
@@ -6636,16 +6638,16 @@
         <v>424</v>
       </c>
       <c r="D145" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E145" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F145" t="s">
         <v>677</v>
       </c>
       <c r="G145" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H145" t="str">
         <f t="shared" si="2"/>
@@ -6666,10 +6668,10 @@
         <v>728</v>
       </c>
       <c r="E146" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G146" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H146" t="str">
         <f t="shared" si="2"/>
@@ -6690,10 +6692,10 @@
         <v>289</v>
       </c>
       <c r="E147" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G147" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H147" t="str">
         <f t="shared" si="2"/>
@@ -6714,13 +6716,13 @@
         <v>714</v>
       </c>
       <c r="E148" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F148" t="s">
         <v>698</v>
       </c>
       <c r="G148" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H148" t="str">
         <f t="shared" si="2"/>
@@ -6741,10 +6743,10 @@
         <v>728</v>
       </c>
       <c r="E149" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G149" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H149" t="str">
         <f t="shared" si="2"/>
@@ -6765,10 +6767,10 @@
         <v>408</v>
       </c>
       <c r="E150" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G150" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H150" t="str">
         <f t="shared" si="2"/>
@@ -6789,13 +6791,13 @@
         <v>689</v>
       </c>
       <c r="E151" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F151" t="s">
         <v>289</v>
       </c>
       <c r="G151" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H151" t="str">
         <f t="shared" si="2"/>
@@ -6816,13 +6818,13 @@
         <v>714</v>
       </c>
       <c r="E152" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F152" t="s">
         <v>689</v>
       </c>
       <c r="G152" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H152" t="str">
         <f t="shared" si="2"/>
@@ -6843,13 +6845,13 @@
         <v>683</v>
       </c>
       <c r="E153" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F153" t="s">
         <v>698</v>
       </c>
       <c r="G153" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H153" t="str">
         <f t="shared" si="2"/>
@@ -6867,16 +6869,16 @@
         <v>451</v>
       </c>
       <c r="D154" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E154" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F154" t="s">
         <v>698</v>
       </c>
       <c r="G154" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H154" t="str">
         <f t="shared" si="2"/>
@@ -6894,13 +6896,13 @@
         <v>454</v>
       </c>
       <c r="D155" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E155" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G155" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H155" t="str">
         <f t="shared" si="2"/>
@@ -6921,10 +6923,10 @@
         <v>703</v>
       </c>
       <c r="E156" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G156" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H156" t="str">
         <f t="shared" si="2"/>
@@ -6942,16 +6944,16 @@
         <v>460</v>
       </c>
       <c r="D157" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E157" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F157" t="s">
         <v>698</v>
       </c>
       <c r="G157" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H157" t="str">
         <f t="shared" si="2"/>
@@ -6972,10 +6974,10 @@
         <v>686</v>
       </c>
       <c r="E158" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G158" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H158" t="str">
         <f t="shared" si="2"/>
@@ -6993,16 +6995,16 @@
         <v>466</v>
       </c>
       <c r="D159" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E159" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F159" t="s">
         <v>677</v>
       </c>
       <c r="G159" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H159" t="str">
         <f t="shared" si="2"/>
@@ -7023,13 +7025,13 @@
         <v>289</v>
       </c>
       <c r="E160" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F160" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="G160" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H160" t="str">
         <f t="shared" si="2"/>
@@ -7050,13 +7052,13 @@
         <v>689</v>
       </c>
       <c r="E161" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F161" t="s">
         <v>698</v>
       </c>
       <c r="G161" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H161" t="str">
         <f t="shared" si="2"/>
@@ -7074,16 +7076,16 @@
         <v>475</v>
       </c>
       <c r="D162" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E162" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F162" t="s">
         <v>677</v>
       </c>
       <c r="G162" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H162" t="str">
         <f t="shared" si="2"/>
@@ -7095,7 +7097,7 @@
         <v>476</v>
       </c>
       <c r="B163" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C163" t="s">
         <v>477</v>
@@ -7104,13 +7106,13 @@
         <v>683</v>
       </c>
       <c r="E163" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F163" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="G163" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H163" t="str">
         <f t="shared" si="2"/>
@@ -7128,16 +7130,16 @@
         <v>480</v>
       </c>
       <c r="D164" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E164" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F164" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="G164" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H164" t="str">
         <f t="shared" si="2"/>
@@ -7158,13 +7160,13 @@
         <v>722</v>
       </c>
       <c r="E165" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F165" t="s">
         <v>698</v>
       </c>
       <c r="G165" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H165" t="str">
         <f t="shared" si="2"/>
@@ -7185,13 +7187,13 @@
         <v>722</v>
       </c>
       <c r="E166" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F166" t="s">
         <v>698</v>
       </c>
       <c r="G166" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H166" t="str">
         <f t="shared" si="2"/>
@@ -7212,13 +7214,13 @@
         <v>683</v>
       </c>
       <c r="E167" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F167" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="G167" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H167" t="str">
         <f t="shared" si="2"/>
@@ -7239,10 +7241,10 @@
         <v>728</v>
       </c>
       <c r="E168" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G168" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H168" t="str">
         <f t="shared" si="2"/>
@@ -7263,13 +7265,13 @@
         <v>714</v>
       </c>
       <c r="E169" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F169" t="s">
         <v>698</v>
       </c>
       <c r="G169" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H169" t="str">
         <f t="shared" si="2"/>
@@ -7281,7 +7283,7 @@
         <v>496</v>
       </c>
       <c r="B170" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C170" t="s">
         <v>497</v>
@@ -7290,13 +7292,13 @@
         <v>677</v>
       </c>
       <c r="E170" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F170" t="s">
         <v>698</v>
       </c>
       <c r="G170" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H170" t="str">
         <f t="shared" si="2"/>
@@ -7308,7 +7310,7 @@
         <v>498</v>
       </c>
       <c r="B171" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C171" t="s">
         <v>499</v>
@@ -7317,13 +7319,13 @@
         <v>677</v>
       </c>
       <c r="E171" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F171" t="s">
         <v>698</v>
       </c>
       <c r="G171" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H171" t="str">
         <f t="shared" si="2"/>
@@ -7344,10 +7346,10 @@
         <v>289</v>
       </c>
       <c r="E172" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G172" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H172" t="str">
         <f t="shared" si="2"/>
@@ -7368,13 +7370,13 @@
         <v>728</v>
       </c>
       <c r="E173" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F173" t="s">
         <v>199</v>
       </c>
       <c r="G173" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H173" t="str">
         <f t="shared" si="2"/>
@@ -7395,13 +7397,13 @@
         <v>683</v>
       </c>
       <c r="E174" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F174" t="s">
         <v>722</v>
       </c>
       <c r="G174" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H174" t="str">
         <f t="shared" si="2"/>
@@ -7422,10 +7424,10 @@
         <v>683</v>
       </c>
       <c r="E175" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G175" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H175" t="str">
         <f t="shared" si="2"/>
@@ -7446,13 +7448,13 @@
         <v>683</v>
       </c>
       <c r="E176" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F176" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="G176" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H176" t="str">
         <f t="shared" si="2"/>
@@ -7473,13 +7475,13 @@
         <v>689</v>
       </c>
       <c r="E177" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F177" t="s">
         <v>698</v>
       </c>
       <c r="G177" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H177" t="str">
         <f t="shared" si="2"/>
@@ -7500,13 +7502,13 @@
         <v>408</v>
       </c>
       <c r="E178" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F178" t="s">
         <v>698</v>
       </c>
       <c r="G178" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H178" t="str">
         <f t="shared" si="2"/>
@@ -7524,16 +7526,16 @@
         <v>523</v>
       </c>
       <c r="D179" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E179" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F179" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="G179" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H179" t="str">
         <f t="shared" si="2"/>
@@ -7554,10 +7556,10 @@
         <v>673</v>
       </c>
       <c r="E180" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G180" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H180" t="str">
         <f t="shared" si="2"/>
@@ -7575,16 +7577,16 @@
         <v>529</v>
       </c>
       <c r="D181" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E181" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F181" t="s">
         <v>722</v>
       </c>
       <c r="G181" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H181" t="str">
         <f t="shared" si="2"/>
@@ -7605,10 +7607,10 @@
         <v>728</v>
       </c>
       <c r="E182" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G182" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H182" t="str">
         <f t="shared" si="2"/>
@@ -7629,10 +7631,10 @@
         <v>673</v>
       </c>
       <c r="E183" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G183" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H183" t="str">
         <f t="shared" si="2"/>
@@ -7650,13 +7652,13 @@
         <v>538</v>
       </c>
       <c r="D184" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E184" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G184" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H184" t="str">
         <f t="shared" si="2"/>
@@ -7677,10 +7679,10 @@
         <v>408</v>
       </c>
       <c r="E185" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G185" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H185" t="str">
         <f t="shared" si="2"/>
@@ -7701,13 +7703,13 @@
         <v>703</v>
       </c>
       <c r="E186" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F186" t="s">
         <v>408</v>
       </c>
       <c r="G186" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H186" t="str">
         <f t="shared" si="2"/>
@@ -7725,16 +7727,16 @@
         <v>547</v>
       </c>
       <c r="D187" t="s">
+        <v>805</v>
+      </c>
+      <c r="E187" t="s">
+        <v>790</v>
+      </c>
+      <c r="F187" t="s">
         <v>806</v>
       </c>
-      <c r="E187" t="s">
-        <v>791</v>
-      </c>
-      <c r="F187" t="s">
-        <v>807</v>
-      </c>
       <c r="G187" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H187" t="str">
         <f t="shared" si="2"/>
@@ -7755,13 +7757,13 @@
         <v>722</v>
       </c>
       <c r="E188" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F188" t="s">
         <v>698</v>
       </c>
       <c r="G188" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H188" t="str">
         <f t="shared" si="2"/>
@@ -7782,13 +7784,13 @@
         <v>289</v>
       </c>
       <c r="E189" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F189" t="s">
         <v>714</v>
       </c>
       <c r="G189" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H189" t="str">
         <f t="shared" si="2"/>
@@ -7806,16 +7808,16 @@
         <v>556</v>
       </c>
       <c r="D190" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E190" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F190" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="G190" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H190" t="str">
         <f t="shared" si="2"/>
@@ -7833,13 +7835,13 @@
         <v>559</v>
       </c>
       <c r="D191" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E191" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G191" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H191" t="str">
         <f t="shared" si="2"/>
@@ -7860,13 +7862,13 @@
         <v>677</v>
       </c>
       <c r="E192" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F192" t="s">
         <v>698</v>
       </c>
       <c r="G192" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H192" t="str">
         <f t="shared" si="2"/>
@@ -7887,13 +7889,13 @@
         <v>722</v>
       </c>
       <c r="E193" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F193" t="s">
         <v>698</v>
       </c>
       <c r="G193" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H193" t="str">
         <f t="shared" si="2"/>
@@ -7911,13 +7913,13 @@
         <v>568</v>
       </c>
       <c r="D194" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E194" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G194" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H194" t="str">
         <f t="shared" si="2"/>
@@ -7938,13 +7940,13 @@
         <v>728</v>
       </c>
       <c r="E195" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F195" t="s">
         <v>199</v>
       </c>
       <c r="G195" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H195" t="str">
         <f t="shared" ref="H195:H211" si="3">IF(NOT(ISBLANK(F195)),"update signs set name_de = """&amp;B195&amp;""", mnemonic = """&amp;C195&amp;""", tag1 ="""&amp;D195&amp;""", tag2 ="""&amp;E195&amp;""", tag3 ="""&amp;F195&amp;""" where name = """&amp;A195&amp;""";","update signs set name_de = """&amp;B195&amp;""", mnemonic = """&amp;C195&amp;""", tag1 ="""&amp;D195&amp;""", tag2 ="""&amp;E195&amp;""" where name = """&amp;A195&amp;""";")</f>
@@ -7962,16 +7964,16 @@
         <v>574</v>
       </c>
       <c r="D196" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E196" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F196" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="G196" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H196" t="str">
         <f t="shared" si="3"/>
@@ -7989,13 +7991,13 @@
         <v>577</v>
       </c>
       <c r="D197" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E197" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G197" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H197" t="str">
         <f t="shared" si="3"/>
@@ -8013,13 +8015,13 @@
         <v>580</v>
       </c>
       <c r="D198" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E198" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G198" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H198" t="str">
         <f t="shared" si="3"/>
@@ -8037,13 +8039,13 @@
         <v>583</v>
       </c>
       <c r="D199" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E199" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G199" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H199" t="str">
         <f t="shared" si="3"/>
@@ -8061,13 +8063,13 @@
         <v>586</v>
       </c>
       <c r="D200" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E200" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G200" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H200" t="str">
         <f t="shared" si="3"/>
@@ -8088,10 +8090,10 @@
         <v>289</v>
       </c>
       <c r="E201" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G201" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H201" t="str">
         <f t="shared" si="3"/>
@@ -8109,13 +8111,13 @@
         <v>592</v>
       </c>
       <c r="D202" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E202" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G202" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H202" t="str">
         <f t="shared" si="3"/>
@@ -8136,10 +8138,10 @@
         <v>686</v>
       </c>
       <c r="E203" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G203" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H203" t="str">
         <f t="shared" si="3"/>
@@ -8160,13 +8162,13 @@
         <v>689</v>
       </c>
       <c r="E204" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F204" t="s">
         <v>698</v>
       </c>
       <c r="G204" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H204" t="str">
         <f t="shared" si="3"/>
@@ -8184,16 +8186,16 @@
         <v>601</v>
       </c>
       <c r="D205" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E205" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F205" t="s">
         <v>677</v>
       </c>
       <c r="G205" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H205" t="str">
         <f t="shared" si="3"/>
@@ -8214,13 +8216,13 @@
         <v>683</v>
       </c>
       <c r="E206" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F206" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="G206" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H206" t="str">
         <f t="shared" si="3"/>
@@ -8241,10 +8243,10 @@
         <v>673</v>
       </c>
       <c r="E207" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G207" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H207" t="str">
         <f t="shared" si="3"/>
@@ -8265,10 +8267,10 @@
         <v>728</v>
       </c>
       <c r="E208" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G208" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H208" t="str">
         <f t="shared" si="3"/>
@@ -8289,13 +8291,13 @@
         <v>686</v>
       </c>
       <c r="E209" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F209" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="G209" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H209" t="str">
         <f t="shared" si="3"/>
@@ -8307,7 +8309,7 @@
         <v>614</v>
       </c>
       <c r="B210" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C210" t="s">
         <v>278</v>
@@ -8316,13 +8318,13 @@
         <v>683</v>
       </c>
       <c r="E210" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F210" t="s">
         <v>698</v>
       </c>
       <c r="G210" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H210" t="str">
         <f t="shared" si="3"/>
@@ -8340,13 +8342,13 @@
         <v>617</v>
       </c>
       <c r="D211" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E211" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G211" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="H211" t="str">
         <f t="shared" si="3"/>
@@ -8433,7 +8435,7 @@
         <v>674</v>
       </c>
       <c r="F215" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H215" t="str">
         <f t="shared" si="4"/>
@@ -8535,7 +8537,7 @@
         <v>625</v>
       </c>
       <c r="C220" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D220" t="s">
         <v>694</v>
@@ -8739,7 +8741,7 @@
         <v>717</v>
       </c>
       <c r="D229" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E229" t="s">
         <v>674</v>
@@ -8799,7 +8801,7 @@
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B232" t="s">
         <v>634</v>
@@ -8814,7 +8816,7 @@
         <v>674</v>
       </c>
       <c r="F232" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H232" t="str">
         <f t="shared" si="4"/>
@@ -8832,7 +8834,7 @@
         <v>725</v>
       </c>
       <c r="D233" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E233" t="s">
         <v>674</v>
@@ -9048,16 +9050,16 @@
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>746</v>
+        <v>834</v>
       </c>
       <c r="B243" t="s">
         <v>645</v>
       </c>
       <c r="C243" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D243" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E243" t="s">
         <v>674</v>
@@ -9067,21 +9069,21 @@
       </c>
       <c r="H243" t="str">
         <f t="shared" si="4"/>
-        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("new","neu","dominante Hand schiebt sich langsam hinter anderer Hand hervor: 'neu erscheinen'","Kleine Worte","Zusatz","Eigenschaften");</v>
+        <v>insert into signs (name, name_de, mnemonic, tag1, tag2, tag3) values ("brand_new","neu","dominante Hand schiebt sich langsam hinter anderer Hand hervor: 'neu erscheinen'","Kleine Worte","Zusatz","Eigenschaften");</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B244" t="s">
         <v>646</v>
       </c>
       <c r="C244" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="D244" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E244" t="s">
         <v>674</v>
@@ -9093,13 +9095,13 @@
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B245" t="s">
         <v>647</v>
       </c>
       <c r="C245" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D245" t="s">
         <v>689</v>
@@ -9117,13 +9119,13 @@
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B246" t="s">
         <v>648</v>
       </c>
       <c r="C246" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="D246" t="s">
         <v>689</v>
@@ -9141,13 +9143,13 @@
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B247" t="s">
         <v>649</v>
       </c>
       <c r="C247" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D247" t="s">
         <v>694</v>
@@ -9162,16 +9164,16 @@
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B248" t="s">
         <v>650</v>
       </c>
       <c r="C248" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D248" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E248" t="s">
         <v>674</v>
@@ -9186,13 +9188,13 @@
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B249" t="s">
         <v>651</v>
       </c>
       <c r="C249" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D249" t="s">
         <v>711</v>
@@ -9207,13 +9209,13 @@
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B250" t="s">
         <v>652</v>
       </c>
       <c r="C250" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D250" t="s">
         <v>694</v>
@@ -9228,13 +9230,13 @@
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B251" t="s">
         <v>653</v>
       </c>
       <c r="C251" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D251" t="s">
         <v>689</v>
@@ -9252,13 +9254,13 @@
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B252" t="s">
         <v>654</v>
       </c>
       <c r="C252" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="D252" t="s">
         <v>673</v>
@@ -9273,13 +9275,13 @@
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B253" t="s">
         <v>655</v>
       </c>
       <c r="C253" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D253" t="s">
         <v>680</v>
@@ -9297,13 +9299,13 @@
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B254" t="s">
         <v>656</v>
       </c>
       <c r="C254" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D254" t="s">
         <v>683</v>
@@ -9321,16 +9323,16 @@
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B255" t="s">
         <v>657</v>
       </c>
       <c r="C255" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D255" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E255" t="s">
         <v>674</v>
@@ -9345,16 +9347,16 @@
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B256" t="s">
         <v>658</v>
       </c>
       <c r="C256" t="s">
+        <v>772</v>
+      </c>
+      <c r="D256" t="s">
         <v>773</v>
-      </c>
-      <c r="D256" t="s">
-        <v>774</v>
       </c>
       <c r="E256" t="s">
         <v>674</v>
@@ -9366,16 +9368,16 @@
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B257" t="s">
         <v>659</v>
       </c>
       <c r="C257" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D257" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E257" t="s">
         <v>674</v>
@@ -9387,16 +9389,16 @@
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B258" t="s">
         <v>660</v>
       </c>
       <c r="C258" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="D258" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E258" t="s">
         <v>674</v>
@@ -9408,16 +9410,16 @@
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B259" t="s">
         <v>661</v>
       </c>
       <c r="C259" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D259" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E259" t="s">
         <v>674</v>
@@ -9429,13 +9431,13 @@
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B260" t="s">
         <v>662</v>
       </c>
       <c r="C260" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D260" t="s">
         <v>711</v>
@@ -9450,13 +9452,13 @@
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B261" t="s">
         <v>663</v>
       </c>
       <c r="C261" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D261" t="s">
         <v>673</v>
@@ -9465,7 +9467,7 @@
         <v>674</v>
       </c>
       <c r="F261" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="H261" t="str">
         <f t="shared" si="4"/>
@@ -9474,13 +9476,13 @@
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="B262" t="s">
         <v>664</v>
       </c>
       <c r="C262" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D262" t="s">
         <v>722</v>
@@ -9498,13 +9500,13 @@
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B263" t="s">
         <v>670</v>
       </c>
       <c r="C263" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="D263" t="s">
         <v>680</v>
@@ -9522,16 +9524,16 @@
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B264" t="s">
         <v>665</v>
       </c>
       <c r="C264" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D264" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E264" t="s">
         <v>674</v>

</xml_diff>